<commit_message>
add GTDB taxid field
column U content filled
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VirJenDB\virjendb_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{696BB408-924E-4C26-960B-57C67839ECF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07056291-CA25-4D52-9AB9-A75CC46242E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D7962945-3ACF-49DB-B8FB-E785F5F91D27}"/>
   </bookViews>
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4647" uniqueCount="1606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4649" uniqueCount="1607">
   <si>
     <t>VJDBv0.3</t>
   </si>
@@ -4469,6 +4469,9 @@
   </si>
   <si>
     <t>Host GTDB TaxID</t>
+  </si>
+  <si>
+    <t>GTDB</t>
   </si>
   <si>
     <t>0hg</t>
@@ -5885,8 +5888,8 @@
   <dimension ref="A1:FY196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AV191" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AW194" sqref="AW194"/>
+      <pane xSplit="1" topLeftCell="T186" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U194" sqref="U194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="23.25" customHeight="1"/>
@@ -47170,9 +47173,28 @@
       <c r="B193" t="s">
         <v>1411</v>
       </c>
+      <c r="U193" t="s">
+        <v>1412</v>
+      </c>
+      <c r="V193" s="48" t="str">
+        <f>"[" &amp; _xlfn.TEXTJOIN(", ", TRUE,
+    IF(H193&lt;&gt;"", """" &amp; H$1 &amp; """", ""),
+    IF(I193&lt;&gt;"", """" &amp; I$1 &amp; """", ""),
+    IF(J193&lt;&gt;"", """" &amp; J$1 &amp; """", ""),
+    IF(K193&lt;&gt;"", """" &amp; K$1 &amp; """", ""),
+    IF(L193&lt;&gt;"", """" &amp; L$1 &amp; """", ""),    IF(M193&lt;&gt;"", """" &amp; M$1 &amp; """", ""),    IF(N193&lt;&gt;"", """" &amp; N$1 &amp; """", ""),     IF(O193&lt;&gt;"", """" &amp; O$1 &amp; """", ""),     IF(P193&lt;&gt;"", """" &amp; P$1 &amp; """", ""),
+    IF(S193&lt;&gt;"", """" &amp; S193 &amp; """", ""), IF(Q193&lt;&gt;"", """" &amp; Q193 &amp; """", ""), IF(R193&lt;&gt;"", """" &amp; R193 &amp; """", ""),
+    IF(T193&lt;&gt;"", """" &amp; T193 &amp; """", ""),
+    IF(U193&lt;&gt;"", """" &amp; U193 &amp; """", "")
+) &amp; "]"</f>
+        <v>["GTDB"]</v>
+      </c>
+      <c r="W193" t="s">
+        <v>1412</v>
+      </c>
       <c r="AS193"/>
       <c r="AW193" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="194" spans="1:49" ht="23.25" customHeight="1">
@@ -48380,7 +48402,7 @@
         <v>361</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
@@ -48390,14 +48412,14 @@
       <c r="AC5" s="8"/>
       <c r="AD5" s="8"/>
       <c r="AE5" s="2" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="AG5" s="8"/>
       <c r="AH5" s="9" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI5" s="8"/>
       <c r="AJ5" s="8"/>
@@ -48424,7 +48446,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -48449,7 +48471,7 @@
         <v>361</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
@@ -48461,14 +48483,14 @@
       </c>
       <c r="AD6" s="13"/>
       <c r="AE6" s="1" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG6" s="13"/>
       <c r="AH6" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI6" s="13"/>
       <c r="AJ6" s="13"/>
@@ -48518,7 +48540,7 @@
         <v>361</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
@@ -48530,14 +48552,14 @@
         <v>121</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="AF7" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG7" s="13"/>
       <c r="AH7" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI7" s="13"/>
       <c r="AJ7" s="13"/>
@@ -48587,7 +48609,7 @@
         <v>361</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X8" s="13"/>
       <c r="Y8" s="13"/>
@@ -48597,14 +48619,14 @@
       <c r="AC8" s="13"/>
       <c r="AD8" s="13"/>
       <c r="AE8" s="1" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG8" s="13"/>
       <c r="AH8" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI8" s="13"/>
       <c r="AJ8" s="13"/>
@@ -48654,7 +48676,7 @@
         <v>361</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
@@ -48664,14 +48686,14 @@
       <c r="AC9" s="13"/>
       <c r="AD9" s="13"/>
       <c r="AE9" s="1" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="AF9" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG9" s="13"/>
       <c r="AH9" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI9" s="13"/>
       <c r="AJ9" s="13"/>
@@ -48698,7 +48720,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -48723,7 +48745,7 @@
         <v>361</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
@@ -48735,14 +48757,14 @@
       </c>
       <c r="AD10" s="13"/>
       <c r="AE10" s="1" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="AF10" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG10" s="13"/>
       <c r="AH10" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI10" s="13"/>
       <c r="AJ10" s="13"/>
@@ -48769,7 +48791,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -48794,7 +48816,7 @@
         <v>361</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -48806,14 +48828,14 @@
       </c>
       <c r="AD11" s="13"/>
       <c r="AE11" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="AF11" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG11" s="13"/>
       <c r="AH11" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI11" s="13"/>
       <c r="AJ11" s="13"/>
@@ -48863,7 +48885,7 @@
         <v>361</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
@@ -48873,14 +48895,14 @@
       <c r="AC12" s="13"/>
       <c r="AD12" s="13"/>
       <c r="AE12" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="AF12" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG12" s="13"/>
       <c r="AH12" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI12" s="13"/>
       <c r="AJ12" s="13"/>
@@ -48930,7 +48952,7 @@
         <v>361</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -48940,14 +48962,14 @@
       <c r="AC13" s="13"/>
       <c r="AD13" s="13"/>
       <c r="AE13" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="AF13" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG13" s="13"/>
       <c r="AH13" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI13" s="13"/>
       <c r="AJ13" s="13"/>
@@ -48974,7 +48996,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -48999,7 +49021,7 @@
         <v>361</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
@@ -49007,20 +49029,20 @@
       <c r="AA14" s="13"/>
       <c r="AB14" s="13"/>
       <c r="AC14" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE14" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="AF14" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG14" s="13"/>
       <c r="AH14" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI14" s="13"/>
       <c r="AJ14" s="13"/>
@@ -49070,7 +49092,7 @@
         <v>361</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -49079,17 +49101,17 @@
       <c r="AB15" s="13"/>
       <c r="AC15" s="13"/>
       <c r="AD15" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="AF15" s="1" t="s">
         <v>249</v>
       </c>
       <c r="AG15" s="13"/>
       <c r="AH15" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI15" s="13"/>
       <c r="AJ15" s="13"/>
@@ -49139,7 +49161,7 @@
         <v>361</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -49149,14 +49171,14 @@
       <c r="AC16" s="13"/>
       <c r="AD16" s="13"/>
       <c r="AE16" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="AF16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG16" s="13"/>
       <c r="AH16" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI16" s="13"/>
       <c r="AJ16" s="13"/>
@@ -49183,7 +49205,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -49208,7 +49230,7 @@
         <v>361</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -49216,20 +49238,20 @@
       <c r="AA17" s="13"/>
       <c r="AB17" s="13"/>
       <c r="AC17" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="AF17" s="1" t="s">
         <v>249</v>
       </c>
       <c r="AG17" s="13"/>
       <c r="AH17" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI17" s="13"/>
       <c r="AJ17" s="13"/>
@@ -49256,7 +49278,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
@@ -49281,7 +49303,7 @@
         <v>361</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X18" s="13"/>
       <c r="Y18" s="13"/>
@@ -49289,20 +49311,20 @@
       <c r="AA18" s="13"/>
       <c r="AB18" s="13"/>
       <c r="AC18" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="AF18" s="1" t="s">
         <v>249</v>
       </c>
       <c r="AG18" s="13"/>
       <c r="AH18" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI18" s="13"/>
       <c r="AJ18" s="13"/>
@@ -49329,7 +49351,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
@@ -49354,7 +49376,7 @@
         <v>361</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -49368,14 +49390,14 @@
         <v>218</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="AF19" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG19" s="13"/>
       <c r="AH19" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI19" s="13"/>
       <c r="AJ19" s="13"/>
@@ -49402,7 +49424,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
@@ -49427,7 +49449,7 @@
         <v>361</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X20" s="13"/>
       <c r="Y20" s="13"/>
@@ -49439,14 +49461,14 @@
       </c>
       <c r="AD20" s="13"/>
       <c r="AE20" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="AF20" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG20" s="13"/>
       <c r="AH20" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI20" s="13"/>
       <c r="AJ20" s="13"/>
@@ -49518,7 +49540,7 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
@@ -49543,7 +49565,7 @@
         <v>361</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
@@ -49551,20 +49573,20 @@
       <c r="AA22" s="13"/>
       <c r="AB22" s="13"/>
       <c r="AC22" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="AF22" s="1" t="s">
         <v>249</v>
       </c>
       <c r="AG22" s="13"/>
       <c r="AH22" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI22" s="13"/>
       <c r="AJ22" s="13"/>
@@ -49591,7 +49613,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -49616,7 +49638,7 @@
         <v>361</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
@@ -49630,14 +49652,14 @@
         <v>121</v>
       </c>
       <c r="AE23" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="AF23" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG23" s="13"/>
       <c r="AH23" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI23" s="13"/>
       <c r="AJ23" s="13"/>
@@ -49664,7 +49686,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
@@ -49689,7 +49711,7 @@
         <v>361</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -49701,14 +49723,14 @@
       </c>
       <c r="AD24" s="13"/>
       <c r="AE24" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="AF24" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG24" s="13"/>
       <c r="AH24" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI24" s="13"/>
       <c r="AJ24" s="13"/>
@@ -49758,7 +49780,7 @@
         <v>361</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
@@ -49768,14 +49790,14 @@
       <c r="AC25" s="13"/>
       <c r="AD25" s="13"/>
       <c r="AE25" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AF25" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG25" s="13"/>
       <c r="AH25" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI25" s="13"/>
       <c r="AJ25" s="13"/>
@@ -49802,7 +49824,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
@@ -49827,7 +49849,7 @@
         <v>361</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X26" s="13"/>
       <c r="Y26" s="13"/>
@@ -49839,14 +49861,14 @@
       </c>
       <c r="AD26" s="13"/>
       <c r="AE26" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="AF26" s="1" t="s">
         <v>731</v>
       </c>
       <c r="AG26" s="13"/>
       <c r="AH26" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI26" s="13"/>
       <c r="AJ26" s="13"/>
@@ -49873,7 +49895,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -49898,7 +49920,7 @@
         <v>361</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X27" s="13"/>
       <c r="Y27" s="13"/>
@@ -49912,14 +49934,14 @@
         <v>218</v>
       </c>
       <c r="AE27" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="AF27" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG27" s="13"/>
       <c r="AH27" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI27" s="13"/>
       <c r="AJ27" s="13"/>
@@ -49946,7 +49968,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
@@ -49971,7 +49993,7 @@
         <v>361</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -49985,14 +50007,14 @@
         <v>218</v>
       </c>
       <c r="AE28" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="AF28" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG28" s="13"/>
       <c r="AH28" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI28" s="13"/>
       <c r="AJ28" s="13"/>
@@ -50019,7 +50041,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
@@ -50044,7 +50066,7 @@
         <v>361</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X29" s="13"/>
       <c r="Y29" s="13"/>
@@ -50058,14 +50080,14 @@
         <v>218</v>
       </c>
       <c r="AE29" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="AF29" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG29" s="13"/>
       <c r="AH29" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI29" s="13"/>
       <c r="AJ29" s="13"/>
@@ -50115,7 +50137,7 @@
         <v>361</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X30" s="13"/>
       <c r="Y30" s="13"/>
@@ -50124,17 +50146,17 @@
       <c r="AB30" s="13"/>
       <c r="AC30" s="13"/>
       <c r="AD30" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE30" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="AF30" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG30" s="13"/>
       <c r="AH30" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI30" s="13"/>
       <c r="AJ30" s="13"/>
@@ -50184,7 +50206,7 @@
         <v>361</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
@@ -50193,17 +50215,17 @@
       <c r="AB31" s="13"/>
       <c r="AC31" s="13"/>
       <c r="AD31" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE31" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="AF31" s="1" t="s">
         <v>249</v>
       </c>
       <c r="AG31" s="13"/>
       <c r="AH31" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI31" s="13"/>
       <c r="AJ31" s="13"/>
@@ -50230,7 +50252,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
@@ -50255,7 +50277,7 @@
         <v>361</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>
@@ -50267,14 +50289,14 @@
       </c>
       <c r="AD32" s="13"/>
       <c r="AE32" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="AF32" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG32" s="13"/>
       <c r="AH32" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI32" s="13"/>
       <c r="AJ32" s="13"/>
@@ -50324,7 +50346,7 @@
         <v>361</v>
       </c>
       <c r="W33" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
@@ -50334,14 +50356,14 @@
       <c r="AC33" s="13"/>
       <c r="AD33" s="13"/>
       <c r="AE33" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="AF33" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG33" s="13"/>
       <c r="AH33" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI33" s="13"/>
       <c r="AJ33" s="13"/>
@@ -50368,7 +50390,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
@@ -50393,7 +50415,7 @@
         <v>361</v>
       </c>
       <c r="W34" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X34" s="13"/>
       <c r="Y34" s="13"/>
@@ -50405,14 +50427,14 @@
       </c>
       <c r="AD34" s="13"/>
       <c r="AE34" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="AF34" s="1" t="s">
         <v>731</v>
       </c>
       <c r="AG34" s="13"/>
       <c r="AH34" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI34" s="13"/>
       <c r="AJ34" s="13"/>
@@ -50462,7 +50484,7 @@
         <v>361</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X35" s="13"/>
       <c r="Y35" s="13"/>
@@ -50474,14 +50496,14 @@
         <v>121</v>
       </c>
       <c r="AE35" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="AF35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG35" s="13"/>
       <c r="AH35" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI35" s="13"/>
       <c r="AJ35" s="13"/>
@@ -50531,7 +50553,7 @@
         <v>361</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X36" s="13"/>
       <c r="Y36" s="13"/>
@@ -50548,7 +50570,7 @@
       </c>
       <c r="AG36" s="13"/>
       <c r="AH36" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI36" s="13"/>
       <c r="AJ36" s="13"/>
@@ -50575,7 +50597,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
@@ -50600,7 +50622,7 @@
         <v>361</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X37" s="13"/>
       <c r="Y37" s="13"/>
@@ -50608,20 +50630,20 @@
       <c r="AA37" s="13"/>
       <c r="AB37" s="13"/>
       <c r="AC37" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="AD37" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AE37" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="AF37" s="1" t="s">
         <v>249</v>
       </c>
       <c r="AG37" s="13"/>
       <c r="AH37" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI37" s="13"/>
       <c r="AJ37" s="13"/>
@@ -50648,7 +50670,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
@@ -50673,7 +50695,7 @@
         <v>361</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X38" s="13"/>
       <c r="Y38" s="13"/>
@@ -50681,20 +50703,20 @@
       <c r="AA38" s="13"/>
       <c r="AB38" s="13"/>
       <c r="AC38" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="AD38" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AE38" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="AF38" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG38" s="13"/>
       <c r="AH38" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI38" s="13"/>
       <c r="AJ38" s="13"/>
@@ -50721,7 +50743,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
@@ -50746,7 +50768,7 @@
         <v>361</v>
       </c>
       <c r="W39" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X39" s="13"/>
       <c r="Y39" s="13"/>
@@ -50754,20 +50776,20 @@
       <c r="AA39" s="13"/>
       <c r="AB39" s="13"/>
       <c r="AC39" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="AD39" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AE39" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="AF39" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG39" s="13"/>
       <c r="AH39" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI39" s="13"/>
       <c r="AJ39" s="13"/>
@@ -50794,7 +50816,7 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
@@ -50819,7 +50841,7 @@
         <v>361</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X40" s="13"/>
       <c r="Y40" s="13"/>
@@ -50827,18 +50849,18 @@
       <c r="AA40" s="13"/>
       <c r="AB40" s="13"/>
       <c r="AC40" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="AD40" s="13"/>
       <c r="AE40" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="AF40" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG40" s="13"/>
       <c r="AH40" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI40" s="13"/>
       <c r="AJ40" s="13"/>
@@ -50865,7 +50887,7 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
@@ -50890,7 +50912,7 @@
         <v>361</v>
       </c>
       <c r="W41" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X41" s="13"/>
       <c r="Y41" s="13"/>
@@ -50904,14 +50926,14 @@
         <v>121</v>
       </c>
       <c r="AE41" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="AF41" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG41" s="13"/>
       <c r="AH41" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI41" s="13"/>
       <c r="AJ41" s="13"/>
@@ -50961,7 +50983,7 @@
         <v>361</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X42" s="13"/>
       <c r="Y42" s="13"/>
@@ -50971,14 +50993,14 @@
       <c r="AC42" s="13"/>
       <c r="AD42" s="13"/>
       <c r="AE42" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="AF42" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG42" s="13"/>
       <c r="AH42" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI42" s="13"/>
       <c r="AJ42" s="13"/>
@@ -51005,7 +51027,7 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
@@ -51030,7 +51052,7 @@
         <v>361</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X43" s="13"/>
       <c r="Y43" s="13"/>
@@ -51042,14 +51064,14 @@
       </c>
       <c r="AD43" s="13"/>
       <c r="AE43" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="AF43" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG43" s="13"/>
       <c r="AH43" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI43" s="13"/>
       <c r="AJ43" s="13"/>
@@ -51076,7 +51098,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
@@ -51101,7 +51123,7 @@
         <v>361</v>
       </c>
       <c r="W44" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X44" s="13"/>
       <c r="Y44" s="13"/>
@@ -51113,14 +51135,14 @@
       </c>
       <c r="AD44" s="13"/>
       <c r="AE44" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="AF44" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG44" s="13"/>
       <c r="AH44" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI44" s="13"/>
       <c r="AJ44" s="13"/>
@@ -51147,7 +51169,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
@@ -51172,7 +51194,7 @@
         <v>361</v>
       </c>
       <c r="W45" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X45" s="13"/>
       <c r="Y45" s="13"/>
@@ -51184,14 +51206,14 @@
       </c>
       <c r="AD45" s="13"/>
       <c r="AE45" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="AF45" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG45" s="13"/>
       <c r="AH45" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI45" s="13"/>
       <c r="AJ45" s="13"/>
@@ -51241,7 +51263,7 @@
         <v>361</v>
       </c>
       <c r="W46" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X46" s="13"/>
       <c r="Y46" s="13"/>
@@ -51251,14 +51273,14 @@
       <c r="AC46" s="13"/>
       <c r="AD46" s="13"/>
       <c r="AE46" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="AF46" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG46" s="13"/>
       <c r="AH46" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI46" s="13"/>
       <c r="AJ46" s="13"/>
@@ -51285,7 +51307,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
@@ -51310,7 +51332,7 @@
         <v>361</v>
       </c>
       <c r="W47" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X47" s="13"/>
       <c r="Y47" s="13"/>
@@ -51322,14 +51344,14 @@
       </c>
       <c r="AD47" s="13"/>
       <c r="AE47" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="AF47" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG47" s="13"/>
       <c r="AH47" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI47" s="13"/>
       <c r="AJ47" s="13"/>
@@ -51379,7 +51401,7 @@
         <v>361</v>
       </c>
       <c r="W48" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X48" s="13"/>
       <c r="Y48" s="13"/>
@@ -51389,14 +51411,14 @@
       <c r="AC48" s="13"/>
       <c r="AD48" s="13"/>
       <c r="AE48" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="AF48" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG48" s="13"/>
       <c r="AH48" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI48" s="13"/>
       <c r="AJ48" s="13"/>
@@ -51423,7 +51445,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
@@ -51448,7 +51470,7 @@
         <v>361</v>
       </c>
       <c r="W49" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X49" s="13"/>
       <c r="Y49" s="13"/>
@@ -51460,14 +51482,14 @@
       </c>
       <c r="AD49" s="13"/>
       <c r="AE49" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="AF49" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG49" s="13"/>
       <c r="AH49" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI49" s="13"/>
       <c r="AJ49" s="13"/>
@@ -51517,7 +51539,7 @@
         <v>361</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X50" s="13"/>
       <c r="Y50" s="13"/>
@@ -51527,14 +51549,14 @@
       <c r="AC50" s="13"/>
       <c r="AD50" s="13"/>
       <c r="AE50" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="AF50" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG50" s="13"/>
       <c r="AH50" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI50" s="13"/>
       <c r="AJ50" s="13"/>
@@ -51584,7 +51606,7 @@
         <v>361</v>
       </c>
       <c r="W51" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X51" s="13"/>
       <c r="Y51" s="13"/>
@@ -51593,17 +51615,17 @@
       <c r="AB51" s="13"/>
       <c r="AC51" s="13"/>
       <c r="AD51" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE51" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="AF51" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG51" s="13"/>
       <c r="AH51" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI51" s="13"/>
       <c r="AJ51" s="13"/>
@@ -51653,7 +51675,7 @@
         <v>361</v>
       </c>
       <c r="W52" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X52" s="13"/>
       <c r="Y52" s="13"/>
@@ -51662,17 +51684,17 @@
       <c r="AB52" s="13"/>
       <c r="AC52" s="13"/>
       <c r="AD52" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE52" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="AF52" s="1" t="s">
         <v>249</v>
       </c>
       <c r="AG52" s="13"/>
       <c r="AH52" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI52" s="13"/>
       <c r="AJ52" s="13"/>
@@ -51699,7 +51721,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
@@ -51724,7 +51746,7 @@
         <v>361</v>
       </c>
       <c r="W53" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X53" s="13"/>
       <c r="Y53" s="13"/>
@@ -51738,14 +51760,14 @@
         <v>121</v>
       </c>
       <c r="AE53" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="AF53" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG53" s="13"/>
       <c r="AH53" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI53" s="13"/>
       <c r="AJ53" s="13"/>
@@ -51795,7 +51817,7 @@
         <v>361</v>
       </c>
       <c r="W54" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X54" s="13"/>
       <c r="Y54" s="13"/>
@@ -51807,14 +51829,14 @@
         <v>121</v>
       </c>
       <c r="AE54" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="AF54" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG54" s="13"/>
       <c r="AH54" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI54" s="13"/>
       <c r="AJ54" s="13"/>
@@ -51841,7 +51863,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
@@ -51866,7 +51888,7 @@
         <v>361</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X55" s="13"/>
       <c r="Y55" s="13"/>
@@ -51880,14 +51902,14 @@
         <v>121</v>
       </c>
       <c r="AE55" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="AF55" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG55" s="13"/>
       <c r="AH55" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI55" s="13"/>
       <c r="AJ55" s="13"/>
@@ -51961,7 +51983,7 @@
         <v>361</v>
       </c>
       <c r="W57" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X57" s="13"/>
       <c r="Y57" s="13"/>
@@ -51973,14 +51995,14 @@
         <v>121</v>
       </c>
       <c r="AE57" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="AF57" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG57" s="13"/>
       <c r="AH57" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI57" s="13"/>
       <c r="AJ57" s="13"/>
@@ -52030,7 +52052,7 @@
         <v>361</v>
       </c>
       <c r="W58" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X58" s="13"/>
       <c r="Y58" s="13"/>
@@ -52042,14 +52064,14 @@
         <v>121</v>
       </c>
       <c r="AE58" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="AF58" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG58" s="13"/>
       <c r="AH58" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI58" s="13"/>
       <c r="AJ58" s="13"/>
@@ -52076,7 +52098,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
@@ -52101,7 +52123,7 @@
         <v>361</v>
       </c>
       <c r="W59" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X59" s="13"/>
       <c r="Y59" s="13"/>
@@ -52109,20 +52131,20 @@
       <c r="AA59" s="13"/>
       <c r="AB59" s="13"/>
       <c r="AC59" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AD59" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE59" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="AF59" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG59" s="13"/>
       <c r="AH59" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI59" s="13"/>
       <c r="AJ59" s="13"/>
@@ -52172,7 +52194,7 @@
         <v>361</v>
       </c>
       <c r="W60" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X60" s="13"/>
       <c r="Y60" s="13"/>
@@ -52181,17 +52203,17 @@
       <c r="AB60" s="13"/>
       <c r="AC60" s="13"/>
       <c r="AD60" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE60" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="AF60" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG60" s="13"/>
       <c r="AH60" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI60" s="13"/>
       <c r="AJ60" s="13"/>
@@ -52218,7 +52240,7 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
@@ -52243,7 +52265,7 @@
         <v>361</v>
       </c>
       <c r="W61" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X61" s="13"/>
       <c r="Y61" s="13"/>
@@ -52255,14 +52277,14 @@
       </c>
       <c r="AD61" s="13"/>
       <c r="AE61" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="AF61" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG61" s="13"/>
       <c r="AH61" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI61" s="13"/>
       <c r="AJ61" s="13"/>
@@ -52312,7 +52334,7 @@
         <v>361</v>
       </c>
       <c r="W62" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X62" s="13"/>
       <c r="Y62" s="13"/>
@@ -52322,14 +52344,14 @@
       <c r="AC62" s="13"/>
       <c r="AD62" s="13"/>
       <c r="AE62" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="AF62" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG62" s="13"/>
       <c r="AH62" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI62" s="13"/>
       <c r="AJ62" s="13"/>
@@ -52356,7 +52378,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="O63" s="6"/>
       <c r="P63" s="6"/>
@@ -52381,7 +52403,7 @@
         <v>361</v>
       </c>
       <c r="W63" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X63" s="13"/>
       <c r="Y63" s="13"/>
@@ -52393,14 +52415,14 @@
       </c>
       <c r="AD63" s="13"/>
       <c r="AE63" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="AF63" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG63" s="13"/>
       <c r="AH63" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI63" s="13"/>
       <c r="AJ63" s="13"/>
@@ -52450,7 +52472,7 @@
         <v>361</v>
       </c>
       <c r="W64" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X64" s="13"/>
       <c r="Y64" s="13"/>
@@ -52460,14 +52482,14 @@
       <c r="AC64" s="13"/>
       <c r="AD64" s="13"/>
       <c r="AE64" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="AF64" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG64" s="13"/>
       <c r="AH64" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI64" s="13"/>
       <c r="AJ64" s="13"/>
@@ -52517,7 +52539,7 @@
         <v>361</v>
       </c>
       <c r="W65" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X65" s="13"/>
       <c r="Y65" s="13"/>
@@ -52526,17 +52548,17 @@
       <c r="AB65" s="13"/>
       <c r="AC65" s="13"/>
       <c r="AD65" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AE65" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="AF65" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG65" s="13"/>
       <c r="AH65" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI65" s="13"/>
       <c r="AJ65" s="13"/>
@@ -52586,7 +52608,7 @@
         <v>361</v>
       </c>
       <c r="W66" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X66" s="13"/>
       <c r="Y66" s="13"/>
@@ -52596,14 +52618,14 @@
       <c r="AC66" s="13"/>
       <c r="AD66" s="13"/>
       <c r="AE66" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="AF66" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG66" s="13"/>
       <c r="AH66" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI66" s="13"/>
       <c r="AJ66" s="13"/>
@@ -52677,7 +52699,7 @@
         <v>361</v>
       </c>
       <c r="W68" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X68" s="13"/>
       <c r="Y68" s="13"/>
@@ -52694,7 +52716,7 @@
       </c>
       <c r="AG68" s="13"/>
       <c r="AH68" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI68" s="13"/>
       <c r="AJ68" s="13"/>
@@ -52721,7 +52743,7 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="O69" s="6"/>
       <c r="P69" s="6"/>
@@ -52746,7 +52768,7 @@
         <v>361</v>
       </c>
       <c r="W69" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X69" s="13"/>
       <c r="Y69" s="13"/>
@@ -52758,14 +52780,14 @@
       </c>
       <c r="AD69" s="13"/>
       <c r="AE69" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="AF69" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG69" s="13"/>
       <c r="AH69" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI69" s="13"/>
       <c r="AJ69" s="13"/>
@@ -52792,7 +52814,7 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="O70" s="6"/>
       <c r="P70" s="6"/>
@@ -52817,7 +52839,7 @@
         <v>361</v>
       </c>
       <c r="W70" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X70" s="13"/>
       <c r="Y70" s="13"/>
@@ -52831,14 +52853,14 @@
         <v>121</v>
       </c>
       <c r="AE70" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="AF70" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG70" s="13"/>
       <c r="AH70" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI70" s="13"/>
       <c r="AJ70" s="13"/>
@@ -52865,7 +52887,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
       <c r="N71" s="4" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="O71" s="6"/>
       <c r="P71" s="6"/>
@@ -52890,7 +52912,7 @@
         <v>361</v>
       </c>
       <c r="W71" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X71" s="13"/>
       <c r="Y71" s="13"/>
@@ -52902,14 +52924,14 @@
       </c>
       <c r="AD71" s="13"/>
       <c r="AE71" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="AF71" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG71" s="13"/>
       <c r="AH71" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI71" s="13"/>
       <c r="AJ71" s="13"/>
@@ -52936,7 +52958,7 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
       <c r="N72" s="4" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="O72" s="6"/>
       <c r="P72" s="6"/>
@@ -52961,7 +52983,7 @@
         <v>361</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X72" s="13"/>
       <c r="Y72" s="13"/>
@@ -52973,14 +52995,14 @@
       </c>
       <c r="AD72" s="13"/>
       <c r="AE72" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="AF72" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG72" s="13"/>
       <c r="AH72" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI72" s="13"/>
       <c r="AJ72" s="13"/>
@@ -53030,7 +53052,7 @@
         <v>361</v>
       </c>
       <c r="W73" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X73" s="13"/>
       <c r="Y73" s="13"/>
@@ -53039,17 +53061,17 @@
       <c r="AB73" s="13"/>
       <c r="AC73" s="13"/>
       <c r="AD73" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AE73" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="AF73" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG73" s="13"/>
       <c r="AH73" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI73" s="13"/>
       <c r="AJ73" s="13"/>
@@ -53076,7 +53098,7 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="O74" s="6"/>
       <c r="P74" s="6"/>
@@ -53101,7 +53123,7 @@
         <v>361</v>
       </c>
       <c r="W74" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X74" s="13"/>
       <c r="Y74" s="13"/>
@@ -53112,17 +53134,17 @@
         <v>729</v>
       </c>
       <c r="AD74" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="AE74" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="AF74" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG74" s="13"/>
       <c r="AH74" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI74" s="13"/>
       <c r="AJ74" s="13"/>
@@ -53172,7 +53194,7 @@
         <v>361</v>
       </c>
       <c r="W75" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X75" s="13"/>
       <c r="Y75" s="13"/>
@@ -53182,14 +53204,14 @@
       <c r="AC75" s="13"/>
       <c r="AD75" s="13"/>
       <c r="AE75" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="AF75" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG75" s="13"/>
       <c r="AH75" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI75" s="13"/>
       <c r="AJ75" s="13"/>
@@ -53239,7 +53261,7 @@
         <v>361</v>
       </c>
       <c r="W76" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X76" s="13"/>
       <c r="Y76" s="13"/>
@@ -53249,14 +53271,14 @@
       <c r="AC76" s="13"/>
       <c r="AD76" s="13"/>
       <c r="AE76" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="AF76" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG76" s="13"/>
       <c r="AH76" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI76" s="13"/>
       <c r="AJ76" s="13"/>
@@ -53306,7 +53328,7 @@
         <v>361</v>
       </c>
       <c r="W77" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X77" s="13"/>
       <c r="Y77" s="13"/>
@@ -53315,17 +53337,17 @@
       <c r="AB77" s="13"/>
       <c r="AC77" s="13"/>
       <c r="AD77" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE77" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="AF77" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG77" s="13"/>
       <c r="AH77" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI77" s="13"/>
       <c r="AJ77" s="13"/>
@@ -53375,7 +53397,7 @@
         <v>361</v>
       </c>
       <c r="W78" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X78" s="13"/>
       <c r="Y78" s="13"/>
@@ -53384,17 +53406,17 @@
       <c r="AB78" s="13"/>
       <c r="AC78" s="13"/>
       <c r="AD78" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE78" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="AF78" s="1" t="s">
         <v>249</v>
       </c>
       <c r="AG78" s="13"/>
       <c r="AH78" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI78" s="13"/>
       <c r="AJ78" s="13"/>
@@ -53421,7 +53443,7 @@
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
       <c r="N79" s="4" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="O79" s="6"/>
       <c r="P79" s="6"/>
@@ -53446,7 +53468,7 @@
         <v>361</v>
       </c>
       <c r="W79" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X79" s="13"/>
       <c r="Y79" s="13"/>
@@ -53458,14 +53480,14 @@
       </c>
       <c r="AD79" s="13"/>
       <c r="AE79" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="AF79" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG79" s="13"/>
       <c r="AH79" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI79" s="13"/>
       <c r="AJ79" s="13"/>
@@ -53492,7 +53514,7 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
       <c r="N80" s="4" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="O80" s="6"/>
       <c r="P80" s="6"/>
@@ -53517,7 +53539,7 @@
         <v>361</v>
       </c>
       <c r="W80" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X80" s="13"/>
       <c r="Y80" s="13"/>
@@ -53529,14 +53551,14 @@
       </c>
       <c r="AD80" s="13"/>
       <c r="AE80" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AF80" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG80" s="13"/>
       <c r="AH80" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI80" s="13"/>
       <c r="AJ80" s="13"/>
@@ -53586,7 +53608,7 @@
         <v>361</v>
       </c>
       <c r="W81" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X81" s="13"/>
       <c r="Y81" s="13"/>
@@ -53595,17 +53617,17 @@
       <c r="AB81" s="13"/>
       <c r="AC81" s="13"/>
       <c r="AD81" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE81" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="AF81" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG81" s="13"/>
       <c r="AH81" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI81" s="13"/>
       <c r="AJ81" s="13"/>
@@ -53632,7 +53654,7 @@
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
       <c r="N82" s="4" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="O82" s="6"/>
       <c r="P82" s="6"/>
@@ -53657,7 +53679,7 @@
         <v>361</v>
       </c>
       <c r="W82" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X82" s="13"/>
       <c r="Y82" s="13"/>
@@ -53669,14 +53691,14 @@
       </c>
       <c r="AD82" s="13"/>
       <c r="AE82" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="AF82" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG82" s="13"/>
       <c r="AH82" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI82" s="13"/>
       <c r="AJ82" s="13"/>
@@ -53726,7 +53748,7 @@
         <v>361</v>
       </c>
       <c r="W83" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X83" s="13"/>
       <c r="Y83" s="13"/>
@@ -53736,14 +53758,14 @@
       <c r="AC83" s="13"/>
       <c r="AD83" s="13"/>
       <c r="AE83" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="AF83" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG83" s="13"/>
       <c r="AH83" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI83" s="13"/>
       <c r="AJ83" s="13"/>
@@ -53815,7 +53837,7 @@
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
       <c r="N85" s="4" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="O85" s="6"/>
       <c r="P85" s="6"/>
@@ -53840,7 +53862,7 @@
         <v>361</v>
       </c>
       <c r="W85" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X85" s="13"/>
       <c r="Y85" s="13"/>
@@ -53854,14 +53876,14 @@
         <v>218</v>
       </c>
       <c r="AE85" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="AF85" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG85" s="13"/>
       <c r="AH85" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI85" s="13"/>
       <c r="AJ85" s="13"/>
@@ -53911,7 +53933,7 @@
         <v>361</v>
       </c>
       <c r="W86" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X86" s="13"/>
       <c r="Y86" s="13"/>
@@ -53920,17 +53942,17 @@
       <c r="AB86" s="13"/>
       <c r="AC86" s="13"/>
       <c r="AD86" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE86" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="AF86" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG86" s="13"/>
       <c r="AH86" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI86" s="13"/>
       <c r="AJ86" s="13"/>
@@ -53980,7 +54002,7 @@
         <v>361</v>
       </c>
       <c r="W87" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X87" s="13"/>
       <c r="Y87" s="13"/>
@@ -53989,17 +54011,17 @@
       <c r="AB87" s="13"/>
       <c r="AC87" s="13"/>
       <c r="AD87" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE87" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="AF87" s="1" t="s">
         <v>249</v>
       </c>
       <c r="AG87" s="13"/>
       <c r="AH87" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI87" s="13"/>
       <c r="AJ87" s="13"/>
@@ -54026,7 +54048,7 @@
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
       <c r="N88" s="4" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="O88" s="6"/>
       <c r="P88" s="6"/>
@@ -54051,7 +54073,7 @@
         <v>361</v>
       </c>
       <c r="W88" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X88" s="13"/>
       <c r="Y88" s="13"/>
@@ -54062,7 +54084,7 @@
         <v>729</v>
       </c>
       <c r="AD88" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="AE88" s="1" t="s">
         <v>58</v>
@@ -54072,7 +54094,7 @@
       </c>
       <c r="AG88" s="13"/>
       <c r="AH88" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI88" s="13"/>
       <c r="AJ88" s="13"/>
@@ -54122,7 +54144,7 @@
         <v>361</v>
       </c>
       <c r="W89" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X89" s="13"/>
       <c r="Y89" s="13"/>
@@ -54139,7 +54161,7 @@
       </c>
       <c r="AG89" s="13"/>
       <c r="AH89" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI89" s="13"/>
       <c r="AJ89" s="13"/>
@@ -54189,7 +54211,7 @@
         <v>361</v>
       </c>
       <c r="W90" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X90" s="13"/>
       <c r="Y90" s="13"/>
@@ -54199,14 +54221,14 @@
       <c r="AC90" s="13"/>
       <c r="AD90" s="13"/>
       <c r="AE90" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="AF90" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG90" s="13"/>
       <c r="AH90" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI90" s="13"/>
       <c r="AJ90" s="13"/>
@@ -54256,7 +54278,7 @@
         <v>361</v>
       </c>
       <c r="W91" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X91" s="13"/>
       <c r="Y91" s="13"/>
@@ -54265,17 +54287,17 @@
       <c r="AB91" s="13"/>
       <c r="AC91" s="13"/>
       <c r="AD91" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE91" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="AF91" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG91" s="13"/>
       <c r="AH91" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI91" s="13"/>
       <c r="AJ91" s="13"/>
@@ -54325,7 +54347,7 @@
         <v>361</v>
       </c>
       <c r="W92" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X92" s="13"/>
       <c r="Y92" s="13"/>
@@ -54335,14 +54357,14 @@
       <c r="AC92" s="13"/>
       <c r="AD92" s="13"/>
       <c r="AE92" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="AF92" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG92" s="13"/>
       <c r="AH92" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI92" s="13"/>
       <c r="AJ92" s="13"/>
@@ -54369,7 +54391,7 @@
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6"/>
@@ -54394,7 +54416,7 @@
         <v>361</v>
       </c>
       <c r="W93" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X93" s="13"/>
       <c r="Y93" s="13"/>
@@ -54402,20 +54424,20 @@
       <c r="AA93" s="13"/>
       <c r="AB93" s="13"/>
       <c r="AC93" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AD93" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE93" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="AF93" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG93" s="13"/>
       <c r="AH93" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI93" s="13"/>
       <c r="AJ93" s="13"/>
@@ -54465,7 +54487,7 @@
         <v>361</v>
       </c>
       <c r="W94" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X94" s="13"/>
       <c r="Y94" s="13"/>
@@ -54475,14 +54497,14 @@
       <c r="AC94" s="13"/>
       <c r="AD94" s="13"/>
       <c r="AE94" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AF94" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG94" s="13"/>
       <c r="AH94" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI94" s="13"/>
       <c r="AJ94" s="13"/>
@@ -54509,7 +54531,7 @@
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
       <c r="N95" s="4" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="O95" s="6"/>
       <c r="P95" s="6"/>
@@ -54534,7 +54556,7 @@
         <v>361</v>
       </c>
       <c r="W95" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X95" s="13"/>
       <c r="Y95" s="13"/>
@@ -54548,14 +54570,14 @@
         <v>121</v>
       </c>
       <c r="AE95" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="AF95" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG95" s="13"/>
       <c r="AH95" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI95" s="13"/>
       <c r="AJ95" s="13"/>
@@ -54607,7 +54629,7 @@
         <v>361</v>
       </c>
       <c r="W96" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X96" s="13"/>
       <c r="Y96" s="13"/>
@@ -54619,14 +54641,14 @@
       </c>
       <c r="AD96" s="13"/>
       <c r="AE96" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="AF96" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG96" s="13"/>
       <c r="AH96" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI96" s="13"/>
       <c r="AJ96" s="13"/>
@@ -54676,7 +54698,7 @@
         <v>361</v>
       </c>
       <c r="W97" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X97" s="13"/>
       <c r="Y97" s="13"/>
@@ -54688,14 +54710,14 @@
         <v>218</v>
       </c>
       <c r="AE97" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="AF97" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG97" s="13"/>
       <c r="AH97" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI97" s="13"/>
       <c r="AJ97" s="13"/>
@@ -54722,7 +54744,7 @@
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
       <c r="N98" s="4" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="O98" s="6"/>
       <c r="P98" s="6"/>
@@ -54747,7 +54769,7 @@
         <v>361</v>
       </c>
       <c r="W98" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X98" s="13"/>
       <c r="Y98" s="13"/>
@@ -54759,14 +54781,14 @@
       </c>
       <c r="AD98" s="13"/>
       <c r="AE98" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="AF98" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG98" s="13"/>
       <c r="AH98" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI98" s="13"/>
       <c r="AJ98" s="13"/>
@@ -54793,7 +54815,7 @@
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
       <c r="N99" s="4" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="O99" s="6"/>
       <c r="P99" s="6"/>
@@ -54818,7 +54840,7 @@
         <v>361</v>
       </c>
       <c r="W99" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X99" s="13"/>
       <c r="Y99" s="13"/>
@@ -54830,14 +54852,14 @@
       </c>
       <c r="AD99" s="13"/>
       <c r="AE99" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="AF99" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG99" s="13"/>
       <c r="AH99" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI99" s="13"/>
       <c r="AJ99" s="13"/>
@@ -54887,7 +54909,7 @@
         <v>361</v>
       </c>
       <c r="W100" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X100" s="13"/>
       <c r="Y100" s="13"/>
@@ -54897,14 +54919,14 @@
       <c r="AC100" s="13"/>
       <c r="AD100" s="13"/>
       <c r="AE100" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="AF100" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG100" s="13"/>
       <c r="AH100" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI100" s="13"/>
       <c r="AJ100" s="13"/>
@@ -54931,7 +54953,7 @@
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
       <c r="N101" s="4" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="O101" s="6"/>
       <c r="P101" s="6"/>
@@ -54956,7 +54978,7 @@
         <v>361</v>
       </c>
       <c r="W101" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X101" s="13"/>
       <c r="Y101" s="13"/>
@@ -54970,14 +54992,14 @@
         <v>121</v>
       </c>
       <c r="AE101" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="AF101" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG101" s="13"/>
       <c r="AH101" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI101" s="13"/>
       <c r="AJ101" s="13"/>
@@ -55029,7 +55051,7 @@
         <v>361</v>
       </c>
       <c r="W102" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X102" s="13"/>
       <c r="Y102" s="13"/>
@@ -55048,7 +55070,7 @@
       </c>
       <c r="AG102" s="13"/>
       <c r="AH102" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI102" s="13"/>
       <c r="AJ102" s="13"/>
@@ -55075,7 +55097,7 @@
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="O103" s="6"/>
       <c r="P103" s="6"/>
@@ -55100,7 +55122,7 @@
         <v>361</v>
       </c>
       <c r="W103" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X103" s="13"/>
       <c r="Y103" s="13"/>
@@ -55112,14 +55134,14 @@
       </c>
       <c r="AD103" s="13"/>
       <c r="AE103" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="AF103" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG103" s="13"/>
       <c r="AH103" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI103" s="13"/>
       <c r="AJ103" s="13"/>
@@ -55146,7 +55168,7 @@
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="O104" s="6"/>
       <c r="P104" s="6"/>
@@ -55171,7 +55193,7 @@
         <v>361</v>
       </c>
       <c r="W104" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X104" s="13"/>
       <c r="Y104" s="13"/>
@@ -55183,14 +55205,14 @@
       </c>
       <c r="AD104" s="13"/>
       <c r="AE104" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="AF104" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG104" s="13"/>
       <c r="AH104" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI104" s="13"/>
       <c r="AJ104" s="13"/>
@@ -55217,7 +55239,7 @@
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="O105" s="6"/>
       <c r="P105" s="6"/>
@@ -55242,7 +55264,7 @@
         <v>361</v>
       </c>
       <c r="W105" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X105" s="13"/>
       <c r="Y105" s="13"/>
@@ -55256,14 +55278,14 @@
         <v>634</v>
       </c>
       <c r="AE105" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="AF105" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG105" s="13"/>
       <c r="AH105" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI105" s="13"/>
       <c r="AJ105" s="13"/>
@@ -55291,7 +55313,7 @@
       <c r="M106" s="4"/>
       <c r="AG106" s="13"/>
       <c r="AH106" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI106" s="13"/>
       <c r="AJ106" s="13"/>
@@ -55341,7 +55363,7 @@
         <v>361</v>
       </c>
       <c r="W107" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X107" s="13"/>
       <c r="Y107" s="13"/>
@@ -55351,14 +55373,14 @@
       <c r="AC107" s="13"/>
       <c r="AD107" s="13"/>
       <c r="AE107" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="AF107" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG107" s="13"/>
       <c r="AH107" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI107" s="13"/>
       <c r="AJ107" s="13"/>
@@ -55408,7 +55430,7 @@
         <v>361</v>
       </c>
       <c r="W108" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X108" s="13"/>
       <c r="Y108" s="13"/>
@@ -55421,11 +55443,11 @@
         <v>69</v>
       </c>
       <c r="AF108" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="AG108" s="13"/>
       <c r="AH108" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI108" s="13"/>
       <c r="AJ108" s="13"/>
@@ -55452,7 +55474,7 @@
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="O109" s="6"/>
       <c r="P109" s="6"/>
@@ -55477,7 +55499,7 @@
         <v>361</v>
       </c>
       <c r="W109" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X109" s="13"/>
       <c r="Y109" s="13"/>
@@ -55485,20 +55507,20 @@
       <c r="AA109" s="13"/>
       <c r="AB109" s="13"/>
       <c r="AC109" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AD109" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="AE109" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="AF109" s="1" t="s">
         <v>220</v>
       </c>
       <c r="AG109" s="13"/>
       <c r="AH109" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI109" s="13"/>
       <c r="AJ109" s="13"/>
@@ -55525,7 +55547,7 @@
       <c r="L110" s="4"/>
       <c r="M110" s="4"/>
       <c r="N110" s="4" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="O110" s="6"/>
       <c r="P110" s="6"/>
@@ -55550,7 +55572,7 @@
         <v>361</v>
       </c>
       <c r="W110" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X110" s="13"/>
       <c r="Y110" s="13"/>
@@ -55562,14 +55584,14 @@
       </c>
       <c r="AD110" s="13"/>
       <c r="AE110" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="AF110" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG110" s="13"/>
       <c r="AH110" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI110" s="13"/>
       <c r="AJ110" s="13"/>
@@ -55619,7 +55641,7 @@
         <v>361</v>
       </c>
       <c r="W111" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X111" s="13"/>
       <c r="Y111" s="13"/>
@@ -55629,14 +55651,14 @@
       <c r="AC111" s="13"/>
       <c r="AD111" s="13"/>
       <c r="AE111" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="AF111" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AG111" s="13"/>
       <c r="AH111" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI111" s="13"/>
       <c r="AJ111" s="13"/>
@@ -55686,7 +55708,7 @@
         <v>361</v>
       </c>
       <c r="W112" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X112" s="13"/>
       <c r="Y112" s="13"/>
@@ -55695,17 +55717,17 @@
       <c r="AB112" s="13"/>
       <c r="AC112" s="13"/>
       <c r="AD112" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="AE112" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="AF112" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG112" s="13"/>
       <c r="AH112" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI112" s="13"/>
       <c r="AJ112" s="13"/>
@@ -55755,7 +55777,7 @@
         <v>361</v>
       </c>
       <c r="W113" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X113" s="13"/>
       <c r="Y113" s="13"/>
@@ -55764,17 +55786,17 @@
       <c r="AB113" s="13"/>
       <c r="AC113" s="13"/>
       <c r="AD113" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="AE113" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="AF113" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG113" s="13"/>
       <c r="AH113" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI113" s="13"/>
       <c r="AJ113" s="13"/>
@@ -55801,7 +55823,7 @@
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
       <c r="N114" s="4" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="O114" s="6"/>
       <c r="P114" s="6"/>
@@ -55826,7 +55848,7 @@
         <v>361</v>
       </c>
       <c r="W114" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="X114" s="13"/>
       <c r="Y114" s="13"/>
@@ -55841,7 +55863,7 @@
       <c r="AF114" s="13"/>
       <c r="AG114" s="13"/>
       <c r="AH114" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AI114" s="13"/>
       <c r="AJ114" s="13"/>
@@ -55896,14 +55918,14 @@
       <c r="X115" s="34"/>
       <c r="Y115" s="34"/>
       <c r="Z115" s="36" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="AA115" s="36" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="AB115" s="34"/>
       <c r="AC115" s="34" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AD115" s="34"/>
       <c r="AE115" s="34"/>
@@ -56066,7 +56088,7 @@
       <c r="K116" s="34"/>
       <c r="L116" s="34"/>
       <c r="M116" s="36" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="N116" s="34"/>
       <c r="O116" s="34"/>
@@ -56099,14 +56121,14 @@
       <c r="X116" s="34"/>
       <c r="Y116" s="34"/>
       <c r="Z116" s="36" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="AA116" s="36" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="AB116" s="34"/>
       <c r="AC116" s="34" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="AD116" s="34"/>
       <c r="AE116" s="34"/>
@@ -56128,7 +56150,7 @@
       <c r="AU116" s="34"/>
       <c r="AV116" s="37"/>
       <c r="AW116" s="37" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="AX116" s="37"/>
       <c r="AY116" s="37"/>
@@ -56302,14 +56324,14 @@
       <c r="X117" s="34"/>
       <c r="Y117" s="34"/>
       <c r="Z117" s="36" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="AA117" s="36" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="AB117" s="34"/>
       <c r="AC117" s="34" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="AD117" s="34"/>
       <c r="AE117" s="34"/>
@@ -56331,7 +56353,7 @@
       <c r="AU117" s="34"/>
       <c r="AV117" s="37"/>
       <c r="AW117" s="37" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="AX117" s="37"/>
       <c r="AY117" s="37"/>
@@ -56460,13 +56482,13 @@
     </row>
     <row r="118" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A118" s="38" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="B118" s="39" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="C118" s="38" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D118" s="38"/>
       <c r="E118" s="38" t="s">
@@ -56482,10 +56504,10 @@
       <c r="M118" s="39"/>
       <c r="N118" s="39"/>
       <c r="O118" s="38" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="P118" s="38" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="Q118" s="40" t="s">
         <v>90</v>
@@ -56523,12 +56545,12 @@
       <c r="AH118" s="39"/>
       <c r="AI118" s="39"/>
       <c r="AJ118" s="38" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="AK118" s="38"/>
       <c r="AL118" s="38"/>
       <c r="AM118" s="38" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="AN118" s="38"/>
       <c r="AO118" s="38" t="s">
@@ -56547,14 +56569,14 @@
         <v>126</v>
       </c>
       <c r="AT118" s="38" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="AU118" s="39" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="AV118" s="39"/>
       <c r="AW118" s="39" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="AX118" s="39"/>
       <c r="AY118" s="39"/>
@@ -56683,13 +56705,13 @@
     </row>
     <row r="119" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A119" s="38" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="B119" s="39" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="C119" s="38" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D119" s="38"/>
       <c r="E119" s="38" t="s">
@@ -56705,10 +56727,10 @@
       <c r="M119" s="39"/>
       <c r="N119" s="39"/>
       <c r="O119" s="38" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="P119" s="38" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="Q119" s="40" t="s">
         <v>750</v>
@@ -56746,12 +56768,12 @@
       <c r="AH119" s="39"/>
       <c r="AI119" s="39"/>
       <c r="AJ119" s="38" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="AK119" s="38"/>
       <c r="AL119" s="38"/>
       <c r="AM119" s="38" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="AN119" s="38"/>
       <c r="AO119" s="38" t="s">
@@ -56770,14 +56792,14 @@
         <v>126</v>
       </c>
       <c r="AT119" s="38" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="AU119" s="39" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="AV119" s="39"/>
       <c r="AW119" s="39" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="AX119" s="39"/>
       <c r="AY119" s="39"/>
@@ -56906,13 +56928,13 @@
     </row>
     <row r="120" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A120" s="38" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="B120" s="39" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="C120" s="38" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="D120" s="38"/>
       <c r="E120" s="38" t="s">
@@ -56928,10 +56950,10 @@
       <c r="M120" s="39"/>
       <c r="N120" s="39"/>
       <c r="O120" s="38" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="P120" s="38" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="Q120" s="40" t="s">
         <v>906</v>
@@ -56969,12 +56991,12 @@
       <c r="AH120" s="39"/>
       <c r="AI120" s="39"/>
       <c r="AJ120" s="38" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="AK120" s="38"/>
       <c r="AL120" s="38"/>
       <c r="AM120" s="38" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="AN120" s="38"/>
       <c r="AO120" s="38" t="s">
@@ -56993,14 +57015,14 @@
         <v>126</v>
       </c>
       <c r="AT120" s="38" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="AU120" s="39" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="AV120" s="39"/>
       <c r="AW120" s="39" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="AX120" s="39"/>
       <c r="AY120" s="39"/>
@@ -57129,13 +57151,13 @@
     </row>
     <row r="121" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A121" s="38" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="B121" s="39" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="C121" s="38" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D121" s="38"/>
       <c r="E121" s="38" t="s">
@@ -57151,10 +57173,10 @@
       <c r="M121" s="39"/>
       <c r="N121" s="39"/>
       <c r="O121" s="38" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="P121" s="38" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="Q121" s="40" t="s">
         <v>103</v>
@@ -57192,12 +57214,12 @@
       <c r="AH121" s="39"/>
       <c r="AI121" s="39"/>
       <c r="AJ121" s="38" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="AK121" s="38"/>
       <c r="AL121" s="38"/>
       <c r="AM121" s="38" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="AN121" s="38"/>
       <c r="AO121" s="38" t="s">
@@ -57216,14 +57238,14 @@
         <v>126</v>
       </c>
       <c r="AT121" s="38" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="AU121" s="39" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="AV121" s="39"/>
       <c r="AW121" s="39" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="AX121" s="39"/>
       <c r="AY121" s="39"/>
@@ -57352,13 +57374,13 @@
     </row>
     <row r="122" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A122" s="38" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="B122" s="39" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="C122" s="38" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="D122" s="38"/>
       <c r="E122" s="38" t="s">
@@ -57374,10 +57396,10 @@
       <c r="M122" s="39"/>
       <c r="N122" s="39"/>
       <c r="O122" s="38" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="P122" s="38" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="Q122" s="40" t="s">
         <v>906</v>
@@ -57415,12 +57437,12 @@
       <c r="AH122" s="39"/>
       <c r="AI122" s="39"/>
       <c r="AJ122" s="38" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="AK122" s="38"/>
       <c r="AL122" s="38"/>
       <c r="AM122" s="38" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="AN122" s="38"/>
       <c r="AO122" s="38" t="s">
@@ -57439,14 +57461,14 @@
         <v>126</v>
       </c>
       <c r="AT122" s="38" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="AU122" s="39" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="AV122" s="39"/>
       <c r="AW122" s="39" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="AX122" s="39"/>
       <c r="AY122" s="39"/>
@@ -57575,13 +57597,13 @@
     </row>
     <row r="123" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A123" s="32" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="B123" s="42" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="D123" s="32"/>
       <c r="E123" s="32" t="s">
@@ -57597,10 +57619,10 @@
       <c r="M123" s="42"/>
       <c r="N123" s="42"/>
       <c r="O123" s="32" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="P123" s="32" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="Q123" s="43" t="s">
         <v>90</v>
@@ -57638,12 +57660,12 @@
       <c r="AH123" s="42"/>
       <c r="AI123" s="42"/>
       <c r="AJ123" s="32" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="AK123" s="32"/>
       <c r="AL123" s="32"/>
       <c r="AM123" s="32" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="AN123" s="32"/>
       <c r="AO123" s="32" t="s">
@@ -57662,14 +57684,14 @@
         <v>126</v>
       </c>
       <c r="AT123" s="32" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="AU123" s="42" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="AV123" s="42"/>
       <c r="AW123" s="42" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="AX123" s="42"/>
       <c r="AY123" s="42"/>
@@ -57798,13 +57820,13 @@
     </row>
     <row r="124" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A124" s="32" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="B124" s="42" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="D124" s="32"/>
       <c r="E124" s="32" t="s">
@@ -57820,10 +57842,10 @@
       <c r="M124" s="42"/>
       <c r="N124" s="42"/>
       <c r="O124" s="32" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="P124" s="32" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="Q124" s="43" t="s">
         <v>90</v>
@@ -57861,12 +57883,12 @@
       <c r="AH124" s="42"/>
       <c r="AI124" s="42"/>
       <c r="AJ124" s="32" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="AK124" s="32"/>
       <c r="AL124" s="32"/>
       <c r="AM124" s="32" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="AN124" s="32"/>
       <c r="AO124" s="32" t="s">
@@ -57885,14 +57907,14 @@
         <v>145</v>
       </c>
       <c r="AT124" s="32" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="AU124" s="42" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="AV124" s="42"/>
       <c r="AW124" s="42" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="AX124" s="42"/>
       <c r="AY124" s="42"/>

</xml_diff>

<commit_message>
is ICTV field renamed
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VirJenDB\virjendb_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBD5C3FC-B382-4A4C-A73E-38D28BBD5F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1A43AEC-D9B8-45BD-8AF7-6013DC56F51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D7962945-3ACF-49DB-B8FB-E785F5F91D27}"/>
   </bookViews>
@@ -4345,10 +4345,10 @@
     <t>0gv</t>
   </si>
   <si>
-    <t>is_ictv_reference</t>
-  </si>
-  <si>
-    <t>ICTV_Reference</t>
+    <t>is_ictv_exemplar</t>
+  </si>
+  <si>
+    <t>ICTV Exemplar</t>
   </si>
   <si>
     <t>This accession was used to define a species in the ICTV Taxonomy.</t>
@@ -5925,7 +5925,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B175" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E194" sqref="E194"/>
+      <selection pane="topRight" activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="23.25" customHeight="1"/>

</xml_diff>

<commit_message>
make is fields public
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VirJenDB\virjendb_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EB8ABE8-117B-4FA6-94F6-89DF1605480E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D88942-E2EA-41B4-9131-B63BED18BA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D7962945-3ACF-49DB-B8FB-E785F5F91D27}"/>
   </bookViews>
@@ -5324,7 +5324,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5741,7 +5741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5917,20 +5917,19 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -6281,12 +6280,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E033465-2455-477E-A700-6BF7A0771C26}">
   <dimension ref="A1:FY211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S201" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W207" sqref="W207"/>
+    <sheetView tabSelected="1" topLeftCell="A179" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F189" sqref="F189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="23.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.5703125" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.28515625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
@@ -6296,7 +6295,7 @@
     <col min="50" max="50" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:181" s="19" customFormat="1" ht="23.25" customHeight="1">
+    <row r="1" spans="1:181" s="19" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -6585,7 +6584,7 @@
       <c r="FX1"/>
       <c r="FY1"/>
     </row>
-    <row r="2" spans="1:181" s="19" customFormat="1" ht="23.25" customHeight="1">
+    <row r="2" spans="1:181" s="19" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>16</v>
       </c>
@@ -6874,7 +6873,7 @@
       <c r="FX2"/>
       <c r="FY2"/>
     </row>
-    <row r="3" spans="1:181" s="19" customFormat="1" ht="23.25" customHeight="1">
+    <row r="3" spans="1:181" s="19" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="str">
         <f t="shared" ref="A3:AY3" si="0">_xlfn.TEXTJOIN(" ", TRUE, LOWER(A1), LOWER(A2))</f>
         <v>vjdbv0.3 field id</v>
@@ -7216,7 +7215,7 @@
       <c r="FX3"/>
       <c r="FY3"/>
     </row>
-    <row r="4" spans="1:181" s="19" customFormat="1" ht="23.25" customHeight="1">
+    <row r="4" spans="1:181" s="19" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="str">
         <f t="shared" ref="A4:AY4" si="2">SUBSTITUTE(A3, " ", "_")</f>
         <v>vjdbv0.3_field_id</v>
@@ -7558,7 +7557,7 @@
       <c r="FX4"/>
       <c r="FY4"/>
     </row>
-    <row r="5" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="5" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>57</v>
       </c>
@@ -7801,7 +7800,7 @@
       <c r="FX5"/>
       <c r="FY5"/>
     </row>
-    <row r="6" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="6" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>77</v>
       </c>
@@ -8048,7 +8047,7 @@
       <c r="FX6"/>
       <c r="FY6"/>
     </row>
-    <row r="7" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="7" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>89</v>
       </c>
@@ -8288,7 +8287,7 @@
       <c r="FX7"/>
       <c r="FY7"/>
     </row>
-    <row r="8" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="8" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>101</v>
       </c>
@@ -8532,7 +8531,7 @@
       <c r="FX8"/>
       <c r="FY8"/>
     </row>
-    <row r="9" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="9" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>113</v>
       </c>
@@ -8796,7 +8795,7 @@
       <c r="FX9"/>
       <c r="FY9"/>
     </row>
-    <row r="10" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="10" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>135</v>
       </c>
@@ -9060,7 +9059,7 @@
       <c r="FX10"/>
       <c r="FY10"/>
     </row>
-    <row r="11" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="11" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
         <v>155</v>
       </c>
@@ -9284,7 +9283,7 @@
       <c r="FX11"/>
       <c r="FY11"/>
     </row>
-    <row r="12" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="12" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
         <v>163</v>
       </c>
@@ -9297,8 +9296,8 @@
       <c r="D12" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E12" s="53" t="s">
-        <v>167</v>
+      <c r="E12" s="48" t="s">
+        <v>61</v>
       </c>
       <c r="F12" s="48" t="s">
         <v>163</v>
@@ -9508,7 +9507,7 @@
       <c r="FX12"/>
       <c r="FY12"/>
     </row>
-    <row r="13" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="13" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
         <v>175</v>
       </c>
@@ -9521,8 +9520,8 @@
       <c r="D13" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="53" t="s">
-        <v>167</v>
+      <c r="E13" s="48" t="s">
+        <v>61</v>
       </c>
       <c r="F13" s="48" t="s">
         <v>175</v>
@@ -9744,7 +9743,7 @@
       <c r="FX13"/>
       <c r="FY13"/>
     </row>
-    <row r="14" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="14" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
         <v>184</v>
       </c>
@@ -9982,7 +9981,7 @@
       <c r="FX14"/>
       <c r="FY14"/>
     </row>
-    <row r="15" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="15" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
         <v>196</v>
       </c>
@@ -10234,7 +10233,7 @@
       <c r="FX15"/>
       <c r="FY15"/>
     </row>
-    <row r="16" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="16" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>206</v>
       </c>
@@ -10492,7 +10491,7 @@
       <c r="FX16"/>
       <c r="FY16"/>
     </row>
-    <row r="17" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="17" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
         <v>220</v>
       </c>
@@ -10732,7 +10731,7 @@
       <c r="FX17"/>
       <c r="FY17"/>
     </row>
-    <row r="18" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="18" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
         <v>234</v>
       </c>
@@ -10968,7 +10967,7 @@
       <c r="FX18"/>
       <c r="FY18"/>
     </row>
-    <row r="19" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="19" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
         <v>247</v>
       </c>
@@ -11198,7 +11197,7 @@
       <c r="FX19"/>
       <c r="FY19"/>
     </row>
-    <row r="20" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="20" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
         <v>257</v>
       </c>
@@ -11403,7 +11402,7 @@
       <c r="FX20"/>
       <c r="FY20"/>
     </row>
-    <row r="21" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="21" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
         <v>262</v>
       </c>
@@ -11633,7 +11632,7 @@
       <c r="FX21"/>
       <c r="FY21"/>
     </row>
-    <row r="22" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="22" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>272</v>
       </c>
@@ -11866,7 +11865,7 @@
       <c r="FX22"/>
       <c r="FY22"/>
     </row>
-    <row r="23" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="23" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>283</v>
       </c>
@@ -12098,7 +12097,7 @@
       <c r="FX23"/>
       <c r="FY23"/>
     </row>
-    <row r="24" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="24" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>294</v>
       </c>
@@ -12330,7 +12329,7 @@
       <c r="FX24"/>
       <c r="FY24"/>
     </row>
-    <row r="25" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="25" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>302</v>
       </c>
@@ -12566,7 +12565,7 @@
       <c r="FX25"/>
       <c r="FY25"/>
     </row>
-    <row r="26" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="26" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>310</v>
       </c>
@@ -12797,7 +12796,7 @@
       <c r="FX26"/>
       <c r="FY26"/>
     </row>
-    <row r="27" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="27" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
         <v>317</v>
       </c>
@@ -13053,7 +13052,7 @@
       <c r="FX27"/>
       <c r="FY27"/>
     </row>
-    <row r="28" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="28" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>333</v>
       </c>
@@ -13283,7 +13282,7 @@
       <c r="FX28"/>
       <c r="FY28"/>
     </row>
-    <row r="29" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="29" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
         <v>344</v>
       </c>
@@ -13506,7 +13505,7 @@
       <c r="FX29"/>
       <c r="FY29"/>
     </row>
-    <row r="30" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="30" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
         <v>350</v>
       </c>
@@ -13736,7 +13735,7 @@
       <c r="FX30"/>
       <c r="FY30"/>
     </row>
-    <row r="31" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="31" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
         <v>358</v>
       </c>
@@ -13964,7 +13963,7 @@
       <c r="FX31"/>
       <c r="FY31"/>
     </row>
-    <row r="32" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="32" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
         <v>364</v>
       </c>
@@ -14210,7 +14209,7 @@
       <c r="FX32"/>
       <c r="FY32"/>
     </row>
-    <row r="33" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="33" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
         <v>376</v>
       </c>
@@ -14442,7 +14441,7 @@
       <c r="FX33"/>
       <c r="FY33"/>
     </row>
-    <row r="34" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="34" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
         <v>383</v>
       </c>
@@ -14674,7 +14673,7 @@
       <c r="FX34"/>
       <c r="FY34"/>
     </row>
-    <row r="35" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="35" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
         <v>392</v>
       </c>
@@ -14914,7 +14913,7 @@
       <c r="FX35"/>
       <c r="FY35"/>
     </row>
-    <row r="36" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="36" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
         <v>400</v>
       </c>
@@ -15158,7 +15157,7 @@
       <c r="FX36"/>
       <c r="FY36"/>
     </row>
-    <row r="37" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="37" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
         <v>408</v>
       </c>
@@ -15402,7 +15401,7 @@
       <c r="FX37"/>
       <c r="FY37"/>
     </row>
-    <row r="38" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="38" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
         <v>419</v>
       </c>
@@ -15646,7 +15645,7 @@
       <c r="FX38"/>
       <c r="FY38"/>
     </row>
-    <row r="39" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="39" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
         <v>338</v>
       </c>
@@ -15870,7 +15869,7 @@
       <c r="FX39"/>
       <c r="FY39"/>
     </row>
-    <row r="40" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="40" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
         <v>436</v>
       </c>
@@ -16112,7 +16111,7 @@
       <c r="FX40"/>
       <c r="FY40"/>
     </row>
-    <row r="41" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="41" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
         <v>444</v>
       </c>
@@ -16354,7 +16353,7 @@
       <c r="FX41"/>
       <c r="FY41"/>
     </row>
-    <row r="42" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="42" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
         <v>451</v>
       </c>
@@ -16592,7 +16591,7 @@
       <c r="FX42"/>
       <c r="FY42"/>
     </row>
-    <row r="43" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="43" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
         <v>458</v>
       </c>
@@ -16813,7 +16812,7 @@
       <c r="FX43"/>
       <c r="FY43"/>
     </row>
-    <row r="44" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="44" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
         <v>463</v>
       </c>
@@ -17057,7 +17056,7 @@
       <c r="FX44"/>
       <c r="FY44"/>
     </row>
-    <row r="45" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="45" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="48" t="s">
         <v>470</v>
       </c>
@@ -17281,7 +17280,7 @@
       <c r="FX45"/>
       <c r="FY45"/>
     </row>
-    <row r="46" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="46" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
         <v>475</v>
       </c>
@@ -17525,7 +17524,7 @@
       <c r="FX46"/>
       <c r="FY46"/>
     </row>
-    <row r="47" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="47" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
         <v>482</v>
       </c>
@@ -17757,7 +17756,7 @@
       <c r="FX47"/>
       <c r="FY47"/>
     </row>
-    <row r="48" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="48" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
         <v>488</v>
       </c>
@@ -17989,7 +17988,7 @@
       <c r="FX48"/>
       <c r="FY48"/>
     </row>
-    <row r="49" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="49" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
         <v>494</v>
       </c>
@@ -18231,7 +18230,7 @@
       <c r="FX49"/>
       <c r="FY49"/>
     </row>
-    <row r="50" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="50" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
         <v>501</v>
       </c>
@@ -18458,7 +18457,7 @@
       <c r="FX50"/>
       <c r="FY50"/>
     </row>
-    <row r="51" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="51" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
         <v>509</v>
       </c>
@@ -18679,7 +18678,7 @@
       <c r="FX51"/>
       <c r="FY51"/>
     </row>
-    <row r="52" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="52" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
         <v>516</v>
       </c>
@@ -18906,7 +18905,7 @@
       <c r="FX52"/>
       <c r="FY52"/>
     </row>
-    <row r="53" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="53" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
         <v>520</v>
       </c>
@@ -19162,7 +19161,7 @@
       <c r="FX53"/>
       <c r="FY53"/>
     </row>
-    <row r="54" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="54" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
         <v>532</v>
       </c>
@@ -19400,7 +19399,7 @@
       <c r="FX54"/>
       <c r="FY54"/>
     </row>
-    <row r="55" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="55" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
         <v>541</v>
       </c>
@@ -19652,7 +19651,7 @@
       <c r="FX55"/>
       <c r="FY55"/>
     </row>
-    <row r="56" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="56" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
         <v>550</v>
       </c>
@@ -19891,7 +19890,7 @@
       <c r="FX56"/>
       <c r="FY56"/>
     </row>
-    <row r="57" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="57" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
         <v>557</v>
       </c>
@@ -20129,7 +20128,7 @@
       <c r="FX57"/>
       <c r="FY57"/>
     </row>
-    <row r="58" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="58" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
         <v>565</v>
       </c>
@@ -20367,7 +20366,7 @@
       <c r="FX58"/>
       <c r="FY58"/>
     </row>
-    <row r="59" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="59" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
         <v>573</v>
       </c>
@@ -20607,7 +20606,7 @@
       <c r="FX59"/>
       <c r="FY59"/>
     </row>
-    <row r="60" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="60" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
         <v>581</v>
       </c>
@@ -20823,7 +20822,7 @@
       <c r="FX60"/>
       <c r="FY60"/>
     </row>
-    <row r="61" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="61" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
         <v>586</v>
       </c>
@@ -21061,7 +21060,7 @@
       <c r="FX61"/>
       <c r="FY61"/>
     </row>
-    <row r="62" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="62" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
         <v>594</v>
       </c>
@@ -21299,7 +21298,7 @@
       <c r="FX62"/>
       <c r="FY62"/>
     </row>
-    <row r="63" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="63" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
         <v>602</v>
       </c>
@@ -21529,7 +21528,7 @@
       <c r="FX63"/>
       <c r="FY63"/>
     </row>
-    <row r="64" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="64" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
         <v>610</v>
       </c>
@@ -21751,7 +21750,7 @@
       <c r="FX64"/>
       <c r="FY64"/>
     </row>
-    <row r="65" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="65" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
         <v>615</v>
       </c>
@@ -21991,7 +21990,7 @@
       <c r="FX65"/>
       <c r="FY65"/>
     </row>
-    <row r="66" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="66" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
         <v>621</v>
       </c>
@@ -22212,7 +22211,7 @@
       <c r="FX66"/>
       <c r="FY66"/>
     </row>
-    <row r="67" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="67" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
         <v>626</v>
       </c>
@@ -22437,7 +22436,7 @@
       <c r="FX67"/>
       <c r="FY67"/>
     </row>
-    <row r="68" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="68" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
         <v>631</v>
       </c>
@@ -22695,7 +22694,7 @@
       <c r="FX68"/>
       <c r="FY68"/>
     </row>
-    <row r="69" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="69" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
         <v>647</v>
       </c>
@@ -22941,7 +22940,7 @@
       <c r="FX69"/>
       <c r="FY69"/>
     </row>
-    <row r="70" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="70" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
         <v>657</v>
       </c>
@@ -23180,7 +23179,7 @@
       <c r="FX70"/>
       <c r="FY70"/>
     </row>
-    <row r="71" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="71" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="49" t="s">
         <v>668</v>
       </c>
@@ -23373,7 +23372,7 @@
       <c r="FX71" s="61"/>
       <c r="FY71" s="61"/>
     </row>
-    <row r="72" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="72" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
         <v>675</v>
       </c>
@@ -23613,7 +23612,7 @@
       <c r="FX72"/>
       <c r="FY72"/>
     </row>
-    <row r="73" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="73" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="48" t="s">
         <v>685</v>
       </c>
@@ -23847,7 +23846,7 @@
       <c r="FX73"/>
       <c r="FY73"/>
     </row>
-    <row r="74" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="74" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="48" t="s">
         <v>692</v>
       </c>
@@ -24069,7 +24068,7 @@
       <c r="FX74"/>
       <c r="FY74"/>
     </row>
-    <row r="75" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="75" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
         <v>698</v>
       </c>
@@ -24305,7 +24304,7 @@
       <c r="FX75"/>
       <c r="FY75"/>
     </row>
-    <row r="76" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="76" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="48" t="s">
         <v>708</v>
       </c>
@@ -24533,7 +24532,7 @@
       <c r="FX76"/>
       <c r="FY76"/>
     </row>
-    <row r="77" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="77" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="48" t="s">
         <v>716</v>
       </c>
@@ -24758,7 +24757,7 @@
       <c r="FX77"/>
       <c r="FY77"/>
     </row>
-    <row r="78" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="78" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="48" t="s">
         <v>724</v>
       </c>
@@ -24989,7 +24988,7 @@
       <c r="FX78"/>
       <c r="FY78"/>
     </row>
-    <row r="79" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="79" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="48" t="s">
         <v>733</v>
       </c>
@@ -25225,7 +25224,7 @@
       <c r="FX79"/>
       <c r="FY79"/>
     </row>
-    <row r="80" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="80" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="48" t="s">
         <v>743</v>
       </c>
@@ -25451,7 +25450,7 @@
       <c r="FX80"/>
       <c r="FY80"/>
     </row>
-    <row r="81" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="81" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="48" t="s">
         <v>749</v>
       </c>
@@ -25683,7 +25682,7 @@
       <c r="FX81"/>
       <c r="FY81"/>
     </row>
-    <row r="82" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="82" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="48" t="s">
         <v>755</v>
       </c>
@@ -25921,7 +25920,7 @@
       <c r="FX82"/>
       <c r="FY82"/>
     </row>
-    <row r="83" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="83" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="48" t="s">
         <v>765</v>
       </c>
@@ -26165,7 +26164,7 @@
       <c r="FX83"/>
       <c r="FY83"/>
     </row>
-    <row r="84" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="84" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="48" t="s">
         <v>774</v>
       </c>
@@ -26405,7 +26404,7 @@
       <c r="FX84"/>
       <c r="FY84"/>
     </row>
-    <row r="85" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="85" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="48" t="s">
         <v>781</v>
       </c>
@@ -26645,7 +26644,7 @@
       <c r="FX85"/>
       <c r="FY85"/>
     </row>
-    <row r="86" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="86" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="48" t="s">
         <v>788</v>
       </c>
@@ -26889,7 +26888,7 @@
       <c r="FX86"/>
       <c r="FY86"/>
     </row>
-    <row r="87" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="87" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="48" t="s">
         <v>796</v>
       </c>
@@ -27131,7 +27130,7 @@
       <c r="FX87"/>
       <c r="FY87"/>
     </row>
-    <row r="88" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="88" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="48" t="s">
         <v>803</v>
       </c>
@@ -27375,7 +27374,7 @@
       <c r="FX88"/>
       <c r="FY88"/>
     </row>
-    <row r="89" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="89" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="48" t="s">
         <v>812</v>
       </c>
@@ -27617,7 +27616,7 @@
       <c r="FX89"/>
       <c r="FY89"/>
     </row>
-    <row r="90" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="90" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="48" t="s">
         <v>820</v>
       </c>
@@ -27861,7 +27860,7 @@
       <c r="FX90"/>
       <c r="FY90"/>
     </row>
-    <row r="91" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="91" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="48" t="s">
         <v>829</v>
       </c>
@@ -28115,7 +28114,7 @@
       <c r="FX91"/>
       <c r="FY91"/>
     </row>
-    <row r="92" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="92" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="48" t="s">
         <v>839</v>
       </c>
@@ -28345,7 +28344,7 @@
       <c r="FX92"/>
       <c r="FY92"/>
     </row>
-    <row r="93" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="93" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="48" t="s">
         <v>845</v>
       </c>
@@ -28567,7 +28566,7 @@
       <c r="FX93"/>
       <c r="FY93"/>
     </row>
-    <row r="94" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="94" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="48" t="s">
         <v>853</v>
       </c>
@@ -28793,7 +28792,7 @@
       <c r="FX94"/>
       <c r="FY94"/>
     </row>
-    <row r="95" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="95" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="48" t="s">
         <v>858</v>
       </c>
@@ -29013,7 +29012,7 @@
       <c r="FX95"/>
       <c r="FY95"/>
     </row>
-    <row r="96" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="96" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="48" t="s">
         <v>863</v>
       </c>
@@ -29239,7 +29238,7 @@
       <c r="FX96"/>
       <c r="FY96"/>
     </row>
-    <row r="97" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="97" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="48" t="s">
         <v>870</v>
       </c>
@@ -29448,7 +29447,7 @@
       <c r="FX97"/>
       <c r="FY97"/>
     </row>
-    <row r="98" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="98" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="48" t="s">
         <v>874</v>
       </c>
@@ -29688,7 +29687,7 @@
       <c r="FX98"/>
       <c r="FY98"/>
     </row>
-    <row r="99" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="99" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="48" t="s">
         <v>882</v>
       </c>
@@ -29912,7 +29911,7 @@
       <c r="FX99"/>
       <c r="FY99"/>
     </row>
-    <row r="100" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="100" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="48" t="s">
         <v>889</v>
       </c>
@@ -30136,7 +30135,7 @@
       <c r="FX100"/>
       <c r="FY100"/>
     </row>
-    <row r="101" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="101" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="48" t="s">
         <v>897</v>
       </c>
@@ -30360,7 +30359,7 @@
       <c r="FX101"/>
       <c r="FY101"/>
     </row>
-    <row r="102" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="102" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="48" t="s">
         <v>905</v>
       </c>
@@ -30584,7 +30583,7 @@
       <c r="FX102"/>
       <c r="FY102"/>
     </row>
-    <row r="103" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="103" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="48" t="s">
         <v>913</v>
       </c>
@@ -30810,7 +30809,7 @@
       <c r="FX103"/>
       <c r="FY103"/>
     </row>
-    <row r="104" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="104" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="48" t="s">
         <v>921</v>
       </c>
@@ -31036,7 +31035,7 @@
       <c r="FX104"/>
       <c r="FY104"/>
     </row>
-    <row r="105" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="105" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="48" t="s">
         <v>926</v>
       </c>
@@ -31266,7 +31265,7 @@
       <c r="FX105"/>
       <c r="FY105"/>
     </row>
-    <row r="106" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="106" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="48" t="s">
         <v>933</v>
       </c>
@@ -31496,7 +31495,7 @@
       <c r="FX106"/>
       <c r="FY106"/>
     </row>
-    <row r="107" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="107" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="48" t="s">
         <v>939</v>
       </c>
@@ -31724,7 +31723,7 @@
       <c r="FX107"/>
       <c r="FY107"/>
     </row>
-    <row r="108" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="108" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="48" t="s">
         <v>946</v>
       </c>
@@ -31954,7 +31953,7 @@
       <c r="FX108"/>
       <c r="FY108"/>
     </row>
-    <row r="109" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="109" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="48" t="s">
         <v>953</v>
       </c>
@@ -32178,7 +32177,7 @@
       <c r="FX109"/>
       <c r="FY109"/>
     </row>
-    <row r="110" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="110" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="48" t="s">
         <v>960</v>
       </c>
@@ -32408,7 +32407,7 @@
       <c r="FX110"/>
       <c r="FY110"/>
     </row>
-    <row r="111" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1">
+    <row r="111" spans="1:181" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="48" t="s">
         <v>967</v>
       </c>
@@ -32632,7 +32631,7 @@
       <c r="FX111"/>
       <c r="FY111"/>
     </row>
-    <row r="112" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="112" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="48" t="s">
         <v>974</v>
       </c>
@@ -32831,7 +32830,7 @@
       <c r="FX112"/>
       <c r="FY112"/>
     </row>
-    <row r="113" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="113" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="48" t="s">
         <v>981</v>
       </c>
@@ -33030,7 +33029,7 @@
       <c r="FX113"/>
       <c r="FY113"/>
     </row>
-    <row r="114" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="114" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="48" t="s">
         <v>988</v>
       </c>
@@ -33229,7 +33228,7 @@
       <c r="FX114"/>
       <c r="FY114"/>
     </row>
-    <row r="115" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="115" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="48" t="s">
         <v>994</v>
       </c>
@@ -33426,7 +33425,7 @@
       <c r="FX115"/>
       <c r="FY115"/>
     </row>
-    <row r="116" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="116" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="48" t="s">
         <v>1000</v>
       </c>
@@ -33623,7 +33622,7 @@
       <c r="FX116"/>
       <c r="FY116"/>
     </row>
-    <row r="117" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="117" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="48" t="s">
         <v>1006</v>
       </c>
@@ -33820,7 +33819,7 @@
       <c r="FX117"/>
       <c r="FY117"/>
     </row>
-    <row r="118" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="118" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="48" t="s">
         <v>1012</v>
       </c>
@@ -34017,7 +34016,7 @@
       <c r="FX118"/>
       <c r="FY118"/>
     </row>
-    <row r="119" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="119" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="48" t="s">
         <v>1018</v>
       </c>
@@ -34214,7 +34213,7 @@
       <c r="FX119"/>
       <c r="FY119"/>
     </row>
-    <row r="120" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="120" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="48" t="s">
         <v>1024</v>
       </c>
@@ -34413,7 +34412,7 @@
       <c r="FX120"/>
       <c r="FY120"/>
     </row>
-    <row r="121" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="121" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="48" t="s">
         <v>1030</v>
       </c>
@@ -34618,7 +34617,7 @@
       <c r="FX121"/>
       <c r="FY121"/>
     </row>
-    <row r="122" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="122" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="48" t="s">
         <v>1038</v>
       </c>
@@ -34823,7 +34822,7 @@
       <c r="FX122"/>
       <c r="FY122"/>
     </row>
-    <row r="123" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="123" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="48" t="s">
         <v>1044</v>
       </c>
@@ -35026,7 +35025,7 @@
       <c r="FX123"/>
       <c r="FY123"/>
     </row>
-    <row r="124" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="124" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="48" t="s">
         <v>1051</v>
       </c>
@@ -35229,7 +35228,7 @@
       <c r="FX124"/>
       <c r="FY124"/>
     </row>
-    <row r="125" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="125" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="48" t="s">
         <v>1056</v>
       </c>
@@ -35428,7 +35427,7 @@
       <c r="FX125"/>
       <c r="FY125"/>
     </row>
-    <row r="126" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="126" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="48" t="s">
         <v>1063</v>
       </c>
@@ -35637,7 +35636,7 @@
       <c r="FX126"/>
       <c r="FY126"/>
     </row>
-    <row r="127" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="127" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="48" t="s">
         <v>1068</v>
       </c>
@@ -35840,7 +35839,7 @@
       <c r="FX127"/>
       <c r="FY127"/>
     </row>
-    <row r="128" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="128" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="48" t="s">
         <v>1073</v>
       </c>
@@ -36045,7 +36044,7 @@
       <c r="FX128"/>
       <c r="FY128"/>
     </row>
-    <row r="129" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="129" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="48" t="s">
         <v>1080</v>
       </c>
@@ -36250,7 +36249,7 @@
       <c r="FX129"/>
       <c r="FY129"/>
     </row>
-    <row r="130" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="130" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="48" t="s">
         <v>1089</v>
       </c>
@@ -36453,7 +36452,7 @@
       <c r="FX130"/>
       <c r="FY130"/>
     </row>
-    <row r="131" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="131" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="48" t="s">
         <v>1095</v>
       </c>
@@ -36656,7 +36655,7 @@
       <c r="FX131"/>
       <c r="FY131"/>
     </row>
-    <row r="132" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="132" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="48" t="s">
         <v>1101</v>
       </c>
@@ -36859,7 +36858,7 @@
       <c r="FX132"/>
       <c r="FY132"/>
     </row>
-    <row r="133" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="133" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="48" t="s">
         <v>1106</v>
       </c>
@@ -37064,7 +37063,7 @@
       <c r="FX133"/>
       <c r="FY133"/>
     </row>
-    <row r="134" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="134" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="48" t="s">
         <v>1114</v>
       </c>
@@ -37272,7 +37271,7 @@
       <c r="FX134"/>
       <c r="FY134"/>
     </row>
-    <row r="135" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="135" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="48" t="s">
         <v>1121</v>
       </c>
@@ -37469,7 +37468,7 @@
       <c r="FX135"/>
       <c r="FY135"/>
     </row>
-    <row r="136" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="136" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="48" t="s">
         <v>1127</v>
       </c>
@@ -37666,7 +37665,7 @@
       <c r="FX136"/>
       <c r="FY136"/>
     </row>
-    <row r="137" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="137" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="48" t="s">
         <v>1133</v>
       </c>
@@ -37865,7 +37864,7 @@
       <c r="FX137"/>
       <c r="FY137"/>
     </row>
-    <row r="138" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="138" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="53" t="s">
         <v>1140</v>
       </c>
@@ -38028,7 +38027,7 @@
       <c r="FX138"/>
       <c r="FY138"/>
     </row>
-    <row r="139" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="139" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="53" t="s">
         <v>1144</v>
       </c>
@@ -38191,7 +38190,7 @@
       <c r="FX139"/>
       <c r="FY139"/>
     </row>
-    <row r="140" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="140" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="53" t="s">
         <v>1149</v>
       </c>
@@ -38354,7 +38353,7 @@
       <c r="FX140"/>
       <c r="FY140"/>
     </row>
-    <row r="141" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="141" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="53" t="s">
         <v>1153</v>
       </c>
@@ -38517,7 +38516,7 @@
       <c r="FX141"/>
       <c r="FY141"/>
     </row>
-    <row r="142" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="142" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="53" t="s">
         <v>736</v>
       </c>
@@ -38676,7 +38675,7 @@
       <c r="FX142"/>
       <c r="FY142"/>
     </row>
-    <row r="143" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="143" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="53" t="s">
         <v>1159</v>
       </c>
@@ -38852,7 +38851,7 @@
       <c r="FX143"/>
       <c r="FY143"/>
     </row>
-    <row r="144" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="144" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="53" t="s">
         <v>1167</v>
       </c>
@@ -39028,7 +39027,7 @@
       <c r="FX144"/>
       <c r="FY144"/>
     </row>
-    <row r="145" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="145" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="53" t="s">
         <v>1172</v>
       </c>
@@ -39204,7 +39203,7 @@
       <c r="FX145"/>
       <c r="FY145"/>
     </row>
-    <row r="146" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="146" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="53" t="s">
         <v>1177</v>
       </c>
@@ -39380,7 +39379,7 @@
       <c r="FX146"/>
       <c r="FY146"/>
     </row>
-    <row r="147" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="147" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="53" t="s">
         <v>1182</v>
       </c>
@@ -39556,7 +39555,7 @@
       <c r="FX147"/>
       <c r="FY147"/>
     </row>
-    <row r="148" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="148" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="53" t="s">
         <v>1187</v>
       </c>
@@ -39732,7 +39731,7 @@
       <c r="FX148"/>
       <c r="FY148"/>
     </row>
-    <row r="149" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="149" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="53" t="s">
         <v>1192</v>
       </c>
@@ -39908,7 +39907,7 @@
       <c r="FX149"/>
       <c r="FY149"/>
     </row>
-    <row r="150" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="150" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="53" t="s">
         <v>1197</v>
       </c>
@@ -40084,7 +40083,7 @@
       <c r="FX150"/>
       <c r="FY150"/>
     </row>
-    <row r="151" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="151" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="53" t="s">
         <v>1202</v>
       </c>
@@ -40260,7 +40259,7 @@
       <c r="FX151"/>
       <c r="FY151"/>
     </row>
-    <row r="152" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="152" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="53" t="s">
         <v>1207</v>
       </c>
@@ -40436,7 +40435,7 @@
       <c r="FX152"/>
       <c r="FY152"/>
     </row>
-    <row r="153" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="153" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="53" t="s">
         <v>1212</v>
       </c>
@@ -40612,7 +40611,7 @@
       <c r="FX153"/>
       <c r="FY153"/>
     </row>
-    <row r="154" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="154" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="53" t="s">
         <v>1217</v>
       </c>
@@ -40788,7 +40787,7 @@
       <c r="FX154"/>
       <c r="FY154"/>
     </row>
-    <row r="155" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="155" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="53" t="s">
         <v>1222</v>
       </c>
@@ -40964,7 +40963,7 @@
       <c r="FX155"/>
       <c r="FY155"/>
     </row>
-    <row r="156" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="156" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="53" t="s">
         <v>1227</v>
       </c>
@@ -41140,7 +41139,7 @@
       <c r="FX156"/>
       <c r="FY156"/>
     </row>
-    <row r="157" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="157" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="53" t="s">
         <v>1232</v>
       </c>
@@ -41366,7 +41365,7 @@
       <c r="FX157"/>
       <c r="FY157"/>
     </row>
-    <row r="158" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="158" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="53" t="str">
         <f>SUBSTITUTE(A143,"ictv","ncbi")</f>
         <v>ncbi_realm</v>
@@ -41537,7 +41536,7 @@
       <c r="FX158"/>
       <c r="FY158"/>
     </row>
-    <row r="159" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="159" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="53" t="s">
         <v>1243</v>
       </c>
@@ -41707,7 +41706,7 @@
       <c r="FX159"/>
       <c r="FY159"/>
     </row>
-    <row r="160" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="160" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="53" t="s">
         <v>1247</v>
       </c>
@@ -41905,7 +41904,7 @@
       <c r="FX160"/>
       <c r="FY160"/>
     </row>
-    <row r="161" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="161" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="53" t="s">
         <v>1252</v>
       </c>
@@ -42075,7 +42074,7 @@
       <c r="FX161"/>
       <c r="FY161"/>
     </row>
-    <row r="162" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="162" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="53" t="s">
         <v>1256</v>
       </c>
@@ -42273,7 +42272,7 @@
       <c r="FX162"/>
       <c r="FY162"/>
     </row>
-    <row r="163" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="163" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="53" t="s">
         <v>1261</v>
       </c>
@@ -42443,7 +42442,7 @@
       <c r="FX163"/>
       <c r="FY163"/>
     </row>
-    <row r="164" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="164" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="53" t="s">
         <v>1265</v>
       </c>
@@ -42641,7 +42640,7 @@
       <c r="FX164"/>
       <c r="FY164"/>
     </row>
-    <row r="165" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="165" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="53" t="s">
         <v>1270</v>
       </c>
@@ -42811,7 +42810,7 @@
       <c r="FX165"/>
       <c r="FY165"/>
     </row>
-    <row r="166" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="166" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="53" t="s">
         <v>1274</v>
       </c>
@@ -43009,7 +43008,7 @@
       <c r="FX166"/>
       <c r="FY166"/>
     </row>
-    <row r="167" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="167" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="53" t="s">
         <v>1279</v>
       </c>
@@ -43179,7 +43178,7 @@
       <c r="FX167"/>
       <c r="FY167"/>
     </row>
-    <row r="168" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="168" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="53" t="s">
         <v>1283</v>
       </c>
@@ -43414,7 +43413,7 @@
       <c r="FX168"/>
       <c r="FY168"/>
     </row>
-    <row r="169" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="169" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="53" t="s">
         <v>1290</v>
       </c>
@@ -43584,7 +43583,7 @@
       <c r="FX169"/>
       <c r="FY169"/>
     </row>
-    <row r="170" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="170" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="53" t="s">
         <v>1294</v>
       </c>
@@ -43819,7 +43818,7 @@
       <c r="FX170"/>
       <c r="FY170"/>
     </row>
-    <row r="171" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="171" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="53" t="s">
         <v>1301</v>
       </c>
@@ -43989,7 +43988,7 @@
       <c r="FX171"/>
       <c r="FY171"/>
     </row>
-    <row r="172" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="172" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="53" t="s">
         <v>1305</v>
       </c>
@@ -44234,7 +44233,7 @@
       <c r="FX172"/>
       <c r="FY172"/>
     </row>
-    <row r="173" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="173" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="48" t="s">
         <v>1315</v>
       </c>
@@ -44462,7 +44461,7 @@
       <c r="FX173"/>
       <c r="FY173"/>
     </row>
-    <row r="174" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="174" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="48" t="s">
         <v>1322</v>
       </c>
@@ -44706,7 +44705,7 @@
       <c r="FX174"/>
       <c r="FY174"/>
     </row>
-    <row r="175" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="175" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="48" t="s">
         <v>1331</v>
       </c>
@@ -44878,7 +44877,7 @@
       <c r="FX175"/>
       <c r="FY175"/>
     </row>
-    <row r="176" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="176" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="48" t="s">
         <v>1336</v>
       </c>
@@ -45106,7 +45105,7 @@
       <c r="FX176"/>
       <c r="FY176"/>
     </row>
-    <row r="177" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="177" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="53" t="s">
         <v>1344</v>
       </c>
@@ -45272,7 +45271,7 @@
       <c r="FX177"/>
       <c r="FY177"/>
     </row>
-    <row r="178" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="178" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="53" t="s">
         <v>1349</v>
       </c>
@@ -45523,7 +45522,7 @@
       <c r="FX178"/>
       <c r="FY178"/>
     </row>
-    <row r="179" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="179" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="53" t="s">
         <v>1357</v>
       </c>
@@ -45692,7 +45691,7 @@
       <c r="FX179"/>
       <c r="FY179"/>
     </row>
-    <row r="180" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="180" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="48" t="s">
         <v>1361</v>
       </c>
@@ -45924,7 +45923,7 @@
       <c r="FX180"/>
       <c r="FY180"/>
     </row>
-    <row r="181" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="181" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="53" t="s">
         <v>1369</v>
       </c>
@@ -46118,7 +46117,7 @@
       <c r="FX181"/>
       <c r="FY181"/>
     </row>
-    <row r="182" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="182" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="53" t="s">
         <v>1375</v>
       </c>
@@ -46284,7 +46283,7 @@
       <c r="FX182"/>
       <c r="FY182"/>
     </row>
-    <row r="183" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1">
+    <row r="183" spans="1:181" s="53" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="53" t="s">
         <v>1379</v>
       </c>
@@ -46297,8 +46296,8 @@
       <c r="D183" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="E183" s="53" t="s">
-        <v>167</v>
+      <c r="E183" s="48" t="s">
+        <v>61</v>
       </c>
       <c r="V183" s="48" t="str">
         <f t="shared" si="6"/>
@@ -46450,7 +46449,7 @@
       <c r="FX183"/>
       <c r="FY183"/>
     </row>
-    <row r="184" spans="1:181" ht="23.25" customHeight="1">
+    <row r="184" spans="1:181" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>1383</v>
       </c>
@@ -46483,7 +46482,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="185" spans="1:181" ht="23.25" customHeight="1">
+    <row r="185" spans="1:181" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>1388</v>
       </c>
@@ -46526,7 +46525,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="186" spans="1:181" ht="23.25" customHeight="1">
+    <row r="186" spans="1:181" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>1393</v>
       </c>
@@ -46565,7 +46564,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="187" spans="1:181" ht="23.25" customHeight="1">
+    <row r="187" spans="1:181" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>1398</v>
       </c>
@@ -46607,7 +46606,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="188" spans="1:181" ht="23.25" customHeight="1">
+    <row r="188" spans="1:181" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>1403</v>
       </c>
@@ -46664,7 +46663,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="189" spans="1:181" ht="23.25" customHeight="1">
+    <row r="189" spans="1:181" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>1407</v>
       </c>
@@ -46695,7 +46694,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="190" spans="1:181" ht="23.25" customHeight="1">
+    <row r="190" spans="1:181" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>1410</v>
       </c>
@@ -46728,7 +46727,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="191" spans="1:181" ht="23.25" customHeight="1">
+    <row r="191" spans="1:181" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>1414</v>
       </c>
@@ -46761,7 +46760,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="192" spans="1:181" ht="23.25" customHeight="1">
+    <row r="192" spans="1:181" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>1419</v>
       </c>
@@ -46794,7 +46793,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="193" spans="1:53" ht="23.25" customHeight="1">
+    <row r="193" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>1423</v>
       </c>
@@ -46822,7 +46821,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="194" spans="1:53" ht="23.25" customHeight="1">
+    <row r="194" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>1428</v>
       </c>
@@ -46850,7 +46849,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="195" spans="1:53" ht="23.25" customHeight="1">
+    <row r="195" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>1431</v>
       </c>
@@ -46884,7 +46883,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="196" spans="1:53" ht="23.25" customHeight="1">
+    <row r="196" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>1435</v>
       </c>
@@ -46915,7 +46914,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="197" spans="1:53" ht="23.25" customHeight="1">
+    <row r="197" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>1439</v>
       </c>
@@ -46957,7 +46956,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="198" spans="1:53" ht="23.25" customHeight="1">
+    <row r="198" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>1443</v>
       </c>
@@ -46987,7 +46986,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="199" spans="1:53" ht="23.25" customHeight="1">
+    <row r="199" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>1447</v>
       </c>
@@ -47020,8 +47019,8 @@
         <v>219</v>
       </c>
     </row>
-    <row r="200" spans="1:53" ht="23.25" customHeight="1">
-      <c r="A200" s="68" t="s">
+    <row r="200" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="67" t="s">
         <v>1453</v>
       </c>
       <c r="B200" s="49" t="s">
@@ -47069,8 +47068,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="201" spans="1:53" ht="23.25" customHeight="1">
-      <c r="A201" s="69" t="s">
+    <row r="201" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="68" t="s">
         <v>1458</v>
       </c>
       <c r="B201" s="62" t="s">
@@ -47112,8 +47111,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="202" spans="1:53" ht="23.25" customHeight="1">
-      <c r="A202" s="70" t="s">
+    <row r="202" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="69" t="s">
         <v>1462</v>
       </c>
       <c r="B202" s="49" t="s">
@@ -47153,8 +47152,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="203" spans="1:53" ht="23.25" customHeight="1">
-      <c r="A203" s="70" t="s">
+    <row r="203" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="69" t="s">
         <v>1466</v>
       </c>
       <c r="B203" s="49" t="s">
@@ -47197,8 +47196,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="204" spans="1:53" ht="23.25" customHeight="1">
-      <c r="A204" s="70" t="s">
+    <row r="204" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="69" t="s">
         <v>1470</v>
       </c>
       <c r="B204" s="49" t="s">
@@ -47243,8 +47242,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="205" spans="1:53" ht="23.25" customHeight="1">
-      <c r="A205" s="70" t="s">
+    <row r="205" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="69" t="s">
         <v>1474</v>
       </c>
       <c r="B205" s="49" t="s">
@@ -47289,8 +47288,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="206" spans="1:53" ht="23.25" customHeight="1">
-      <c r="A206" s="70" t="s">
+    <row r="206" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="69" t="s">
         <v>1478</v>
       </c>
       <c r="B206" s="65" t="s">
@@ -47325,8 +47324,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="207" spans="1:53" ht="23.25" customHeight="1">
-      <c r="A207" s="70" t="s">
+    <row r="207" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="69" t="s">
         <v>1482</v>
       </c>
       <c r="B207" s="64" t="s">
@@ -47357,15 +47356,15 @@
       <c r="W207" t="s">
         <v>1451</v>
       </c>
-      <c r="AW207" s="67" t="s">
+      <c r="AW207" t="s">
         <v>1485</v>
       </c>
       <c r="AY207" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="208" spans="1:53" ht="23.25" customHeight="1">
-      <c r="A208" s="70" t="s">
+    <row r="208" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="69" t="s">
         <v>1486</v>
       </c>
       <c r="B208" t="s">
@@ -47393,7 +47392,7 @@
       <c r="W208" t="s">
         <v>14</v>
       </c>
-      <c r="AW208" s="67" t="s">
+      <c r="AW208" t="s">
         <v>1457</v>
       </c>
       <c r="AY208" t="s">
@@ -47406,8 +47405,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="209" spans="1:51" ht="23.25" customHeight="1">
-      <c r="A209" s="70" t="s">
+    <row r="209" spans="1:51" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="69" t="s">
         <v>1489</v>
       </c>
       <c r="B209" s="65" t="s">
@@ -47429,15 +47428,15 @@
       <c r="W209" t="s">
         <v>14</v>
       </c>
-      <c r="AW209" s="67" t="s">
+      <c r="AW209" t="s">
         <v>1492</v>
       </c>
       <c r="AY209" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="210" spans="1:51" ht="23.25" customHeight="1">
-      <c r="A210" s="70" t="s">
+    <row r="210" spans="1:51" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="69" t="s">
         <v>1493</v>
       </c>
       <c r="B210" s="49" t="s">
@@ -47472,15 +47471,15 @@
       </c>
       <c r="AU210" s="49"/>
       <c r="AV210" s="49"/>
-      <c r="AW210" s="67" t="s">
+      <c r="AW210" t="s">
         <v>1496</v>
       </c>
       <c r="AY210" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="211" spans="1:51" ht="23.25" customHeight="1">
-      <c r="A211" s="70" t="s">
+    <row r="211" spans="1:51" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="69" t="s">
         <v>1497</v>
       </c>
       <c r="B211" s="49" t="s">
@@ -47511,7 +47510,7 @@
       <c r="AT211" s="48" t="s">
         <v>406</v>
       </c>
-      <c r="AW211" s="67" t="s">
+      <c r="AW211" t="s">
         <v>1500</v>
       </c>
       <c r="AY211" t="s">
@@ -47543,12 +47542,12 @@
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="40" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:172" s="19" customFormat="1" ht="23.25" customHeight="1">
+    <row r="1" spans="1:172" s="19" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -47808,7 +47807,7 @@
       <c r="FO1" s="29"/>
       <c r="FP1" s="29"/>
     </row>
-    <row r="2" spans="1:172" s="19" customFormat="1" ht="23.25" customHeight="1">
+    <row r="2" spans="1:172" s="19" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>16</v>
       </c>
@@ -48068,7 +48067,7 @@
       <c r="FO2" s="29"/>
       <c r="FP2" s="29"/>
     </row>
-    <row r="3" spans="1:172" s="19" customFormat="1" ht="23.25" customHeight="1">
+    <row r="3" spans="1:172" s="19" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="str">
         <f t="shared" ref="A3:AQ3" si="0">_xlfn.TEXTJOIN(" ", TRUE, LOWER(A1), LOWER(A2))</f>
         <v>vjdbv0.3 field id</v>
@@ -48371,7 +48370,7 @@
       <c r="FO3" s="29"/>
       <c r="FP3" s="29"/>
     </row>
-    <row r="4" spans="1:172" s="22" customFormat="1" ht="23.25" customHeight="1">
+    <row r="4" spans="1:172" s="22" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="str">
         <f t="shared" ref="A4:AQ4" si="1">SUBSTITUTE(A3, " ", "_")</f>
         <v>vjdbv0.3_field_id</v>
@@ -48674,7 +48673,7 @@
       <c r="FO4" s="29"/>
       <c r="FP4" s="29"/>
     </row>
-    <row r="5" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="5" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -48741,7 +48740,7 @@
       <c r="AN5" s="8"/>
       <c r="AO5" s="27"/>
     </row>
-    <row r="6" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="6" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -48812,7 +48811,7 @@
       <c r="AN6" s="13"/>
       <c r="AO6" s="28"/>
     </row>
-    <row r="7" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="7" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -48881,7 +48880,7 @@
       <c r="AN7" s="13"/>
       <c r="AO7" s="28"/>
     </row>
-    <row r="8" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="8" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -48948,7 +48947,7 @@
       <c r="AN8" s="13"/>
       <c r="AO8" s="28"/>
     </row>
-    <row r="9" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="9" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -49015,7 +49014,7 @@
       <c r="AN9" s="13"/>
       <c r="AO9" s="28"/>
     </row>
-    <row r="10" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="10" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -49086,7 +49085,7 @@
       <c r="AN10" s="13"/>
       <c r="AO10" s="28"/>
     </row>
-    <row r="11" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="11" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -49157,7 +49156,7 @@
       <c r="AN11" s="13"/>
       <c r="AO11" s="28"/>
     </row>
-    <row r="12" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="12" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -49224,7 +49223,7 @@
       <c r="AN12" s="13"/>
       <c r="AO12" s="28"/>
     </row>
-    <row r="13" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="13" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -49291,7 +49290,7 @@
       <c r="AN13" s="13"/>
       <c r="AO13" s="28"/>
     </row>
-    <row r="14" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="14" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -49364,7 +49363,7 @@
       <c r="AN14" s="13"/>
       <c r="AO14" s="28"/>
     </row>
-    <row r="15" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="15" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -49433,7 +49432,7 @@
       <c r="AN15" s="13"/>
       <c r="AO15" s="28"/>
     </row>
-    <row r="16" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="16" spans="1:172" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -49500,7 +49499,7 @@
       <c r="AN16" s="13"/>
       <c r="AO16" s="28"/>
     </row>
-    <row r="17" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="17" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -49573,7 +49572,7 @@
       <c r="AN17" s="13"/>
       <c r="AO17" s="28"/>
     </row>
-    <row r="18" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="18" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -49646,7 +49645,7 @@
       <c r="AN18" s="13"/>
       <c r="AO18" s="28"/>
     </row>
-    <row r="19" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="19" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -49719,7 +49718,7 @@
       <c r="AN19" s="13"/>
       <c r="AO19" s="28"/>
     </row>
-    <row r="20" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="20" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -49790,7 +49789,7 @@
       <c r="AN20" s="13"/>
       <c r="AO20" s="28"/>
     </row>
-    <row r="21" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="21" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -49835,7 +49834,7 @@
       <c r="AN21" s="13"/>
       <c r="AO21" s="28"/>
     </row>
-    <row r="22" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="22" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -49908,7 +49907,7 @@
       <c r="AN22" s="13"/>
       <c r="AO22" s="28"/>
     </row>
-    <row r="23" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="23" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -49981,7 +49980,7 @@
       <c r="AN23" s="13"/>
       <c r="AO23" s="28"/>
     </row>
-    <row r="24" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="24" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -50052,7 +50051,7 @@
       <c r="AN24" s="13"/>
       <c r="AO24" s="28"/>
     </row>
-    <row r="25" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="25" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -50119,7 +50118,7 @@
       <c r="AN25" s="13"/>
       <c r="AO25" s="28"/>
     </row>
-    <row r="26" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="26" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -50190,7 +50189,7 @@
       <c r="AN26" s="13"/>
       <c r="AO26" s="28"/>
     </row>
-    <row r="27" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="27" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -50263,7 +50262,7 @@
       <c r="AN27" s="13"/>
       <c r="AO27" s="28"/>
     </row>
-    <row r="28" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="28" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -50336,7 +50335,7 @@
       <c r="AN28" s="13"/>
       <c r="AO28" s="28"/>
     </row>
-    <row r="29" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="29" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -50409,7 +50408,7 @@
       <c r="AN29" s="13"/>
       <c r="AO29" s="28"/>
     </row>
-    <row r="30" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="30" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -50478,7 +50477,7 @@
       <c r="AN30" s="13"/>
       <c r="AO30" s="28"/>
     </row>
-    <row r="31" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="31" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -50547,7 +50546,7 @@
       <c r="AN31" s="13"/>
       <c r="AO31" s="28"/>
     </row>
-    <row r="32" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="32" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -50618,7 +50617,7 @@
       <c r="AN32" s="13"/>
       <c r="AO32" s="28"/>
     </row>
-    <row r="33" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="33" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -50685,7 +50684,7 @@
       <c r="AN33" s="13"/>
       <c r="AO33" s="28"/>
     </row>
-    <row r="34" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="34" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -50756,7 +50755,7 @@
       <c r="AN34" s="13"/>
       <c r="AO34" s="28"/>
     </row>
-    <row r="35" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="35" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -50825,7 +50824,7 @@
       <c r="AN35" s="13"/>
       <c r="AO35" s="28"/>
     </row>
-    <row r="36" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="36" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -50892,7 +50891,7 @@
       <c r="AN36" s="13"/>
       <c r="AO36" s="28"/>
     </row>
-    <row r="37" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="37" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -50965,7 +50964,7 @@
       <c r="AN37" s="13"/>
       <c r="AO37" s="28"/>
     </row>
-    <row r="38" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="38" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -51038,7 +51037,7 @@
       <c r="AN38" s="13"/>
       <c r="AO38" s="28"/>
     </row>
-    <row r="39" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="39" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -51111,7 +51110,7 @@
       <c r="AN39" s="13"/>
       <c r="AO39" s="28"/>
     </row>
-    <row r="40" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="40" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -51182,7 +51181,7 @@
       <c r="AN40" s="13"/>
       <c r="AO40" s="28"/>
     </row>
-    <row r="41" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="41" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -51255,7 +51254,7 @@
       <c r="AN41" s="13"/>
       <c r="AO41" s="28"/>
     </row>
-    <row r="42" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="42" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -51322,7 +51321,7 @@
       <c r="AN42" s="13"/>
       <c r="AO42" s="28"/>
     </row>
-    <row r="43" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="43" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -51393,7 +51392,7 @@
       <c r="AN43" s="13"/>
       <c r="AO43" s="28"/>
     </row>
-    <row r="44" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="44" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -51464,7 +51463,7 @@
       <c r="AN44" s="13"/>
       <c r="AO44" s="28"/>
     </row>
-    <row r="45" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="45" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -51535,7 +51534,7 @@
       <c r="AN45" s="13"/>
       <c r="AO45" s="28"/>
     </row>
-    <row r="46" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="46" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -51602,7 +51601,7 @@
       <c r="AN46" s="13"/>
       <c r="AO46" s="28"/>
     </row>
-    <row r="47" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="47" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -51673,7 +51672,7 @@
       <c r="AN47" s="13"/>
       <c r="AO47" s="28"/>
     </row>
-    <row r="48" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="48" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -51740,7 +51739,7 @@
       <c r="AN48" s="13"/>
       <c r="AO48" s="28"/>
     </row>
-    <row r="49" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="49" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -51811,7 +51810,7 @@
       <c r="AN49" s="13"/>
       <c r="AO49" s="28"/>
     </row>
-    <row r="50" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="50" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -51878,7 +51877,7 @@
       <c r="AN50" s="13"/>
       <c r="AO50" s="28"/>
     </row>
-    <row r="51" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="51" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -51947,7 +51946,7 @@
       <c r="AN51" s="13"/>
       <c r="AO51" s="28"/>
     </row>
-    <row r="52" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="52" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -52016,7 +52015,7 @@
       <c r="AN52" s="13"/>
       <c r="AO52" s="28"/>
     </row>
-    <row r="53" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="53" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -52089,7 +52088,7 @@
       <c r="AN53" s="13"/>
       <c r="AO53" s="28"/>
     </row>
-    <row r="54" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="54" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -52158,7 +52157,7 @@
       <c r="AN54" s="13"/>
       <c r="AO54" s="28"/>
     </row>
-    <row r="55" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="55" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -52231,7 +52230,7 @@
       <c r="AN55" s="13"/>
       <c r="AO55" s="28"/>
     </row>
-    <row r="56" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="56" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -52255,7 +52254,7 @@
       <c r="AN56" s="13"/>
       <c r="AO56" s="28"/>
     </row>
-    <row r="57" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="57" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -52324,7 +52323,7 @@
       <c r="AN57" s="13"/>
       <c r="AO57" s="28"/>
     </row>
-    <row r="58" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="58" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -52393,7 +52392,7 @@
       <c r="AN58" s="13"/>
       <c r="AO58" s="28"/>
     </row>
-    <row r="59" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="59" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -52466,7 +52465,7 @@
       <c r="AN59" s="13"/>
       <c r="AO59" s="28"/>
     </row>
-    <row r="60" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="60" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -52535,7 +52534,7 @@
       <c r="AN60" s="13"/>
       <c r="AO60" s="28"/>
     </row>
-    <row r="61" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="61" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -52606,7 +52605,7 @@
       <c r="AN61" s="13"/>
       <c r="AO61" s="28"/>
     </row>
-    <row r="62" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="62" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -52673,7 +52672,7 @@
       <c r="AN62" s="13"/>
       <c r="AO62" s="28"/>
     </row>
-    <row r="63" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="63" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -52744,7 +52743,7 @@
       <c r="AN63" s="13"/>
       <c r="AO63" s="28"/>
     </row>
-    <row r="64" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="64" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -52811,7 +52810,7 @@
       <c r="AN64" s="13"/>
       <c r="AO64" s="28"/>
     </row>
-    <row r="65" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="65" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -52880,7 +52879,7 @@
       <c r="AN65" s="13"/>
       <c r="AO65" s="28"/>
     </row>
-    <row r="66" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="66" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -52947,7 +52946,7 @@
       <c r="AN66" s="13"/>
       <c r="AO66" s="28"/>
     </row>
-    <row r="67" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="67" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -52971,7 +52970,7 @@
       <c r="AN67" s="13"/>
       <c r="AO67" s="28"/>
     </row>
-    <row r="68" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="68" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -53038,7 +53037,7 @@
       <c r="AN68" s="13"/>
       <c r="AO68" s="28"/>
     </row>
-    <row r="69" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="69" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -53109,7 +53108,7 @@
       <c r="AN69" s="13"/>
       <c r="AO69" s="28"/>
     </row>
-    <row r="70" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="70" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -53182,7 +53181,7 @@
       <c r="AN70" s="13"/>
       <c r="AO70" s="28"/>
     </row>
-    <row r="71" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="71" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -53253,7 +53252,7 @@
       <c r="AN71" s="13"/>
       <c r="AO71" s="28"/>
     </row>
-    <row r="72" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="72" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -53324,7 +53323,7 @@
       <c r="AN72" s="13"/>
       <c r="AO72" s="28"/>
     </row>
-    <row r="73" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="73" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -53393,7 +53392,7 @@
       <c r="AN73" s="13"/>
       <c r="AO73" s="28"/>
     </row>
-    <row r="74" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="74" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -53466,7 +53465,7 @@
       <c r="AN74" s="13"/>
       <c r="AO74" s="28"/>
     </row>
-    <row r="75" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="75" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -53533,7 +53532,7 @@
       <c r="AN75" s="13"/>
       <c r="AO75" s="28"/>
     </row>
-    <row r="76" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="76" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -53600,7 +53599,7 @@
       <c r="AN76" s="13"/>
       <c r="AO76" s="28"/>
     </row>
-    <row r="77" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="77" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -53669,7 +53668,7 @@
       <c r="AN77" s="13"/>
       <c r="AO77" s="28"/>
     </row>
-    <row r="78" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="78" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -53738,7 +53737,7 @@
       <c r="AN78" s="13"/>
       <c r="AO78" s="28"/>
     </row>
-    <row r="79" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="79" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -53809,7 +53808,7 @@
       <c r="AN79" s="13"/>
       <c r="AO79" s="28"/>
     </row>
-    <row r="80" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="80" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -53880,7 +53879,7 @@
       <c r="AN80" s="13"/>
       <c r="AO80" s="28"/>
     </row>
-    <row r="81" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="81" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -53949,7 +53948,7 @@
       <c r="AN81" s="13"/>
       <c r="AO81" s="28"/>
     </row>
-    <row r="82" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="82" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -54020,7 +54019,7 @@
       <c r="AN82" s="13"/>
       <c r="AO82" s="28"/>
     </row>
-    <row r="83" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="83" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -54087,7 +54086,7 @@
       <c r="AN83" s="13"/>
       <c r="AO83" s="28"/>
     </row>
-    <row r="84" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="84" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -54132,7 +54131,7 @@
       <c r="AN84" s="13"/>
       <c r="AO84" s="28"/>
     </row>
-    <row r="85" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="85" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -54205,7 +54204,7 @@
       <c r="AN85" s="13"/>
       <c r="AO85" s="28"/>
     </row>
-    <row r="86" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="86" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -54274,7 +54273,7 @@
       <c r="AN86" s="13"/>
       <c r="AO86" s="28"/>
     </row>
-    <row r="87" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="87" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -54343,7 +54342,7 @@
       <c r="AN87" s="13"/>
       <c r="AO87" s="28"/>
     </row>
-    <row r="88" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="88" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -54416,7 +54415,7 @@
       <c r="AN88" s="13"/>
       <c r="AO88" s="28"/>
     </row>
-    <row r="89" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="89" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -54483,7 +54482,7 @@
       <c r="AN89" s="13"/>
       <c r="AO89" s="28"/>
     </row>
-    <row r="90" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="90" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -54550,7 +54549,7 @@
       <c r="AN90" s="13"/>
       <c r="AO90" s="28"/>
     </row>
-    <row r="91" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="91" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -54619,7 +54618,7 @@
       <c r="AN91" s="13"/>
       <c r="AO91" s="28"/>
     </row>
-    <row r="92" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="92" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -54686,7 +54685,7 @@
       <c r="AN92" s="13"/>
       <c r="AO92" s="28"/>
     </row>
-    <row r="93" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="93" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -54759,7 +54758,7 @@
       <c r="AN93" s="13"/>
       <c r="AO93" s="28"/>
     </row>
-    <row r="94" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="94" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -54826,7 +54825,7 @@
       <c r="AN94" s="13"/>
       <c r="AO94" s="28"/>
     </row>
-    <row r="95" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="95" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -54899,7 +54898,7 @@
       <c r="AN95" s="13"/>
       <c r="AO95" s="28"/>
     </row>
-    <row r="96" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="96" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -54970,7 +54969,7 @@
       <c r="AN96" s="13"/>
       <c r="AO96" s="28"/>
     </row>
-    <row r="97" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="97" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -55039,7 +55038,7 @@
       <c r="AN97" s="13"/>
       <c r="AO97" s="28"/>
     </row>
-    <row r="98" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="98" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -55110,7 +55109,7 @@
       <c r="AN98" s="13"/>
       <c r="AO98" s="28"/>
     </row>
-    <row r="99" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="99" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -55181,7 +55180,7 @@
       <c r="AN99" s="13"/>
       <c r="AO99" s="28"/>
     </row>
-    <row r="100" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="100" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -55248,7 +55247,7 @@
       <c r="AN100" s="13"/>
       <c r="AO100" s="28"/>
     </row>
-    <row r="101" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="101" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -55321,7 +55320,7 @@
       <c r="AN101" s="13"/>
       <c r="AO101" s="28"/>
     </row>
-    <row r="102" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="102" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -55392,7 +55391,7 @@
       <c r="AN102" s="13"/>
       <c r="AO102" s="28"/>
     </row>
-    <row r="103" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="103" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -55463,7 +55462,7 @@
       <c r="AN103" s="13"/>
       <c r="AO103" s="28"/>
     </row>
-    <row r="104" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="104" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -55534,7 +55533,7 @@
       <c r="AN104" s="13"/>
       <c r="AO104" s="28"/>
     </row>
-    <row r="105" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="105" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -55607,7 +55606,7 @@
       <c r="AN105" s="13"/>
       <c r="AO105" s="28"/>
     </row>
-    <row r="106" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="106" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -55635,7 +55634,7 @@
       <c r="AN106" s="13"/>
       <c r="AO106" s="28"/>
     </row>
-    <row r="107" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="107" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -55702,7 +55701,7 @@
       <c r="AN107" s="13"/>
       <c r="AO107" s="28"/>
     </row>
-    <row r="108" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="108" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -55769,7 +55768,7 @@
       <c r="AN108" s="13"/>
       <c r="AO108" s="28"/>
     </row>
-    <row r="109" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="109" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -55842,7 +55841,7 @@
       <c r="AN109" s="13"/>
       <c r="AO109" s="28"/>
     </row>
-    <row r="110" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="110" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -55913,7 +55912,7 @@
       <c r="AN110" s="13"/>
       <c r="AO110" s="28"/>
     </row>
-    <row r="111" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="111" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -55980,7 +55979,7 @@
       <c r="AN111" s="13"/>
       <c r="AO111" s="28"/>
     </row>
-    <row r="112" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="112" spans="1:41" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -56049,7 +56048,7 @@
       <c r="AN112" s="13"/>
       <c r="AO112" s="28"/>
     </row>
-    <row r="113" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="113" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -56118,7 +56117,7 @@
       <c r="AN113" s="13"/>
       <c r="AO113" s="28"/>
     </row>
-    <row r="114" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="114" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -56185,7 +56184,7 @@
       <c r="AN114" s="13"/>
       <c r="AO114" s="28"/>
     </row>
-    <row r="115" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="115" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="34"/>
       <c r="B115" s="34"/>
       <c r="C115" s="34"/>
@@ -56384,7 +56383,7 @@
       <c r="FP115" s="37"/>
       <c r="FQ115" s="37"/>
     </row>
-    <row r="116" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="116" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="34"/>
       <c r="B116" s="34"/>
       <c r="C116" s="34"/>
@@ -56589,7 +56588,7 @@
       <c r="FP116" s="37"/>
       <c r="FQ116" s="37"/>
     </row>
-    <row r="117" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="117" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="34"/>
       <c r="B117" s="34"/>
       <c r="C117" s="34"/>
@@ -56792,7 +56791,7 @@
       <c r="FP117" s="37"/>
       <c r="FQ117" s="37"/>
     </row>
-    <row r="118" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="118" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="38" t="s">
         <v>1665</v>
       </c>
@@ -57015,7 +57014,7 @@
       <c r="FP118" s="39"/>
       <c r="FQ118" s="39"/>
     </row>
-    <row r="119" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="119" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="38" t="s">
         <v>1671</v>
       </c>
@@ -57238,7 +57237,7 @@
       <c r="FP119" s="39"/>
       <c r="FQ119" s="39"/>
     </row>
-    <row r="120" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="120" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="38" t="s">
         <v>1675</v>
       </c>
@@ -57461,7 +57460,7 @@
       <c r="FP120" s="39"/>
       <c r="FQ120" s="39"/>
     </row>
-    <row r="121" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="121" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="38" t="s">
         <v>1680</v>
       </c>
@@ -57684,7 +57683,7 @@
       <c r="FP121" s="39"/>
       <c r="FQ121" s="39"/>
     </row>
-    <row r="122" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="122" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="38" t="s">
         <v>1671</v>
       </c>
@@ -57907,7 +57906,7 @@
       <c r="FP122" s="39"/>
       <c r="FQ122" s="39"/>
     </row>
-    <row r="123" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="123" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="32" t="s">
         <v>1685</v>
       </c>
@@ -58130,7 +58129,7 @@
       <c r="FP123" s="42"/>
       <c r="FQ123" s="42"/>
     </row>
-    <row r="124" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="124" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="32" t="s">
         <v>1690</v>
       </c>
@@ -58353,7 +58352,7 @@
       <c r="FP124" s="42"/>
       <c r="FQ124" s="42"/>
     </row>
-    <row r="125" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
+    <row r="125" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -58407,7 +58406,7 @@
       <c r="AM125" s="13"/>
       <c r="AN125" s="28"/>
     </row>
-    <row r="126" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="126" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -58461,7 +58460,7 @@
       <c r="AM126" s="13"/>
       <c r="AN126" s="28"/>
     </row>
-    <row r="127" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="127" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -58515,7 +58514,7 @@
       <c r="AM127" s="13"/>
       <c r="AN127" s="28"/>
     </row>
-    <row r="128" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="128" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -58569,7 +58568,7 @@
       <c r="AM128" s="13"/>
       <c r="AN128" s="28"/>
     </row>
-    <row r="129" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="129" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -58623,7 +58622,7 @@
       <c r="AM129" s="13"/>
       <c r="AN129" s="28"/>
     </row>
-    <row r="130" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="130" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -58677,7 +58676,7 @@
       <c r="AM130" s="13"/>
       <c r="AN130" s="28"/>
     </row>
-    <row r="131" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="131" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -58731,7 +58730,7 @@
       <c r="AM131" s="13"/>
       <c r="AN131" s="28"/>
     </row>
-    <row r="132" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="132" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -58785,7 +58784,7 @@
       <c r="AM132" s="13"/>
       <c r="AN132" s="28"/>
     </row>
-    <row r="133" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="133" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -58839,7 +58838,7 @@
       <c r="AM133" s="13"/>
       <c r="AN133" s="28"/>
     </row>
-    <row r="134" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="134" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -58893,7 +58892,7 @@
       <c r="AM134" s="13"/>
       <c r="AN134" s="28"/>
     </row>
-    <row r="135" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="135" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -58947,7 +58946,7 @@
       <c r="AM135" s="13"/>
       <c r="AN135" s="28"/>
     </row>
-    <row r="136" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="136" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -59001,7 +59000,7 @@
       <c r="AM136" s="13"/>
       <c r="AN136" s="28"/>
     </row>
-    <row r="137" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="137" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
@@ -59055,7 +59054,7 @@
       <c r="AM137" s="13"/>
       <c r="AN137" s="28"/>
     </row>
-    <row r="138" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="138" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
@@ -59109,7 +59108,7 @@
       <c r="AM138" s="13"/>
       <c r="AN138" s="28"/>
     </row>
-    <row r="139" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="139" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
@@ -59163,7 +59162,7 @@
       <c r="AM139" s="13"/>
       <c r="AN139" s="28"/>
     </row>
-    <row r="140" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="140" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -59217,7 +59216,7 @@
       <c r="AM140" s="13"/>
       <c r="AN140" s="28"/>
     </row>
-    <row r="141" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="141" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
@@ -59271,7 +59270,7 @@
       <c r="AM141" s="13"/>
       <c r="AN141" s="28"/>
     </row>
-    <row r="142" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="142" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
@@ -59325,7 +59324,7 @@
       <c r="AM142" s="13"/>
       <c r="AN142" s="28"/>
     </row>
-    <row r="143" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="143" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="4"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
@@ -59379,7 +59378,7 @@
       <c r="AM143" s="13"/>
       <c r="AN143" s="28"/>
     </row>
-    <row r="144" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="144" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
@@ -59433,7 +59432,7 @@
       <c r="AM144" s="13"/>
       <c r="AN144" s="28"/>
     </row>
-    <row r="145" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="145" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="4"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
@@ -59487,7 +59486,7 @@
       <c r="AM145" s="13"/>
       <c r="AN145" s="28"/>
     </row>
-    <row r="146" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="146" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="4"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
@@ -59541,7 +59540,7 @@
       <c r="AM146" s="13"/>
       <c r="AN146" s="28"/>
     </row>
-    <row r="147" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="147" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="4"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
@@ -59595,7 +59594,7 @@
       <c r="AM147" s="13"/>
       <c r="AN147" s="28"/>
     </row>
-    <row r="148" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="148" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="4"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
@@ -59649,7 +59648,7 @@
       <c r="AM148" s="13"/>
       <c r="AN148" s="28"/>
     </row>
-    <row r="149" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="149" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="4"/>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
@@ -59703,7 +59702,7 @@
       <c r="AM149" s="13"/>
       <c r="AN149" s="28"/>
     </row>
-    <row r="150" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="150" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="4"/>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
@@ -59757,7 +59756,7 @@
       <c r="AM150" s="13"/>
       <c r="AN150" s="28"/>
     </row>
-    <row r="151" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="151" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
@@ -59811,7 +59810,7 @@
       <c r="AM151" s="13"/>
       <c r="AN151" s="28"/>
     </row>
-    <row r="152" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="152" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
@@ -59865,7 +59864,7 @@
       <c r="AM152" s="13"/>
       <c r="AN152" s="28"/>
     </row>
-    <row r="153" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="153" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="4"/>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
@@ -59919,7 +59918,7 @@
       <c r="AM153" s="13"/>
       <c r="AN153" s="28"/>
     </row>
-    <row r="154" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="154" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="4"/>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
@@ -59973,7 +59972,7 @@
       <c r="AM154" s="13"/>
       <c r="AN154" s="28"/>
     </row>
-    <row r="155" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="155" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="4"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
@@ -60027,7 +60026,7 @@
       <c r="AM155" s="13"/>
       <c r="AN155" s="28"/>
     </row>
-    <row r="156" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="156" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="4"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
@@ -60081,7 +60080,7 @@
       <c r="AM156" s="13"/>
       <c r="AN156" s="28"/>
     </row>
-    <row r="157" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="157" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="4"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
@@ -60135,7 +60134,7 @@
       <c r="AM157" s="13"/>
       <c r="AN157" s="28"/>
     </row>
-    <row r="158" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="158" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
@@ -60189,7 +60188,7 @@
       <c r="AM158" s="13"/>
       <c r="AN158" s="28"/>
     </row>
-    <row r="159" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="159" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="4"/>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -60243,7 +60242,7 @@
       <c r="AM159" s="13"/>
       <c r="AN159" s="28"/>
     </row>
-    <row r="160" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="160" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="4"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
@@ -60297,7 +60296,7 @@
       <c r="AM160" s="13"/>
       <c r="AN160" s="28"/>
     </row>
-    <row r="161" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="161" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="4"/>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
@@ -60351,7 +60350,7 @@
       <c r="AM161" s="13"/>
       <c r="AN161" s="28"/>
     </row>
-    <row r="162" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="162" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="4"/>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
@@ -60405,7 +60404,7 @@
       <c r="AM162" s="13"/>
       <c r="AN162" s="28"/>
     </row>
-    <row r="163" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="163" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="4"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -60459,7 +60458,7 @@
       <c r="AM163" s="13"/>
       <c r="AN163" s="28"/>
     </row>
-    <row r="164" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="164" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="4"/>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
@@ -60513,7 +60512,7 @@
       <c r="AM164" s="13"/>
       <c r="AN164" s="28"/>
     </row>
-    <row r="165" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="165" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="4"/>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
@@ -60567,7 +60566,7 @@
       <c r="AM165" s="13"/>
       <c r="AN165" s="28"/>
     </row>
-    <row r="166" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="166" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="4"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
@@ -60621,7 +60620,7 @@
       <c r="AM166" s="13"/>
       <c r="AN166" s="28"/>
     </row>
-    <row r="167" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="167" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="4"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
@@ -60675,7 +60674,7 @@
       <c r="AM167" s="13"/>
       <c r="AN167" s="28"/>
     </row>
-    <row r="168" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="168" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4"/>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
@@ -60729,7 +60728,7 @@
       <c r="AM168" s="13"/>
       <c r="AN168" s="28"/>
     </row>
-    <row r="169" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="169" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="4"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
@@ -60783,7 +60782,7 @@
       <c r="AM169" s="13"/>
       <c r="AN169" s="28"/>
     </row>
-    <row r="170" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="170" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="4"/>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
@@ -60837,7 +60836,7 @@
       <c r="AM170" s="13"/>
       <c r="AN170" s="28"/>
     </row>
-    <row r="171" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="171" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="4"/>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
@@ -60891,7 +60890,7 @@
       <c r="AM171" s="13"/>
       <c r="AN171" s="28"/>
     </row>
-    <row r="172" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="172" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A172" s="4"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
@@ -60945,7 +60944,7 @@
       <c r="AM172" s="13"/>
       <c r="AN172" s="28"/>
     </row>
-    <row r="173" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="173" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="4"/>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
@@ -60999,7 +60998,7 @@
       <c r="AM173" s="13"/>
       <c r="AN173" s="28"/>
     </row>
-    <row r="174" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="174" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="4"/>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
@@ -61053,7 +61052,7 @@
       <c r="AM174" s="13"/>
       <c r="AN174" s="28"/>
     </row>
-    <row r="175" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="175" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="4"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
@@ -61107,7 +61106,7 @@
       <c r="AM175" s="13"/>
       <c r="AN175" s="28"/>
     </row>
-    <row r="176" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="176" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A176" s="4"/>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
@@ -61161,7 +61160,7 @@
       <c r="AM176" s="13"/>
       <c r="AN176" s="28"/>
     </row>
-    <row r="177" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="177" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="4"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
@@ -61215,7 +61214,7 @@
       <c r="AM177" s="13"/>
       <c r="AN177" s="28"/>
     </row>
-    <row r="178" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="178" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A178" s="4"/>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
@@ -61269,7 +61268,7 @@
       <c r="AM178" s="13"/>
       <c r="AN178" s="28"/>
     </row>
-    <row r="179" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="179" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A179" s="4"/>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
@@ -61323,7 +61322,7 @@
       <c r="AM179" s="13"/>
       <c r="AN179" s="28"/>
     </row>
-    <row r="180" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="180" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A180" s="4"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
@@ -61377,7 +61376,7 @@
       <c r="AM180" s="13"/>
       <c r="AN180" s="28"/>
     </row>
-    <row r="181" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="181" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="4"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
@@ -61431,7 +61430,7 @@
       <c r="AM181" s="13"/>
       <c r="AN181" s="28"/>
     </row>
-    <row r="182" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="182" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="4"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
@@ -61485,7 +61484,7 @@
       <c r="AM182" s="13"/>
       <c r="AN182" s="28"/>
     </row>
-    <row r="183" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="183" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="4"/>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
@@ -61539,7 +61538,7 @@
       <c r="AM183" s="13"/>
       <c r="AN183" s="28"/>
     </row>
-    <row r="184" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="184" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="4"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
@@ -61593,7 +61592,7 @@
       <c r="AM184" s="13"/>
       <c r="AN184" s="28"/>
     </row>
-    <row r="185" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="185" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A185" s="4"/>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
@@ -61647,7 +61646,7 @@
       <c r="AM185" s="13"/>
       <c r="AN185" s="28"/>
     </row>
-    <row r="186" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="186" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A186" s="4"/>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
@@ -61701,7 +61700,7 @@
       <c r="AM186" s="13"/>
       <c r="AN186" s="28"/>
     </row>
-    <row r="187" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="187" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A187" s="4"/>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
@@ -61755,7 +61754,7 @@
       <c r="AM187" s="13"/>
       <c r="AN187" s="28"/>
     </row>
-    <row r="188" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="188" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="4"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
@@ -61809,7 +61808,7 @@
       <c r="AM188" s="13"/>
       <c r="AN188" s="28"/>
     </row>
-    <row r="189" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="189" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189" s="4"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
@@ -61863,7 +61862,7 @@
       <c r="AM189" s="13"/>
       <c r="AN189" s="28"/>
     </row>
-    <row r="190" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="190" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A190" s="4"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
@@ -61917,7 +61916,7 @@
       <c r="AM190" s="13"/>
       <c r="AN190" s="28"/>
     </row>
-    <row r="191" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="191" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="4"/>
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
@@ -61971,7 +61970,7 @@
       <c r="AM191" s="13"/>
       <c r="AN191" s="28"/>
     </row>
-    <row r="192" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="192" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A192" s="4"/>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
@@ -62025,7 +62024,7 @@
       <c r="AM192" s="13"/>
       <c r="AN192" s="28"/>
     </row>
-    <row r="193" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="193" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A193" s="4"/>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
@@ -62079,7 +62078,7 @@
       <c r="AM193" s="13"/>
       <c r="AN193" s="28"/>
     </row>
-    <row r="194" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="194" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A194" s="4"/>
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
@@ -62133,7 +62132,7 @@
       <c r="AM194" s="13"/>
       <c r="AN194" s="28"/>
     </row>
-    <row r="195" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="195" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A195" s="4"/>
       <c r="B195" s="4"/>
       <c r="C195" s="4"/>
@@ -62187,7 +62186,7 @@
       <c r="AM195" s="13"/>
       <c r="AN195" s="28"/>
     </row>
-    <row r="196" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="196" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A196" s="4"/>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
@@ -62241,7 +62240,7 @@
       <c r="AM196" s="13"/>
       <c r="AN196" s="28"/>
     </row>
-    <row r="197" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="197" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A197" s="4"/>
       <c r="B197" s="4"/>
       <c r="C197" s="4"/>
@@ -62295,7 +62294,7 @@
       <c r="AM197" s="13"/>
       <c r="AN197" s="28"/>
     </row>
-    <row r="198" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="198" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A198" s="4"/>
       <c r="B198" s="4"/>
       <c r="C198" s="4"/>
@@ -62349,7 +62348,7 @@
       <c r="AM198" s="13"/>
       <c r="AN198" s="28"/>
     </row>
-    <row r="199" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="199" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A199" s="4"/>
       <c r="B199" s="4"/>
       <c r="C199" s="4"/>
@@ -62403,7 +62402,7 @@
       <c r="AM199" s="13"/>
       <c r="AN199" s="28"/>
     </row>
-    <row r="200" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="200" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A200" s="4"/>
       <c r="B200" s="4"/>
       <c r="C200" s="4"/>
@@ -62457,7 +62456,7 @@
       <c r="AM200" s="13"/>
       <c r="AN200" s="28"/>
     </row>
-    <row r="201" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="201" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A201" s="4"/>
       <c r="B201" s="4"/>
       <c r="C201" s="4"/>
@@ -62511,7 +62510,7 @@
       <c r="AM201" s="13"/>
       <c r="AN201" s="28"/>
     </row>
-    <row r="202" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="202" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A202" s="4"/>
       <c r="B202" s="4"/>
       <c r="C202" s="4"/>
@@ -62565,7 +62564,7 @@
       <c r="AM202" s="13"/>
       <c r="AN202" s="28"/>
     </row>
-    <row r="203" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="203" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203" s="4"/>
       <c r="B203" s="4"/>
       <c r="C203" s="4"/>
@@ -62619,7 +62618,7 @@
       <c r="AM203" s="13"/>
       <c r="AN203" s="28"/>
     </row>
-    <row r="204" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="204" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A204" s="4"/>
       <c r="B204" s="4"/>
       <c r="C204" s="4"/>
@@ -62673,7 +62672,7 @@
       <c r="AM204" s="13"/>
       <c r="AN204" s="28"/>
     </row>
-    <row r="205" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="205" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A205" s="4"/>
       <c r="B205" s="4"/>
       <c r="C205" s="4"/>
@@ -62727,7 +62726,7 @@
       <c r="AM205" s="13"/>
       <c r="AN205" s="28"/>
     </row>
-    <row r="206" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="206" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A206" s="4"/>
       <c r="B206" s="4"/>
       <c r="C206" s="4"/>
@@ -62781,7 +62780,7 @@
       <c r="AM206" s="13"/>
       <c r="AN206" s="28"/>
     </row>
-    <row r="207" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="207" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A207" s="4"/>
       <c r="B207" s="4"/>
       <c r="C207" s="4"/>
@@ -62835,7 +62834,7 @@
       <c r="AM207" s="13"/>
       <c r="AN207" s="28"/>
     </row>
-    <row r="208" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="208" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A208" s="4"/>
       <c r="B208" s="4"/>
       <c r="C208" s="4"/>
@@ -62889,7 +62888,7 @@
       <c r="AM208" s="13"/>
       <c r="AN208" s="28"/>
     </row>
-    <row r="209" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="209" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A209" s="4"/>
       <c r="B209" s="4"/>
       <c r="C209" s="4"/>
@@ -62943,7 +62942,7 @@
       <c r="AM209" s="13"/>
       <c r="AN209" s="28"/>
     </row>
-    <row r="210" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="210" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A210" s="4"/>
       <c r="B210" s="4"/>
       <c r="C210" s="4"/>
@@ -62997,7 +62996,7 @@
       <c r="AM210" s="13"/>
       <c r="AN210" s="28"/>
     </row>
-    <row r="211" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="211" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A211" s="4"/>
       <c r="B211" s="4"/>
       <c r="C211" s="4"/>
@@ -63051,7 +63050,7 @@
       <c r="AM211" s="13"/>
       <c r="AN211" s="28"/>
     </row>
-    <row r="212" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="212" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A212" s="4"/>
       <c r="B212" s="4"/>
       <c r="C212" s="4"/>
@@ -63105,7 +63104,7 @@
       <c r="AM212" s="13"/>
       <c r="AN212" s="28"/>
     </row>
-    <row r="213" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="213" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A213" s="4"/>
       <c r="B213" s="4"/>
       <c r="C213" s="4"/>
@@ -63159,7 +63158,7 @@
       <c r="AM213" s="13"/>
       <c r="AN213" s="28"/>
     </row>
-    <row r="214" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="214" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A214" s="4"/>
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
@@ -63213,7 +63212,7 @@
       <c r="AM214" s="13"/>
       <c r="AN214" s="28"/>
     </row>
-    <row r="215" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="215" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A215" s="4"/>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
@@ -63267,7 +63266,7 @@
       <c r="AM215" s="13"/>
       <c r="AN215" s="28"/>
     </row>
-    <row r="216" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="216" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A216" s="4"/>
       <c r="B216" s="4"/>
       <c r="C216" s="4"/>
@@ -63321,7 +63320,7 @@
       <c r="AM216" s="13"/>
       <c r="AN216" s="28"/>
     </row>
-    <row r="217" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="217" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A217" s="4"/>
       <c r="B217" s="4"/>
       <c r="C217" s="4"/>
@@ -63375,7 +63374,7 @@
       <c r="AM217" s="13"/>
       <c r="AN217" s="28"/>
     </row>
-    <row r="218" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="218" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A218" s="4"/>
       <c r="B218" s="4"/>
       <c r="C218" s="4"/>
@@ -63429,7 +63428,7 @@
       <c r="AM218" s="13"/>
       <c r="AN218" s="28"/>
     </row>
-    <row r="219" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="219" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A219" s="4"/>
       <c r="B219" s="4"/>
       <c r="C219" s="4"/>
@@ -63483,7 +63482,7 @@
       <c r="AM219" s="13"/>
       <c r="AN219" s="28"/>
     </row>
-    <row r="220" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="220" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A220" s="4"/>
       <c r="B220" s="4"/>
       <c r="C220" s="4"/>
@@ -63537,7 +63536,7 @@
       <c r="AM220" s="13"/>
       <c r="AN220" s="28"/>
     </row>
-    <row r="221" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="221" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A221" s="4"/>
       <c r="B221" s="4"/>
       <c r="C221" s="4"/>
@@ -63591,7 +63590,7 @@
       <c r="AM221" s="13"/>
       <c r="AN221" s="28"/>
     </row>
-    <row r="222" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="222" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A222" s="4"/>
       <c r="B222" s="4"/>
       <c r="C222" s="4"/>
@@ -63645,7 +63644,7 @@
       <c r="AM222" s="13"/>
       <c r="AN222" s="28"/>
     </row>
-    <row r="223" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="223" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A223" s="4"/>
       <c r="B223" s="4"/>
       <c r="C223" s="4"/>
@@ -63699,7 +63698,7 @@
       <c r="AM223" s="13"/>
       <c r="AN223" s="28"/>
     </row>
-    <row r="224" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="224" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A224" s="4"/>
       <c r="B224" s="4"/>
       <c r="C224" s="4"/>
@@ -63753,7 +63752,7 @@
       <c r="AM224" s="13"/>
       <c r="AN224" s="28"/>
     </row>
-    <row r="225" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="225" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A225" s="4"/>
       <c r="B225" s="4"/>
       <c r="C225" s="4"/>
@@ -63807,7 +63806,7 @@
       <c r="AM225" s="13"/>
       <c r="AN225" s="28"/>
     </row>
-    <row r="226" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="226" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A226" s="4"/>
       <c r="B226" s="4"/>
       <c r="C226" s="4"/>
@@ -63861,7 +63860,7 @@
       <c r="AM226" s="13"/>
       <c r="AN226" s="28"/>
     </row>
-    <row r="227" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="227" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A227" s="4"/>
       <c r="B227" s="4"/>
       <c r="C227" s="4"/>
@@ -63915,7 +63914,7 @@
       <c r="AM227" s="13"/>
       <c r="AN227" s="28"/>
     </row>
-    <row r="228" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="228" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A228" s="4"/>
       <c r="B228" s="4"/>
       <c r="C228" s="4"/>
@@ -63969,7 +63968,7 @@
       <c r="AM228" s="13"/>
       <c r="AN228" s="28"/>
     </row>
-    <row r="229" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="229" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A229" s="4"/>
       <c r="B229" s="4"/>
       <c r="C229" s="4"/>
@@ -64023,7 +64022,7 @@
       <c r="AM229" s="13"/>
       <c r="AN229" s="28"/>
     </row>
-    <row r="230" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="230" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A230" s="4"/>
       <c r="B230" s="4"/>
       <c r="C230" s="4"/>
@@ -64077,7 +64076,7 @@
       <c r="AM230" s="13"/>
       <c r="AN230" s="28"/>
     </row>
-    <row r="231" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="231" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A231" s="4"/>
       <c r="B231" s="4"/>
       <c r="C231" s="4"/>
@@ -64131,7 +64130,7 @@
       <c r="AM231" s="13"/>
       <c r="AN231" s="28"/>
     </row>
-    <row r="232" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="232" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A232" s="4"/>
       <c r="B232" s="4"/>
       <c r="C232" s="4"/>
@@ -64185,7 +64184,7 @@
       <c r="AM232" s="13"/>
       <c r="AN232" s="28"/>
     </row>
-    <row r="233" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="233" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A233" s="4"/>
       <c r="B233" s="4"/>
       <c r="C233" s="4"/>
@@ -64239,7 +64238,7 @@
       <c r="AM233" s="13"/>
       <c r="AN233" s="28"/>
     </row>
-    <row r="234" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="234" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A234" s="4"/>
       <c r="B234" s="4"/>
       <c r="C234" s="4"/>
@@ -64293,7 +64292,7 @@
       <c r="AM234" s="13"/>
       <c r="AN234" s="28"/>
     </row>
-    <row r="235" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="235" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A235" s="4"/>
       <c r="B235" s="4"/>
       <c r="C235" s="4"/>
@@ -64347,7 +64346,7 @@
       <c r="AM235" s="13"/>
       <c r="AN235" s="28"/>
     </row>
-    <row r="236" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="236" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A236" s="4"/>
       <c r="B236" s="4"/>
       <c r="C236" s="4"/>
@@ -64401,7 +64400,7 @@
       <c r="AM236" s="13"/>
       <c r="AN236" s="28"/>
     </row>
-    <row r="237" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="237" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A237" s="4"/>
       <c r="B237" s="4"/>
       <c r="C237" s="4"/>
@@ -64455,7 +64454,7 @@
       <c r="AM237" s="13"/>
       <c r="AN237" s="28"/>
     </row>
-    <row r="238" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="238" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A238" s="4"/>
       <c r="B238" s="4"/>
       <c r="C238" s="4"/>
@@ -64509,7 +64508,7 @@
       <c r="AM238" s="13"/>
       <c r="AN238" s="28"/>
     </row>
-    <row r="239" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="239" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A239" s="4"/>
       <c r="B239" s="4"/>
       <c r="C239" s="4"/>
@@ -64563,7 +64562,7 @@
       <c r="AM239" s="13"/>
       <c r="AN239" s="28"/>
     </row>
-    <row r="240" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="240" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A240" s="4"/>
       <c r="B240" s="4"/>
       <c r="C240" s="4"/>
@@ -64617,7 +64616,7 @@
       <c r="AM240" s="13"/>
       <c r="AN240" s="28"/>
     </row>
-    <row r="241" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="241" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A241" s="4"/>
       <c r="B241" s="4"/>
       <c r="C241" s="4"/>
@@ -64671,7 +64670,7 @@
       <c r="AM241" s="13"/>
       <c r="AN241" s="28"/>
     </row>
-    <row r="242" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="242" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A242" s="4"/>
       <c r="B242" s="4"/>
       <c r="C242" s="4"/>
@@ -64725,7 +64724,7 @@
       <c r="AM242" s="13"/>
       <c r="AN242" s="28"/>
     </row>
-    <row r="243" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="243" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A243" s="4"/>
       <c r="B243" s="4"/>
       <c r="C243" s="4"/>
@@ -64779,7 +64778,7 @@
       <c r="AM243" s="13"/>
       <c r="AN243" s="28"/>
     </row>
-    <row r="244" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="244" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A244" s="4"/>
       <c r="B244" s="4"/>
       <c r="C244" s="4"/>
@@ -64833,7 +64832,7 @@
       <c r="AM244" s="13"/>
       <c r="AN244" s="28"/>
     </row>
-    <row r="245" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="245" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A245" s="4"/>
       <c r="B245" s="4"/>
       <c r="C245" s="4"/>
@@ -64887,7 +64886,7 @@
       <c r="AM245" s="13"/>
       <c r="AN245" s="28"/>
     </row>
-    <row r="246" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="246" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A246" s="4"/>
       <c r="B246" s="4"/>
       <c r="C246" s="4"/>
@@ -64941,7 +64940,7 @@
       <c r="AM246" s="13"/>
       <c r="AN246" s="28"/>
     </row>
-    <row r="247" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="247" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A247" s="4"/>
       <c r="B247" s="4"/>
       <c r="C247" s="4"/>
@@ -64995,7 +64994,7 @@
       <c r="AM247" s="13"/>
       <c r="AN247" s="28"/>
     </row>
-    <row r="248" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="248" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A248" s="4"/>
       <c r="B248" s="4"/>
       <c r="C248" s="4"/>
@@ -65049,7 +65048,7 @@
       <c r="AM248" s="13"/>
       <c r="AN248" s="28"/>
     </row>
-    <row r="249" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="249" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A249" s="4"/>
       <c r="B249" s="4"/>
       <c r="C249" s="4"/>
@@ -65103,7 +65102,7 @@
       <c r="AM249" s="13"/>
       <c r="AN249" s="28"/>
     </row>
-    <row r="250" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="250" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A250" s="4"/>
       <c r="B250" s="4"/>
       <c r="C250" s="4"/>
@@ -65157,7 +65156,7 @@
       <c r="AM250" s="13"/>
       <c r="AN250" s="28"/>
     </row>
-    <row r="251" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="251" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A251" s="4"/>
       <c r="B251" s="4"/>
       <c r="C251" s="4"/>
@@ -65211,7 +65210,7 @@
       <c r="AM251" s="13"/>
       <c r="AN251" s="28"/>
     </row>
-    <row r="252" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="252" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A252" s="4"/>
       <c r="B252" s="4"/>
       <c r="C252" s="4"/>
@@ -65265,7 +65264,7 @@
       <c r="AM252" s="13"/>
       <c r="AN252" s="28"/>
     </row>
-    <row r="253" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="253" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A253" s="4"/>
       <c r="B253" s="4"/>
       <c r="C253" s="4"/>
@@ -65319,7 +65318,7 @@
       <c r="AM253" s="13"/>
       <c r="AN253" s="28"/>
     </row>
-    <row r="254" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="254" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A254" s="4"/>
       <c r="B254" s="4"/>
       <c r="C254" s="4"/>
@@ -65373,7 +65372,7 @@
       <c r="AM254" s="13"/>
       <c r="AN254" s="28"/>
     </row>
-    <row r="255" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="255" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A255" s="4"/>
       <c r="B255" s="4"/>
       <c r="C255" s="4"/>
@@ -65427,7 +65426,7 @@
       <c r="AM255" s="13"/>
       <c r="AN255" s="28"/>
     </row>
-    <row r="256" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="256" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A256" s="4"/>
       <c r="B256" s="4"/>
       <c r="C256" s="4"/>
@@ -65481,7 +65480,7 @@
       <c r="AM256" s="13"/>
       <c r="AN256" s="28"/>
     </row>
-    <row r="257" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="257" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A257" s="4"/>
       <c r="B257" s="4"/>
       <c r="C257" s="4"/>
@@ -65535,7 +65534,7 @@
       <c r="AM257" s="13"/>
       <c r="AN257" s="28"/>
     </row>
-    <row r="258" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="258" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A258" s="4"/>
       <c r="B258" s="4"/>
       <c r="C258" s="4"/>
@@ -65589,7 +65588,7 @@
       <c r="AM258" s="13"/>
       <c r="AN258" s="28"/>
     </row>
-    <row r="259" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="259" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A259" s="4"/>
       <c r="B259" s="4"/>
       <c r="C259" s="4"/>
@@ -65643,7 +65642,7 @@
       <c r="AM259" s="13"/>
       <c r="AN259" s="28"/>
     </row>
-    <row r="260" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="260" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A260" s="4"/>
       <c r="B260" s="4"/>
       <c r="C260" s="4"/>
@@ -65697,7 +65696,7 @@
       <c r="AM260" s="13"/>
       <c r="AN260" s="28"/>
     </row>
-    <row r="261" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="261" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A261" s="4"/>
       <c r="B261" s="4"/>
       <c r="C261" s="4"/>
@@ -65751,7 +65750,7 @@
       <c r="AM261" s="13"/>
       <c r="AN261" s="28"/>
     </row>
-    <row r="262" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="262" spans="1:40" s="10" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A262" s="4"/>
       <c r="B262" s="4"/>
       <c r="C262" s="4"/>
@@ -65805,7 +65804,7 @@
       <c r="AM262" s="13"/>
       <c r="AN262" s="28"/>
     </row>
-    <row r="263" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="263" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A263" s="6"/>
       <c r="B263" s="6"/>
       <c r="C263" s="6"/>
@@ -65859,7 +65858,7 @@
       <c r="AM263" s="13"/>
       <c r="AN263" s="28"/>
     </row>
-    <row r="264" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="264" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A264" s="6"/>
       <c r="B264" s="6"/>
       <c r="C264" s="6"/>
@@ -65913,7 +65912,7 @@
       <c r="AM264" s="13"/>
       <c r="AN264" s="28"/>
     </row>
-    <row r="265" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="265" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A265" s="6"/>
       <c r="B265" s="6"/>
       <c r="C265" s="6"/>
@@ -65967,7 +65966,7 @@
       <c r="AM265" s="13"/>
       <c r="AN265" s="28"/>
     </row>
-    <row r="266" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="266" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A266" s="6"/>
       <c r="B266" s="6"/>
       <c r="C266" s="6"/>
@@ -66021,7 +66020,7 @@
       <c r="AM266" s="13"/>
       <c r="AN266" s="28"/>
     </row>
-    <row r="267" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="267" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A267" s="6"/>
       <c r="B267" s="6"/>
       <c r="C267" s="6"/>
@@ -66075,7 +66074,7 @@
       <c r="AM267" s="13"/>
       <c r="AN267" s="28"/>
     </row>
-    <row r="268" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="268" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A268" s="6"/>
       <c r="B268" s="6"/>
       <c r="C268" s="6"/>
@@ -66116,7 +66115,7 @@
       <c r="AM268" s="13"/>
       <c r="AN268" s="28"/>
     </row>
-    <row r="269" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="269" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A269" s="6"/>
       <c r="B269" s="6"/>
       <c r="C269" s="6"/>
@@ -66157,7 +66156,7 @@
       <c r="AM269" s="13"/>
       <c r="AN269" s="28"/>
     </row>
-    <row r="270" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="270" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A270" s="6"/>
       <c r="B270" s="6"/>
       <c r="C270" s="6"/>
@@ -66198,7 +66197,7 @@
       <c r="AM270" s="13"/>
       <c r="AN270" s="28"/>
     </row>
-    <row r="271" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="271" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A271" s="6"/>
       <c r="B271" s="6"/>
       <c r="C271" s="6"/>
@@ -66239,7 +66238,7 @@
       <c r="AM271" s="13"/>
       <c r="AN271" s="28"/>
     </row>
-    <row r="272" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="272" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A272" s="6"/>
       <c r="B272" s="6"/>
       <c r="C272" s="6"/>
@@ -66280,7 +66279,7 @@
       <c r="AM272" s="13"/>
       <c r="AN272" s="28"/>
     </row>
-    <row r="273" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="273" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A273" s="6"/>
       <c r="B273" s="6"/>
       <c r="C273" s="6"/>
@@ -66321,7 +66320,7 @@
       <c r="AM273" s="13"/>
       <c r="AN273" s="28"/>
     </row>
-    <row r="274" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="274" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A274" s="6"/>
       <c r="B274" s="6"/>
       <c r="C274" s="6"/>
@@ -66362,7 +66361,7 @@
       <c r="AM274" s="13"/>
       <c r="AN274" s="28"/>
     </row>
-    <row r="275" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="275" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A275" s="6"/>
       <c r="B275" s="6"/>
       <c r="C275" s="6"/>
@@ -66403,7 +66402,7 @@
       <c r="AM275" s="13"/>
       <c r="AN275" s="28"/>
     </row>
-    <row r="276" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="276" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A276" s="6"/>
       <c r="B276" s="6"/>
       <c r="C276" s="6"/>
@@ -66444,7 +66443,7 @@
       <c r="AM276" s="13"/>
       <c r="AN276" s="28"/>
     </row>
-    <row r="277" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="277" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A277" s="6"/>
       <c r="B277" s="6"/>
       <c r="C277" s="6"/>
@@ -66485,7 +66484,7 @@
       <c r="AM277" s="13"/>
       <c r="AN277" s="28"/>
     </row>
-    <row r="278" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="278" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A278" s="6"/>
       <c r="B278" s="6"/>
       <c r="C278" s="6"/>
@@ -66526,7 +66525,7 @@
       <c r="AM278" s="13"/>
       <c r="AN278" s="28"/>
     </row>
-    <row r="279" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="279" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A279" s="6"/>
       <c r="B279" s="6"/>
       <c r="C279" s="6"/>
@@ -66567,7 +66566,7 @@
       <c r="AM279" s="13"/>
       <c r="AN279" s="28"/>
     </row>
-    <row r="280" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="280" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A280" s="6"/>
       <c r="B280" s="6"/>
       <c r="C280" s="6"/>
@@ -66608,7 +66607,7 @@
       <c r="AM280" s="13"/>
       <c r="AN280" s="28"/>
     </row>
-    <row r="281" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="281" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A281" s="6"/>
       <c r="B281" s="6"/>
       <c r="C281" s="6"/>
@@ -66649,7 +66648,7 @@
       <c r="AM281" s="13"/>
       <c r="AN281" s="28"/>
     </row>
-    <row r="282" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="282" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A282" s="6"/>
       <c r="B282" s="6"/>
       <c r="C282" s="6"/>
@@ -66690,7 +66689,7 @@
       <c r="AM282" s="13"/>
       <c r="AN282" s="28"/>
     </row>
-    <row r="283" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="283" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A283" s="6"/>
       <c r="B283" s="6"/>
       <c r="C283" s="6"/>
@@ -66731,7 +66730,7 @@
       <c r="AM283" s="13"/>
       <c r="AN283" s="28"/>
     </row>
-    <row r="284" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="284" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A284" s="6"/>
       <c r="B284" s="6"/>
       <c r="C284" s="6"/>
@@ -66772,7 +66771,7 @@
       <c r="AM284" s="13"/>
       <c r="AN284" s="28"/>
     </row>
-    <row r="285" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="285" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A285" s="6"/>
       <c r="B285" s="6"/>
       <c r="C285" s="6"/>
@@ -66813,7 +66812,7 @@
       <c r="AM285" s="13"/>
       <c r="AN285" s="28"/>
     </row>
-    <row r="286" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="286" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A286" s="6"/>
       <c r="B286" s="6"/>
       <c r="C286" s="6"/>
@@ -66854,7 +66853,7 @@
       <c r="AM286" s="13"/>
       <c r="AN286" s="28"/>
     </row>
-    <row r="287" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="287" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A287" s="6"/>
       <c r="B287" s="6"/>
       <c r="C287" s="6"/>
@@ -66895,7 +66894,7 @@
       <c r="AM287" s="13"/>
       <c r="AN287" s="28"/>
     </row>
-    <row r="288" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="288" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A288" s="6"/>
       <c r="B288" s="6"/>
       <c r="C288" s="6"/>
@@ -66936,7 +66935,7 @@
       <c r="AM288" s="13"/>
       <c r="AN288" s="28"/>
     </row>
-    <row r="289" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="289" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A289" s="6"/>
       <c r="B289" s="6"/>
       <c r="C289" s="6"/>
@@ -66977,7 +66976,7 @@
       <c r="AM289" s="13"/>
       <c r="AN289" s="28"/>
     </row>
-    <row r="290" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="290" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A290" s="6"/>
       <c r="B290" s="6"/>
       <c r="C290" s="6"/>
@@ -67018,7 +67017,7 @@
       <c r="AM290" s="13"/>
       <c r="AN290" s="28"/>
     </row>
-    <row r="291" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="291" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A291" s="6"/>
       <c r="B291" s="6"/>
       <c r="C291" s="6"/>
@@ -67059,7 +67058,7 @@
       <c r="AM291" s="13"/>
       <c r="AN291" s="28"/>
     </row>
-    <row r="292" spans="1:40" ht="23.25" customHeight="1" thickBot="1">
+    <row r="292" spans="1:40" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A292" s="6"/>
       <c r="B292" s="6"/>
       <c r="C292" s="6"/>
@@ -67100,16 +67099,16 @@
       <c r="AM292" s="13"/>
       <c r="AN292" s="28"/>
     </row>
-    <row r="293" spans="1:40" ht="18.75">
+    <row r="293" spans="1:40" ht="18.75" x14ac:dyDescent="0.25">
       <c r="Q293" s="6"/>
     </row>
-    <row r="294" spans="1:40" ht="18.75">
+    <row r="294" spans="1:40" ht="18.75" x14ac:dyDescent="0.25">
       <c r="Q294" s="6"/>
     </row>
-    <row r="295" spans="1:40" ht="18.75">
+    <row r="295" spans="1:40" ht="18.75" x14ac:dyDescent="0.25">
       <c r="Q295" s="6"/>
     </row>
-    <row r="296" spans="1:40" ht="18.75">
+    <row r="296" spans="1:40" ht="18.75" x14ac:dyDescent="0.25">
       <c r="Q296" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
two new records added
imgvr_uvig_id and host_imgm_genome_id added
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29203"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VirJenDB\virjendb_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CEC721A-0A39-44A4-9A4E-FF0682C54A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F428A2D2-3E89-40F5-8D1F-698D49466DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D7962945-3ACF-49DB-B8FB-E785F5F91D27}"/>
   </bookViews>
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5417" uniqueCount="1714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5433" uniqueCount="1720">
   <si>
     <t>VJDBv0.3</t>
   </si>
@@ -4799,6 +4799,24 @@
   </si>
   <si>
     <t>0hx</t>
+  </si>
+  <si>
+    <t>imgvr_uvig_id</t>
+  </si>
+  <si>
+    <t>IMGVR UVIG ID</t>
+  </si>
+  <si>
+    <t>0id</t>
+  </si>
+  <si>
+    <t>host_imgm_genome_id</t>
+  </si>
+  <si>
+    <t>Host  IMGM Genome ID</t>
+  </si>
+  <si>
+    <t>0ie</t>
   </si>
   <si>
     <t>do not add</t>
@@ -6313,11 +6331,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E033465-2455-477E-A700-6BF7A0771C26}">
-  <dimension ref="A1:FY216"/>
+  <dimension ref="A1:FY218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AX204" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AZ211" sqref="AZ211"/>
+      <pane xSplit="1" topLeftCell="B209" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="23.25" customHeight="1"/>
@@ -52602,6 +52620,84 @@
       </c>
       <c r="AZ216" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="217" spans="1:53" ht="23.25" customHeight="1">
+      <c r="A217" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B217" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D217" t="s">
+        <v>60</v>
+      </c>
+      <c r="E217" s="56" t="s">
+        <v>938</v>
+      </c>
+      <c r="S217" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="T217" t="s">
+        <v>183</v>
+      </c>
+      <c r="V217" s="63" t="str">
+        <f>"[" &amp; _xlfn.TEXTJOIN(", ", TRUE,
+    IF(H217&lt;&gt;"", """" &amp; H$1 &amp; """", ""),
+    IF(I217&lt;&gt;"", """" &amp; I$1 &amp; """", ""),
+    IF(J217&lt;&gt;"", """" &amp; J$1 &amp; """", ""),
+    IF(K217&lt;&gt;"", """" &amp; K$1 &amp; """", ""),
+    IF(L217&lt;&gt;"", """" &amp; L$1 &amp; """", ""),    IF(M217&lt;&gt;"", """" &amp; M$1 &amp; """", ""),    IF(N217&lt;&gt;"", """" &amp; N$1 &amp; """", ""),     IF(O217&lt;&gt;"", """" &amp; O$1 &amp; """", ""),     IF(P217&lt;&gt;"", """" &amp; P$1 &amp; """", ""),
+    IF(S217&lt;&gt;"", """" &amp; S217 &amp; """", ""), IF(Q217&lt;&gt;"", """" &amp; Q217 &amp; """", ""), IF(R217&lt;&gt;"", """" &amp; R217 &amp; """", ""),
+    IF(T217&lt;&gt;"", """" &amp; T217 &amp; """", ""),
+    IF(U217&lt;&gt;"", """" &amp; U217 &amp; """", "")
+) &amp; "]"</f>
+        <v>["Host", "Identifiers"]</v>
+      </c>
+      <c r="W217" t="s">
+        <v>789</v>
+      </c>
+      <c r="AW217" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="218" spans="1:53" ht="23.25" customHeight="1">
+      <c r="A218" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B218" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D218" t="s">
+        <v>60</v>
+      </c>
+      <c r="E218" s="56" t="s">
+        <v>938</v>
+      </c>
+      <c r="S218" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="T218" t="s">
+        <v>183</v>
+      </c>
+      <c r="V218" s="63" t="str">
+        <f>"[" &amp; _xlfn.TEXTJOIN(", ", TRUE,
+    IF(H218&lt;&gt;"", """" &amp; H$1 &amp; """", ""),
+    IF(I218&lt;&gt;"", """" &amp; I$1 &amp; """", ""),
+    IF(J218&lt;&gt;"", """" &amp; J$1 &amp; """", ""),
+    IF(K218&lt;&gt;"", """" &amp; K$1 &amp; """", ""),
+    IF(L218&lt;&gt;"", """" &amp; L$1 &amp; """", ""),    IF(M218&lt;&gt;"", """" &amp; M$1 &amp; """", ""),    IF(N218&lt;&gt;"", """" &amp; N$1 &amp; """", ""),     IF(O218&lt;&gt;"", """" &amp; O$1 &amp; """", ""),     IF(P218&lt;&gt;"", """" &amp; P$1 &amp; """", ""),
+    IF(S218&lt;&gt;"", """" &amp; S218 &amp; """", ""), IF(Q218&lt;&gt;"", """" &amp; Q218 &amp; """", ""), IF(R218&lt;&gt;"", """" &amp; R218 &amp; """", ""),
+    IF(T218&lt;&gt;"", """" &amp; T218 &amp; """", ""),
+    IF(U218&lt;&gt;"", """" &amp; U218 &amp; """", "")
+) &amp; "]"</f>
+        <v>["Host", "Identifiers"]</v>
+      </c>
+      <c r="W218" t="s">
+        <v>789</v>
+      </c>
+      <c r="AW218" t="s">
+        <v>1526</v>
       </c>
     </row>
   </sheetData>
@@ -53803,7 +53899,7 @@
         <v>315</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
@@ -53813,14 +53909,14 @@
       <c r="AC5" s="8"/>
       <c r="AD5" s="8"/>
       <c r="AE5" s="2" t="s">
-        <v>1522</v>
+        <v>1528</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>1523</v>
+        <v>1529</v>
       </c>
       <c r="AG5" s="8"/>
       <c r="AH5" s="9" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI5" s="8"/>
       <c r="AJ5" s="8"/>
@@ -53847,7 +53943,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>1524</v>
+        <v>1530</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -53872,7 +53968,7 @@
         <v>315</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
@@ -53884,14 +53980,14 @@
       </c>
       <c r="AD6" s="13"/>
       <c r="AE6" s="1" t="s">
-        <v>1525</v>
+        <v>1531</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG6" s="13"/>
       <c r="AH6" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI6" s="13"/>
       <c r="AJ6" s="13"/>
@@ -53941,7 +54037,7 @@
         <v>315</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
@@ -53953,14 +54049,14 @@
         <v>985</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>1526</v>
+        <v>1532</v>
       </c>
       <c r="AF7" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG7" s="13"/>
       <c r="AH7" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI7" s="13"/>
       <c r="AJ7" s="13"/>
@@ -54010,7 +54106,7 @@
         <v>315</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X8" s="13"/>
       <c r="Y8" s="13"/>
@@ -54020,14 +54116,14 @@
       <c r="AC8" s="13"/>
       <c r="AD8" s="13"/>
       <c r="AE8" s="1" t="s">
-        <v>1527</v>
+        <v>1533</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG8" s="13"/>
       <c r="AH8" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI8" s="13"/>
       <c r="AJ8" s="13"/>
@@ -54077,7 +54173,7 @@
         <v>315</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
@@ -54087,14 +54183,14 @@
       <c r="AC9" s="13"/>
       <c r="AD9" s="13"/>
       <c r="AE9" s="1" t="s">
-        <v>1528</v>
+        <v>1534</v>
       </c>
       <c r="AF9" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG9" s="13"/>
       <c r="AH9" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI9" s="13"/>
       <c r="AJ9" s="13"/>
@@ -54121,7 +54217,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>1529</v>
+        <v>1535</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -54146,7 +54242,7 @@
         <v>315</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
@@ -54158,14 +54254,14 @@
       </c>
       <c r="AD10" s="13"/>
       <c r="AE10" s="1" t="s">
-        <v>1530</v>
+        <v>1536</v>
       </c>
       <c r="AF10" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG10" s="13"/>
       <c r="AH10" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI10" s="13"/>
       <c r="AJ10" s="13"/>
@@ -54192,7 +54288,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>1531</v>
+        <v>1537</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -54217,7 +54313,7 @@
         <v>315</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -54229,14 +54325,14 @@
       </c>
       <c r="AD11" s="13"/>
       <c r="AE11" s="1" t="s">
-        <v>1532</v>
+        <v>1538</v>
       </c>
       <c r="AF11" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG11" s="13"/>
       <c r="AH11" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI11" s="13"/>
       <c r="AJ11" s="13"/>
@@ -54286,7 +54382,7 @@
         <v>315</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
@@ -54296,14 +54392,14 @@
       <c r="AC12" s="13"/>
       <c r="AD12" s="13"/>
       <c r="AE12" s="1" t="s">
-        <v>1533</v>
+        <v>1539</v>
       </c>
       <c r="AF12" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG12" s="13"/>
       <c r="AH12" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI12" s="13"/>
       <c r="AJ12" s="13"/>
@@ -54353,7 +54449,7 @@
         <v>315</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -54363,14 +54459,14 @@
       <c r="AC13" s="13"/>
       <c r="AD13" s="13"/>
       <c r="AE13" s="1" t="s">
-        <v>1534</v>
+        <v>1540</v>
       </c>
       <c r="AF13" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG13" s="13"/>
       <c r="AH13" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI13" s="13"/>
       <c r="AJ13" s="13"/>
@@ -54397,7 +54493,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>1535</v>
+        <v>1541</v>
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -54422,7 +54518,7 @@
         <v>315</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
@@ -54430,20 +54526,20 @@
       <c r="AA14" s="13"/>
       <c r="AB14" s="13"/>
       <c r="AC14" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE14" s="1" t="s">
-        <v>1537</v>
+        <v>1543</v>
       </c>
       <c r="AF14" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG14" s="13"/>
       <c r="AH14" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI14" s="13"/>
       <c r="AJ14" s="13"/>
@@ -54493,7 +54589,7 @@
         <v>315</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -54502,17 +54598,17 @@
       <c r="AB15" s="13"/>
       <c r="AC15" s="13"/>
       <c r="AD15" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>1538</v>
+        <v>1544</v>
       </c>
       <c r="AF15" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG15" s="13"/>
       <c r="AH15" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI15" s="13"/>
       <c r="AJ15" s="13"/>
@@ -54562,7 +54658,7 @@
         <v>315</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -54572,14 +54668,14 @@
       <c r="AC16" s="13"/>
       <c r="AD16" s="13"/>
       <c r="AE16" s="1" t="s">
-        <v>1539</v>
+        <v>1545</v>
       </c>
       <c r="AF16" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG16" s="13"/>
       <c r="AH16" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI16" s="13"/>
       <c r="AJ16" s="13"/>
@@ -54606,7 +54702,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4" t="s">
-        <v>1540</v>
+        <v>1546</v>
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -54631,7 +54727,7 @@
         <v>315</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -54639,20 +54735,20 @@
       <c r="AA17" s="13"/>
       <c r="AB17" s="13"/>
       <c r="AC17" s="1" t="s">
-        <v>1541</v>
+        <v>1547</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>1542</v>
+        <v>1548</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>1543</v>
+        <v>1549</v>
       </c>
       <c r="AF17" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG17" s="13"/>
       <c r="AH17" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI17" s="13"/>
       <c r="AJ17" s="13"/>
@@ -54679,7 +54775,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4" t="s">
-        <v>1544</v>
+        <v>1550</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
@@ -54704,7 +54800,7 @@
         <v>315</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X18" s="13"/>
       <c r="Y18" s="13"/>
@@ -54712,20 +54808,20 @@
       <c r="AA18" s="13"/>
       <c r="AB18" s="13"/>
       <c r="AC18" s="1" t="s">
-        <v>1541</v>
+        <v>1547</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>1542</v>
+        <v>1548</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>1545</v>
+        <v>1551</v>
       </c>
       <c r="AF18" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG18" s="13"/>
       <c r="AH18" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI18" s="13"/>
       <c r="AJ18" s="13"/>
@@ -54752,7 +54848,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>1546</v>
+        <v>1552</v>
       </c>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
@@ -54777,7 +54873,7 @@
         <v>315</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -54791,14 +54887,14 @@
         <v>1059</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>1547</v>
+        <v>1553</v>
       </c>
       <c r="AF19" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG19" s="13"/>
       <c r="AH19" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI19" s="13"/>
       <c r="AJ19" s="13"/>
@@ -54825,7 +54921,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>1548</v>
+        <v>1554</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
@@ -54850,7 +54946,7 @@
         <v>315</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X20" s="13"/>
       <c r="Y20" s="13"/>
@@ -54862,14 +54958,14 @@
       </c>
       <c r="AD20" s="13"/>
       <c r="AE20" s="1" t="s">
-        <v>1549</v>
+        <v>1555</v>
       </c>
       <c r="AF20" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG20" s="13"/>
       <c r="AH20" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI20" s="13"/>
       <c r="AJ20" s="13"/>
@@ -54941,7 +55037,7 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4" t="s">
-        <v>1550</v>
+        <v>1556</v>
       </c>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
@@ -54966,7 +55062,7 @@
         <v>315</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
@@ -54974,20 +55070,20 @@
       <c r="AA22" s="13"/>
       <c r="AB22" s="13"/>
       <c r="AC22" s="1" t="s">
-        <v>1541</v>
+        <v>1547</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>1542</v>
+        <v>1548</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>1551</v>
+        <v>1557</v>
       </c>
       <c r="AF22" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG22" s="13"/>
       <c r="AH22" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI22" s="13"/>
       <c r="AJ22" s="13"/>
@@ -55014,7 +55110,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4" t="s">
-        <v>1552</v>
+        <v>1558</v>
       </c>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -55039,7 +55135,7 @@
         <v>315</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
@@ -55053,14 +55149,14 @@
         <v>985</v>
       </c>
       <c r="AE23" s="1" t="s">
-        <v>1553</v>
+        <v>1559</v>
       </c>
       <c r="AF23" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG23" s="13"/>
       <c r="AH23" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI23" s="13"/>
       <c r="AJ23" s="13"/>
@@ -55087,7 +55183,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4" t="s">
-        <v>1554</v>
+        <v>1560</v>
       </c>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
@@ -55112,7 +55208,7 @@
         <v>315</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -55124,14 +55220,14 @@
       </c>
       <c r="AD24" s="13"/>
       <c r="AE24" s="1" t="s">
-        <v>1555</v>
+        <v>1561</v>
       </c>
       <c r="AF24" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG24" s="13"/>
       <c r="AH24" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI24" s="13"/>
       <c r="AJ24" s="13"/>
@@ -55181,7 +55277,7 @@
         <v>315</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
@@ -55191,14 +55287,14 @@
       <c r="AC25" s="13"/>
       <c r="AD25" s="13"/>
       <c r="AE25" s="1" t="s">
-        <v>1556</v>
+        <v>1562</v>
       </c>
       <c r="AF25" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG25" s="13"/>
       <c r="AH25" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI25" s="13"/>
       <c r="AJ25" s="13"/>
@@ -55225,7 +55321,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4" t="s">
-        <v>1557</v>
+        <v>1563</v>
       </c>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
@@ -55250,7 +55346,7 @@
         <v>315</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X26" s="13"/>
       <c r="Y26" s="13"/>
@@ -55262,14 +55358,14 @@
       </c>
       <c r="AD26" s="13"/>
       <c r="AE26" s="1" t="s">
-        <v>1558</v>
+        <v>1564</v>
       </c>
       <c r="AF26" s="1" t="s">
         <v>351</v>
       </c>
       <c r="AG26" s="13"/>
       <c r="AH26" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI26" s="13"/>
       <c r="AJ26" s="13"/>
@@ -55296,7 +55392,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4" t="s">
-        <v>1559</v>
+        <v>1565</v>
       </c>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -55321,7 +55417,7 @@
         <v>315</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X27" s="13"/>
       <c r="Y27" s="13"/>
@@ -55335,14 +55431,14 @@
         <v>1059</v>
       </c>
       <c r="AE27" s="1" t="s">
-        <v>1560</v>
+        <v>1566</v>
       </c>
       <c r="AF27" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG27" s="13"/>
       <c r="AH27" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI27" s="13"/>
       <c r="AJ27" s="13"/>
@@ -55369,7 +55465,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4" t="s">
-        <v>1561</v>
+        <v>1567</v>
       </c>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
@@ -55394,7 +55490,7 @@
         <v>315</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -55408,14 +55504,14 @@
         <v>1059</v>
       </c>
       <c r="AE28" s="1" t="s">
-        <v>1562</v>
+        <v>1568</v>
       </c>
       <c r="AF28" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG28" s="13"/>
       <c r="AH28" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI28" s="13"/>
       <c r="AJ28" s="13"/>
@@ -55442,7 +55538,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4" t="s">
-        <v>1563</v>
+        <v>1569</v>
       </c>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
@@ -55467,7 +55563,7 @@
         <v>315</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X29" s="13"/>
       <c r="Y29" s="13"/>
@@ -55481,14 +55577,14 @@
         <v>1059</v>
       </c>
       <c r="AE29" s="1" t="s">
-        <v>1564</v>
+        <v>1570</v>
       </c>
       <c r="AF29" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG29" s="13"/>
       <c r="AH29" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI29" s="13"/>
       <c r="AJ29" s="13"/>
@@ -55538,7 +55634,7 @@
         <v>315</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X30" s="13"/>
       <c r="Y30" s="13"/>
@@ -55547,17 +55643,17 @@
       <c r="AB30" s="13"/>
       <c r="AC30" s="13"/>
       <c r="AD30" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE30" s="1" t="s">
-        <v>1565</v>
+        <v>1571</v>
       </c>
       <c r="AF30" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG30" s="13"/>
       <c r="AH30" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI30" s="13"/>
       <c r="AJ30" s="13"/>
@@ -55607,7 +55703,7 @@
         <v>315</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
@@ -55616,17 +55712,17 @@
       <c r="AB31" s="13"/>
       <c r="AC31" s="13"/>
       <c r="AD31" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE31" s="1" t="s">
-        <v>1566</v>
+        <v>1572</v>
       </c>
       <c r="AF31" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG31" s="13"/>
       <c r="AH31" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI31" s="13"/>
       <c r="AJ31" s="13"/>
@@ -55653,7 +55749,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4" t="s">
-        <v>1567</v>
+        <v>1573</v>
       </c>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
@@ -55678,7 +55774,7 @@
         <v>315</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>
@@ -55690,14 +55786,14 @@
       </c>
       <c r="AD32" s="13"/>
       <c r="AE32" s="1" t="s">
-        <v>1568</v>
+        <v>1574</v>
       </c>
       <c r="AF32" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG32" s="13"/>
       <c r="AH32" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI32" s="13"/>
       <c r="AJ32" s="13"/>
@@ -55747,7 +55843,7 @@
         <v>315</v>
       </c>
       <c r="W33" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
@@ -55757,14 +55853,14 @@
       <c r="AC33" s="13"/>
       <c r="AD33" s="13"/>
       <c r="AE33" s="1" t="s">
-        <v>1568</v>
+        <v>1574</v>
       </c>
       <c r="AF33" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG33" s="13"/>
       <c r="AH33" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI33" s="13"/>
       <c r="AJ33" s="13"/>
@@ -55791,7 +55887,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4" t="s">
-        <v>1569</v>
+        <v>1575</v>
       </c>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
@@ -55816,7 +55912,7 @@
         <v>315</v>
       </c>
       <c r="W34" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X34" s="13"/>
       <c r="Y34" s="13"/>
@@ -55828,14 +55924,14 @@
       </c>
       <c r="AD34" s="13"/>
       <c r="AE34" s="1" t="s">
-        <v>1570</v>
+        <v>1576</v>
       </c>
       <c r="AF34" s="1" t="s">
         <v>351</v>
       </c>
       <c r="AG34" s="13"/>
       <c r="AH34" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI34" s="13"/>
       <c r="AJ34" s="13"/>
@@ -55885,7 +55981,7 @@
         <v>315</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X35" s="13"/>
       <c r="Y35" s="13"/>
@@ -55897,14 +55993,14 @@
         <v>985</v>
       </c>
       <c r="AE35" s="1" t="s">
-        <v>1571</v>
+        <v>1577</v>
       </c>
       <c r="AF35" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG35" s="13"/>
       <c r="AH35" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI35" s="13"/>
       <c r="AJ35" s="13"/>
@@ -55954,7 +56050,7 @@
         <v>315</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X36" s="13"/>
       <c r="Y36" s="13"/>
@@ -55971,7 +56067,7 @@
       </c>
       <c r="AG36" s="13"/>
       <c r="AH36" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI36" s="13"/>
       <c r="AJ36" s="13"/>
@@ -55998,7 +56094,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4" t="s">
-        <v>1572</v>
+        <v>1578</v>
       </c>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
@@ -56023,7 +56119,7 @@
         <v>315</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X37" s="13"/>
       <c r="Y37" s="13"/>
@@ -56031,20 +56127,20 @@
       <c r="AA37" s="13"/>
       <c r="AB37" s="13"/>
       <c r="AC37" s="1" t="s">
-        <v>1541</v>
+        <v>1547</v>
       </c>
       <c r="AD37" s="1" t="s">
-        <v>1542</v>
+        <v>1548</v>
       </c>
       <c r="AE37" s="1" t="s">
-        <v>1573</v>
+        <v>1579</v>
       </c>
       <c r="AF37" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG37" s="13"/>
       <c r="AH37" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI37" s="13"/>
       <c r="AJ37" s="13"/>
@@ -56071,7 +56167,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4" t="s">
-        <v>1541</v>
+        <v>1547</v>
       </c>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
@@ -56096,7 +56192,7 @@
         <v>315</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X38" s="13"/>
       <c r="Y38" s="13"/>
@@ -56104,20 +56200,20 @@
       <c r="AA38" s="13"/>
       <c r="AB38" s="13"/>
       <c r="AC38" s="1" t="s">
-        <v>1541</v>
+        <v>1547</v>
       </c>
       <c r="AD38" s="1" t="s">
-        <v>1542</v>
+        <v>1548</v>
       </c>
       <c r="AE38" s="1" t="s">
-        <v>1574</v>
+        <v>1580</v>
       </c>
       <c r="AF38" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG38" s="13"/>
       <c r="AH38" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI38" s="13"/>
       <c r="AJ38" s="13"/>
@@ -56144,7 +56240,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4" t="s">
-        <v>1575</v>
+        <v>1581</v>
       </c>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
@@ -56169,7 +56265,7 @@
         <v>315</v>
       </c>
       <c r="W39" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X39" s="13"/>
       <c r="Y39" s="13"/>
@@ -56177,20 +56273,20 @@
       <c r="AA39" s="13"/>
       <c r="AB39" s="13"/>
       <c r="AC39" s="1" t="s">
-        <v>1541</v>
+        <v>1547</v>
       </c>
       <c r="AD39" s="1" t="s">
-        <v>1542</v>
+        <v>1548</v>
       </c>
       <c r="AE39" s="1" t="s">
-        <v>1576</v>
+        <v>1582</v>
       </c>
       <c r="AF39" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG39" s="13"/>
       <c r="AH39" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI39" s="13"/>
       <c r="AJ39" s="13"/>
@@ -56217,7 +56313,7 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4" t="s">
-        <v>1577</v>
+        <v>1583</v>
       </c>
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
@@ -56242,7 +56338,7 @@
         <v>315</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X40" s="13"/>
       <c r="Y40" s="13"/>
@@ -56250,18 +56346,18 @@
       <c r="AA40" s="13"/>
       <c r="AB40" s="13"/>
       <c r="AC40" s="1" t="s">
-        <v>1578</v>
+        <v>1584</v>
       </c>
       <c r="AD40" s="13"/>
       <c r="AE40" s="1" t="s">
-        <v>1579</v>
+        <v>1585</v>
       </c>
       <c r="AF40" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG40" s="13"/>
       <c r="AH40" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI40" s="13"/>
       <c r="AJ40" s="13"/>
@@ -56288,7 +56384,7 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4" t="s">
-        <v>1580</v>
+        <v>1586</v>
       </c>
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
@@ -56313,7 +56409,7 @@
         <v>315</v>
       </c>
       <c r="W41" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X41" s="13"/>
       <c r="Y41" s="13"/>
@@ -56327,14 +56423,14 @@
         <v>985</v>
       </c>
       <c r="AE41" s="1" t="s">
-        <v>1581</v>
+        <v>1587</v>
       </c>
       <c r="AF41" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG41" s="13"/>
       <c r="AH41" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI41" s="13"/>
       <c r="AJ41" s="13"/>
@@ -56384,7 +56480,7 @@
         <v>315</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X42" s="13"/>
       <c r="Y42" s="13"/>
@@ -56394,14 +56490,14 @@
       <c r="AC42" s="13"/>
       <c r="AD42" s="13"/>
       <c r="AE42" s="1" t="s">
-        <v>1582</v>
+        <v>1588</v>
       </c>
       <c r="AF42" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG42" s="13"/>
       <c r="AH42" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI42" s="13"/>
       <c r="AJ42" s="13"/>
@@ -56428,7 +56524,7 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4" t="s">
-        <v>1583</v>
+        <v>1589</v>
       </c>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
@@ -56453,7 +56549,7 @@
         <v>315</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X43" s="13"/>
       <c r="Y43" s="13"/>
@@ -56465,14 +56561,14 @@
       </c>
       <c r="AD43" s="13"/>
       <c r="AE43" s="1" t="s">
-        <v>1584</v>
+        <v>1590</v>
       </c>
       <c r="AF43" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG43" s="13"/>
       <c r="AH43" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI43" s="13"/>
       <c r="AJ43" s="13"/>
@@ -56499,7 +56595,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4" t="s">
-        <v>1585</v>
+        <v>1591</v>
       </c>
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
@@ -56524,7 +56620,7 @@
         <v>315</v>
       </c>
       <c r="W44" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X44" s="13"/>
       <c r="Y44" s="13"/>
@@ -56536,14 +56632,14 @@
       </c>
       <c r="AD44" s="13"/>
       <c r="AE44" s="1" t="s">
-        <v>1586</v>
+        <v>1592</v>
       </c>
       <c r="AF44" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG44" s="13"/>
       <c r="AH44" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI44" s="13"/>
       <c r="AJ44" s="13"/>
@@ -56570,7 +56666,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4" t="s">
-        <v>1587</v>
+        <v>1593</v>
       </c>
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
@@ -56595,7 +56691,7 @@
         <v>315</v>
       </c>
       <c r="W45" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X45" s="13"/>
       <c r="Y45" s="13"/>
@@ -56607,14 +56703,14 @@
       </c>
       <c r="AD45" s="13"/>
       <c r="AE45" s="1" t="s">
-        <v>1588</v>
+        <v>1594</v>
       </c>
       <c r="AF45" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG45" s="13"/>
       <c r="AH45" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI45" s="13"/>
       <c r="AJ45" s="13"/>
@@ -56664,7 +56760,7 @@
         <v>315</v>
       </c>
       <c r="W46" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X46" s="13"/>
       <c r="Y46" s="13"/>
@@ -56674,14 +56770,14 @@
       <c r="AC46" s="13"/>
       <c r="AD46" s="13"/>
       <c r="AE46" s="1" t="s">
-        <v>1589</v>
+        <v>1595</v>
       </c>
       <c r="AF46" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG46" s="13"/>
       <c r="AH46" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI46" s="13"/>
       <c r="AJ46" s="13"/>
@@ -56708,7 +56804,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4" t="s">
-        <v>1590</v>
+        <v>1596</v>
       </c>
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
@@ -56733,7 +56829,7 @@
         <v>315</v>
       </c>
       <c r="W47" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X47" s="13"/>
       <c r="Y47" s="13"/>
@@ -56745,14 +56841,14 @@
       </c>
       <c r="AD47" s="13"/>
       <c r="AE47" s="1" t="s">
-        <v>1591</v>
+        <v>1597</v>
       </c>
       <c r="AF47" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG47" s="13"/>
       <c r="AH47" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI47" s="13"/>
       <c r="AJ47" s="13"/>
@@ -56802,7 +56898,7 @@
         <v>315</v>
       </c>
       <c r="W48" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X48" s="13"/>
       <c r="Y48" s="13"/>
@@ -56812,14 +56908,14 @@
       <c r="AC48" s="13"/>
       <c r="AD48" s="13"/>
       <c r="AE48" s="1" t="s">
-        <v>1592</v>
+        <v>1598</v>
       </c>
       <c r="AF48" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG48" s="13"/>
       <c r="AH48" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI48" s="13"/>
       <c r="AJ48" s="13"/>
@@ -56846,7 +56942,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4" t="s">
-        <v>1593</v>
+        <v>1599</v>
       </c>
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
@@ -56871,7 +56967,7 @@
         <v>315</v>
       </c>
       <c r="W49" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X49" s="13"/>
       <c r="Y49" s="13"/>
@@ -56883,14 +56979,14 @@
       </c>
       <c r="AD49" s="13"/>
       <c r="AE49" s="1" t="s">
-        <v>1594</v>
+        <v>1600</v>
       </c>
       <c r="AF49" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG49" s="13"/>
       <c r="AH49" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI49" s="13"/>
       <c r="AJ49" s="13"/>
@@ -56940,7 +57036,7 @@
         <v>315</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X50" s="13"/>
       <c r="Y50" s="13"/>
@@ -56950,14 +57046,14 @@
       <c r="AC50" s="13"/>
       <c r="AD50" s="13"/>
       <c r="AE50" s="1" t="s">
-        <v>1595</v>
+        <v>1601</v>
       </c>
       <c r="AF50" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG50" s="13"/>
       <c r="AH50" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI50" s="13"/>
       <c r="AJ50" s="13"/>
@@ -57007,7 +57103,7 @@
         <v>315</v>
       </c>
       <c r="W51" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X51" s="13"/>
       <c r="Y51" s="13"/>
@@ -57016,17 +57112,17 @@
       <c r="AB51" s="13"/>
       <c r="AC51" s="13"/>
       <c r="AD51" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE51" s="1" t="s">
-        <v>1596</v>
+        <v>1602</v>
       </c>
       <c r="AF51" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG51" s="13"/>
       <c r="AH51" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI51" s="13"/>
       <c r="AJ51" s="13"/>
@@ -57076,7 +57172,7 @@
         <v>315</v>
       </c>
       <c r="W52" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X52" s="13"/>
       <c r="Y52" s="13"/>
@@ -57085,17 +57181,17 @@
       <c r="AB52" s="13"/>
       <c r="AC52" s="13"/>
       <c r="AD52" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE52" s="1" t="s">
-        <v>1597</v>
+        <v>1603</v>
       </c>
       <c r="AF52" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG52" s="13"/>
       <c r="AH52" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI52" s="13"/>
       <c r="AJ52" s="13"/>
@@ -57122,7 +57218,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4" t="s">
-        <v>1598</v>
+        <v>1604</v>
       </c>
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
@@ -57147,7 +57243,7 @@
         <v>315</v>
       </c>
       <c r="W53" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X53" s="13"/>
       <c r="Y53" s="13"/>
@@ -57161,14 +57257,14 @@
         <v>985</v>
       </c>
       <c r="AE53" s="1" t="s">
-        <v>1599</v>
+        <v>1605</v>
       </c>
       <c r="AF53" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG53" s="13"/>
       <c r="AH53" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI53" s="13"/>
       <c r="AJ53" s="13"/>
@@ -57218,7 +57314,7 @@
         <v>315</v>
       </c>
       <c r="W54" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X54" s="13"/>
       <c r="Y54" s="13"/>
@@ -57230,14 +57326,14 @@
         <v>985</v>
       </c>
       <c r="AE54" s="1" t="s">
-        <v>1600</v>
+        <v>1606</v>
       </c>
       <c r="AF54" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG54" s="13"/>
       <c r="AH54" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI54" s="13"/>
       <c r="AJ54" s="13"/>
@@ -57264,7 +57360,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4" t="s">
-        <v>1601</v>
+        <v>1607</v>
       </c>
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
@@ -57289,7 +57385,7 @@
         <v>315</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X55" s="13"/>
       <c r="Y55" s="13"/>
@@ -57303,14 +57399,14 @@
         <v>985</v>
       </c>
       <c r="AE55" s="1" t="s">
-        <v>1602</v>
+        <v>1608</v>
       </c>
       <c r="AF55" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG55" s="13"/>
       <c r="AH55" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI55" s="13"/>
       <c r="AJ55" s="13"/>
@@ -57384,7 +57480,7 @@
         <v>315</v>
       </c>
       <c r="W57" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X57" s="13"/>
       <c r="Y57" s="13"/>
@@ -57396,14 +57492,14 @@
         <v>985</v>
       </c>
       <c r="AE57" s="1" t="s">
-        <v>1603</v>
+        <v>1609</v>
       </c>
       <c r="AF57" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG57" s="13"/>
       <c r="AH57" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI57" s="13"/>
       <c r="AJ57" s="13"/>
@@ -57453,7 +57549,7 @@
         <v>315</v>
       </c>
       <c r="W58" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X58" s="13"/>
       <c r="Y58" s="13"/>
@@ -57465,14 +57561,14 @@
         <v>985</v>
       </c>
       <c r="AE58" s="1" t="s">
-        <v>1604</v>
+        <v>1610</v>
       </c>
       <c r="AF58" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG58" s="13"/>
       <c r="AH58" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI58" s="13"/>
       <c r="AJ58" s="13"/>
@@ -57499,7 +57595,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4" t="s">
-        <v>1605</v>
+        <v>1611</v>
       </c>
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
@@ -57524,7 +57620,7 @@
         <v>315</v>
       </c>
       <c r="W59" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X59" s="13"/>
       <c r="Y59" s="13"/>
@@ -57532,20 +57628,20 @@
       <c r="AA59" s="13"/>
       <c r="AB59" s="13"/>
       <c r="AC59" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AD59" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE59" s="1" t="s">
-        <v>1606</v>
+        <v>1612</v>
       </c>
       <c r="AF59" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG59" s="13"/>
       <c r="AH59" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI59" s="13"/>
       <c r="AJ59" s="13"/>
@@ -57595,7 +57691,7 @@
         <v>315</v>
       </c>
       <c r="W60" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X60" s="13"/>
       <c r="Y60" s="13"/>
@@ -57604,17 +57700,17 @@
       <c r="AB60" s="13"/>
       <c r="AC60" s="13"/>
       <c r="AD60" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE60" s="1" t="s">
-        <v>1607</v>
+        <v>1613</v>
       </c>
       <c r="AF60" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG60" s="13"/>
       <c r="AH60" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI60" s="13"/>
       <c r="AJ60" s="13"/>
@@ -57641,7 +57737,7 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4" t="s">
-        <v>1608</v>
+        <v>1614</v>
       </c>
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
@@ -57666,7 +57762,7 @@
         <v>315</v>
       </c>
       <c r="W61" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X61" s="13"/>
       <c r="Y61" s="13"/>
@@ -57678,14 +57774,14 @@
       </c>
       <c r="AD61" s="13"/>
       <c r="AE61" s="1" t="s">
-        <v>1609</v>
+        <v>1615</v>
       </c>
       <c r="AF61" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG61" s="13"/>
       <c r="AH61" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI61" s="13"/>
       <c r="AJ61" s="13"/>
@@ -57735,7 +57831,7 @@
         <v>315</v>
       </c>
       <c r="W62" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X62" s="13"/>
       <c r="Y62" s="13"/>
@@ -57745,14 +57841,14 @@
       <c r="AC62" s="13"/>
       <c r="AD62" s="13"/>
       <c r="AE62" s="1" t="s">
-        <v>1610</v>
+        <v>1616</v>
       </c>
       <c r="AF62" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG62" s="13"/>
       <c r="AH62" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI62" s="13"/>
       <c r="AJ62" s="13"/>
@@ -57779,7 +57875,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4" t="s">
-        <v>1611</v>
+        <v>1617</v>
       </c>
       <c r="O63" s="6"/>
       <c r="P63" s="6"/>
@@ -57804,7 +57900,7 @@
         <v>315</v>
       </c>
       <c r="W63" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X63" s="13"/>
       <c r="Y63" s="13"/>
@@ -57816,14 +57912,14 @@
       </c>
       <c r="AD63" s="13"/>
       <c r="AE63" s="1" t="s">
-        <v>1612</v>
+        <v>1618</v>
       </c>
       <c r="AF63" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG63" s="13"/>
       <c r="AH63" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI63" s="13"/>
       <c r="AJ63" s="13"/>
@@ -57873,7 +57969,7 @@
         <v>315</v>
       </c>
       <c r="W64" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X64" s="13"/>
       <c r="Y64" s="13"/>
@@ -57883,14 +57979,14 @@
       <c r="AC64" s="13"/>
       <c r="AD64" s="13"/>
       <c r="AE64" s="1" t="s">
-        <v>1613</v>
+        <v>1619</v>
       </c>
       <c r="AF64" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG64" s="13"/>
       <c r="AH64" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI64" s="13"/>
       <c r="AJ64" s="13"/>
@@ -57940,7 +58036,7 @@
         <v>315</v>
       </c>
       <c r="W65" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X65" s="13"/>
       <c r="Y65" s="13"/>
@@ -57949,17 +58045,17 @@
       <c r="AB65" s="13"/>
       <c r="AC65" s="13"/>
       <c r="AD65" s="1" t="s">
-        <v>1542</v>
+        <v>1548</v>
       </c>
       <c r="AE65" s="1" t="s">
-        <v>1614</v>
+        <v>1620</v>
       </c>
       <c r="AF65" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG65" s="13"/>
       <c r="AH65" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI65" s="13"/>
       <c r="AJ65" s="13"/>
@@ -58009,7 +58105,7 @@
         <v>315</v>
       </c>
       <c r="W66" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X66" s="13"/>
       <c r="Y66" s="13"/>
@@ -58019,14 +58115,14 @@
       <c r="AC66" s="13"/>
       <c r="AD66" s="13"/>
       <c r="AE66" s="1" t="s">
-        <v>1615</v>
+        <v>1621</v>
       </c>
       <c r="AF66" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG66" s="13"/>
       <c r="AH66" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI66" s="13"/>
       <c r="AJ66" s="13"/>
@@ -58100,7 +58196,7 @@
         <v>315</v>
       </c>
       <c r="W68" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X68" s="13"/>
       <c r="Y68" s="13"/>
@@ -58117,7 +58213,7 @@
       </c>
       <c r="AG68" s="13"/>
       <c r="AH68" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI68" s="13"/>
       <c r="AJ68" s="13"/>
@@ -58144,7 +58240,7 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4" t="s">
-        <v>1616</v>
+        <v>1622</v>
       </c>
       <c r="O69" s="6"/>
       <c r="P69" s="6"/>
@@ -58169,7 +58265,7 @@
         <v>315</v>
       </c>
       <c r="W69" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X69" s="13"/>
       <c r="Y69" s="13"/>
@@ -58181,14 +58277,14 @@
       </c>
       <c r="AD69" s="13"/>
       <c r="AE69" s="1" t="s">
-        <v>1617</v>
+        <v>1623</v>
       </c>
       <c r="AF69" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG69" s="13"/>
       <c r="AH69" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI69" s="13"/>
       <c r="AJ69" s="13"/>
@@ -58215,7 +58311,7 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4" t="s">
-        <v>1618</v>
+        <v>1624</v>
       </c>
       <c r="O70" s="6"/>
       <c r="P70" s="6"/>
@@ -58240,7 +58336,7 @@
         <v>315</v>
       </c>
       <c r="W70" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X70" s="13"/>
       <c r="Y70" s="13"/>
@@ -58254,14 +58350,14 @@
         <v>985</v>
       </c>
       <c r="AE70" s="1" t="s">
-        <v>1619</v>
+        <v>1625</v>
       </c>
       <c r="AF70" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG70" s="13"/>
       <c r="AH70" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI70" s="13"/>
       <c r="AJ70" s="13"/>
@@ -58288,7 +58384,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
       <c r="N71" s="4" t="s">
-        <v>1620</v>
+        <v>1626</v>
       </c>
       <c r="O71" s="6"/>
       <c r="P71" s="6"/>
@@ -58313,7 +58409,7 @@
         <v>315</v>
       </c>
       <c r="W71" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X71" s="13"/>
       <c r="Y71" s="13"/>
@@ -58325,14 +58421,14 @@
       </c>
       <c r="AD71" s="13"/>
       <c r="AE71" s="1" t="s">
-        <v>1621</v>
+        <v>1627</v>
       </c>
       <c r="AF71" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG71" s="13"/>
       <c r="AH71" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI71" s="13"/>
       <c r="AJ71" s="13"/>
@@ -58359,7 +58455,7 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
       <c r="N72" s="4" t="s">
-        <v>1622</v>
+        <v>1628</v>
       </c>
       <c r="O72" s="6"/>
       <c r="P72" s="6"/>
@@ -58384,7 +58480,7 @@
         <v>315</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X72" s="13"/>
       <c r="Y72" s="13"/>
@@ -58396,14 +58492,14 @@
       </c>
       <c r="AD72" s="13"/>
       <c r="AE72" s="1" t="s">
-        <v>1623</v>
+        <v>1629</v>
       </c>
       <c r="AF72" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG72" s="13"/>
       <c r="AH72" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI72" s="13"/>
       <c r="AJ72" s="13"/>
@@ -58453,7 +58549,7 @@
         <v>315</v>
       </c>
       <c r="W73" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X73" s="13"/>
       <c r="Y73" s="13"/>
@@ -58462,17 +58558,17 @@
       <c r="AB73" s="13"/>
       <c r="AC73" s="13"/>
       <c r="AD73" s="1" t="s">
-        <v>1542</v>
+        <v>1548</v>
       </c>
       <c r="AE73" s="1" t="s">
-        <v>1624</v>
+        <v>1630</v>
       </c>
       <c r="AF73" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG73" s="13"/>
       <c r="AH73" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI73" s="13"/>
       <c r="AJ73" s="13"/>
@@ -58499,7 +58595,7 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4" t="s">
-        <v>1625</v>
+        <v>1631</v>
       </c>
       <c r="O74" s="6"/>
       <c r="P74" s="6"/>
@@ -58524,7 +58620,7 @@
         <v>315</v>
       </c>
       <c r="W74" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X74" s="13"/>
       <c r="Y74" s="13"/>
@@ -58535,17 +58631,17 @@
         <v>349</v>
       </c>
       <c r="AD74" s="1" t="s">
-        <v>1626</v>
+        <v>1632</v>
       </c>
       <c r="AE74" s="1" t="s">
-        <v>1627</v>
+        <v>1633</v>
       </c>
       <c r="AF74" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG74" s="13"/>
       <c r="AH74" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI74" s="13"/>
       <c r="AJ74" s="13"/>
@@ -58595,7 +58691,7 @@
         <v>315</v>
       </c>
       <c r="W75" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X75" s="13"/>
       <c r="Y75" s="13"/>
@@ -58605,14 +58701,14 @@
       <c r="AC75" s="13"/>
       <c r="AD75" s="13"/>
       <c r="AE75" s="1" t="s">
-        <v>1628</v>
+        <v>1634</v>
       </c>
       <c r="AF75" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG75" s="13"/>
       <c r="AH75" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI75" s="13"/>
       <c r="AJ75" s="13"/>
@@ -58662,7 +58758,7 @@
         <v>315</v>
       </c>
       <c r="W76" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X76" s="13"/>
       <c r="Y76" s="13"/>
@@ -58672,14 +58768,14 @@
       <c r="AC76" s="13"/>
       <c r="AD76" s="13"/>
       <c r="AE76" s="1" t="s">
-        <v>1629</v>
+        <v>1635</v>
       </c>
       <c r="AF76" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG76" s="13"/>
       <c r="AH76" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI76" s="13"/>
       <c r="AJ76" s="13"/>
@@ -58729,7 +58825,7 @@
         <v>315</v>
       </c>
       <c r="W77" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X77" s="13"/>
       <c r="Y77" s="13"/>
@@ -58738,17 +58834,17 @@
       <c r="AB77" s="13"/>
       <c r="AC77" s="13"/>
       <c r="AD77" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE77" s="1" t="s">
-        <v>1630</v>
+        <v>1636</v>
       </c>
       <c r="AF77" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG77" s="13"/>
       <c r="AH77" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI77" s="13"/>
       <c r="AJ77" s="13"/>
@@ -58798,7 +58894,7 @@
         <v>315</v>
       </c>
       <c r="W78" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X78" s="13"/>
       <c r="Y78" s="13"/>
@@ -58807,17 +58903,17 @@
       <c r="AB78" s="13"/>
       <c r="AC78" s="13"/>
       <c r="AD78" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE78" s="1" t="s">
-        <v>1631</v>
+        <v>1637</v>
       </c>
       <c r="AF78" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG78" s="13"/>
       <c r="AH78" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI78" s="13"/>
       <c r="AJ78" s="13"/>
@@ -58844,7 +58940,7 @@
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
       <c r="N79" s="4" t="s">
-        <v>1632</v>
+        <v>1638</v>
       </c>
       <c r="O79" s="6"/>
       <c r="P79" s="6"/>
@@ -58869,7 +58965,7 @@
         <v>315</v>
       </c>
       <c r="W79" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X79" s="13"/>
       <c r="Y79" s="13"/>
@@ -58881,14 +58977,14 @@
       </c>
       <c r="AD79" s="13"/>
       <c r="AE79" s="1" t="s">
-        <v>1633</v>
+        <v>1639</v>
       </c>
       <c r="AF79" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG79" s="13"/>
       <c r="AH79" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI79" s="13"/>
       <c r="AJ79" s="13"/>
@@ -58915,7 +59011,7 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
       <c r="N80" s="4" t="s">
-        <v>1634</v>
+        <v>1640</v>
       </c>
       <c r="O80" s="6"/>
       <c r="P80" s="6"/>
@@ -58940,7 +59036,7 @@
         <v>315</v>
       </c>
       <c r="W80" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X80" s="13"/>
       <c r="Y80" s="13"/>
@@ -58952,14 +59048,14 @@
       </c>
       <c r="AD80" s="13"/>
       <c r="AE80" s="1" t="s">
-        <v>1635</v>
+        <v>1641</v>
       </c>
       <c r="AF80" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG80" s="13"/>
       <c r="AH80" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI80" s="13"/>
       <c r="AJ80" s="13"/>
@@ -59009,7 +59105,7 @@
         <v>315</v>
       </c>
       <c r="W81" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X81" s="13"/>
       <c r="Y81" s="13"/>
@@ -59018,17 +59114,17 @@
       <c r="AB81" s="13"/>
       <c r="AC81" s="13"/>
       <c r="AD81" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE81" s="1" t="s">
-        <v>1636</v>
+        <v>1642</v>
       </c>
       <c r="AF81" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG81" s="13"/>
       <c r="AH81" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI81" s="13"/>
       <c r="AJ81" s="13"/>
@@ -59055,7 +59151,7 @@
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
       <c r="N82" s="4" t="s">
-        <v>1637</v>
+        <v>1643</v>
       </c>
       <c r="O82" s="6"/>
       <c r="P82" s="6"/>
@@ -59080,7 +59176,7 @@
         <v>315</v>
       </c>
       <c r="W82" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X82" s="13"/>
       <c r="Y82" s="13"/>
@@ -59092,14 +59188,14 @@
       </c>
       <c r="AD82" s="13"/>
       <c r="AE82" s="1" t="s">
-        <v>1638</v>
+        <v>1644</v>
       </c>
       <c r="AF82" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG82" s="13"/>
       <c r="AH82" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI82" s="13"/>
       <c r="AJ82" s="13"/>
@@ -59149,7 +59245,7 @@
         <v>315</v>
       </c>
       <c r="W83" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X83" s="13"/>
       <c r="Y83" s="13"/>
@@ -59159,14 +59255,14 @@
       <c r="AC83" s="13"/>
       <c r="AD83" s="13"/>
       <c r="AE83" s="1" t="s">
-        <v>1639</v>
+        <v>1645</v>
       </c>
       <c r="AF83" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG83" s="13"/>
       <c r="AH83" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI83" s="13"/>
       <c r="AJ83" s="13"/>
@@ -59238,7 +59334,7 @@
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
       <c r="N85" s="4" t="s">
-        <v>1640</v>
+        <v>1646</v>
       </c>
       <c r="O85" s="6"/>
       <c r="P85" s="6"/>
@@ -59263,7 +59359,7 @@
         <v>315</v>
       </c>
       <c r="W85" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X85" s="13"/>
       <c r="Y85" s="13"/>
@@ -59277,14 +59373,14 @@
         <v>1059</v>
       </c>
       <c r="AE85" s="1" t="s">
-        <v>1641</v>
+        <v>1647</v>
       </c>
       <c r="AF85" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG85" s="13"/>
       <c r="AH85" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI85" s="13"/>
       <c r="AJ85" s="13"/>
@@ -59334,7 +59430,7 @@
         <v>315</v>
       </c>
       <c r="W86" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X86" s="13"/>
       <c r="Y86" s="13"/>
@@ -59343,17 +59439,17 @@
       <c r="AB86" s="13"/>
       <c r="AC86" s="13"/>
       <c r="AD86" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE86" s="1" t="s">
-        <v>1642</v>
+        <v>1648</v>
       </c>
       <c r="AF86" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG86" s="13"/>
       <c r="AH86" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI86" s="13"/>
       <c r="AJ86" s="13"/>
@@ -59403,7 +59499,7 @@
         <v>315</v>
       </c>
       <c r="W87" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X87" s="13"/>
       <c r="Y87" s="13"/>
@@ -59412,17 +59508,17 @@
       <c r="AB87" s="13"/>
       <c r="AC87" s="13"/>
       <c r="AD87" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE87" s="1" t="s">
-        <v>1643</v>
+        <v>1649</v>
       </c>
       <c r="AF87" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG87" s="13"/>
       <c r="AH87" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI87" s="13"/>
       <c r="AJ87" s="13"/>
@@ -59449,7 +59545,7 @@
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
       <c r="N88" s="4" t="s">
-        <v>1644</v>
+        <v>1650</v>
       </c>
       <c r="O88" s="6"/>
       <c r="P88" s="6"/>
@@ -59474,7 +59570,7 @@
         <v>315</v>
       </c>
       <c r="W88" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X88" s="13"/>
       <c r="Y88" s="13"/>
@@ -59485,7 +59581,7 @@
         <v>349</v>
       </c>
       <c r="AD88" s="1" t="s">
-        <v>1626</v>
+        <v>1632</v>
       </c>
       <c r="AE88" s="1" t="s">
         <v>938</v>
@@ -59495,7 +59591,7 @@
       </c>
       <c r="AG88" s="13"/>
       <c r="AH88" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI88" s="13"/>
       <c r="AJ88" s="13"/>
@@ -59545,7 +59641,7 @@
         <v>315</v>
       </c>
       <c r="W89" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X89" s="13"/>
       <c r="Y89" s="13"/>
@@ -59562,7 +59658,7 @@
       </c>
       <c r="AG89" s="13"/>
       <c r="AH89" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI89" s="13"/>
       <c r="AJ89" s="13"/>
@@ -59612,7 +59708,7 @@
         <v>315</v>
       </c>
       <c r="W90" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X90" s="13"/>
       <c r="Y90" s="13"/>
@@ -59622,14 +59718,14 @@
       <c r="AC90" s="13"/>
       <c r="AD90" s="13"/>
       <c r="AE90" s="1" t="s">
-        <v>1645</v>
+        <v>1651</v>
       </c>
       <c r="AF90" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG90" s="13"/>
       <c r="AH90" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI90" s="13"/>
       <c r="AJ90" s="13"/>
@@ -59679,7 +59775,7 @@
         <v>315</v>
       </c>
       <c r="W91" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X91" s="13"/>
       <c r="Y91" s="13"/>
@@ -59688,17 +59784,17 @@
       <c r="AB91" s="13"/>
       <c r="AC91" s="13"/>
       <c r="AD91" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE91" s="1" t="s">
-        <v>1646</v>
+        <v>1652</v>
       </c>
       <c r="AF91" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG91" s="13"/>
       <c r="AH91" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI91" s="13"/>
       <c r="AJ91" s="13"/>
@@ -59748,7 +59844,7 @@
         <v>315</v>
       </c>
       <c r="W92" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X92" s="13"/>
       <c r="Y92" s="13"/>
@@ -59758,14 +59854,14 @@
       <c r="AC92" s="13"/>
       <c r="AD92" s="13"/>
       <c r="AE92" s="1" t="s">
-        <v>1647</v>
+        <v>1653</v>
       </c>
       <c r="AF92" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG92" s="13"/>
       <c r="AH92" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI92" s="13"/>
       <c r="AJ92" s="13"/>
@@ -59792,7 +59888,7 @@
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4" t="s">
-        <v>1648</v>
+        <v>1654</v>
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6"/>
@@ -59817,7 +59913,7 @@
         <v>315</v>
       </c>
       <c r="W93" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X93" s="13"/>
       <c r="Y93" s="13"/>
@@ -59825,20 +59921,20 @@
       <c r="AA93" s="13"/>
       <c r="AB93" s="13"/>
       <c r="AC93" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AD93" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE93" s="1" t="s">
-        <v>1649</v>
+        <v>1655</v>
       </c>
       <c r="AF93" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG93" s="13"/>
       <c r="AH93" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI93" s="13"/>
       <c r="AJ93" s="13"/>
@@ -59888,7 +59984,7 @@
         <v>315</v>
       </c>
       <c r="W94" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X94" s="13"/>
       <c r="Y94" s="13"/>
@@ -59898,14 +59994,14 @@
       <c r="AC94" s="13"/>
       <c r="AD94" s="13"/>
       <c r="AE94" s="1" t="s">
-        <v>1650</v>
+        <v>1656</v>
       </c>
       <c r="AF94" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG94" s="13"/>
       <c r="AH94" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI94" s="13"/>
       <c r="AJ94" s="13"/>
@@ -59932,7 +60028,7 @@
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
       <c r="N95" s="4" t="s">
-        <v>1651</v>
+        <v>1657</v>
       </c>
       <c r="O95" s="6"/>
       <c r="P95" s="6"/>
@@ -59957,7 +60053,7 @@
         <v>315</v>
       </c>
       <c r="W95" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X95" s="13"/>
       <c r="Y95" s="13"/>
@@ -59971,14 +60067,14 @@
         <v>985</v>
       </c>
       <c r="AE95" s="1" t="s">
-        <v>1652</v>
+        <v>1658</v>
       </c>
       <c r="AF95" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG95" s="13"/>
       <c r="AH95" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI95" s="13"/>
       <c r="AJ95" s="13"/>
@@ -60030,7 +60126,7 @@
         <v>315</v>
       </c>
       <c r="W96" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X96" s="13"/>
       <c r="Y96" s="13"/>
@@ -60042,14 +60138,14 @@
       </c>
       <c r="AD96" s="13"/>
       <c r="AE96" s="1" t="s">
-        <v>1653</v>
+        <v>1659</v>
       </c>
       <c r="AF96" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG96" s="13"/>
       <c r="AH96" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI96" s="13"/>
       <c r="AJ96" s="13"/>
@@ -60099,7 +60195,7 @@
         <v>315</v>
       </c>
       <c r="W97" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X97" s="13"/>
       <c r="Y97" s="13"/>
@@ -60111,14 +60207,14 @@
         <v>1059</v>
       </c>
       <c r="AE97" s="1" t="s">
-        <v>1654</v>
+        <v>1660</v>
       </c>
       <c r="AF97" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG97" s="13"/>
       <c r="AH97" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI97" s="13"/>
       <c r="AJ97" s="13"/>
@@ -60145,7 +60241,7 @@
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
       <c r="N98" s="4" t="s">
-        <v>1655</v>
+        <v>1661</v>
       </c>
       <c r="O98" s="6"/>
       <c r="P98" s="6"/>
@@ -60170,7 +60266,7 @@
         <v>315</v>
       </c>
       <c r="W98" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X98" s="13"/>
       <c r="Y98" s="13"/>
@@ -60182,14 +60278,14 @@
       </c>
       <c r="AD98" s="13"/>
       <c r="AE98" s="1" t="s">
-        <v>1656</v>
+        <v>1662</v>
       </c>
       <c r="AF98" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG98" s="13"/>
       <c r="AH98" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI98" s="13"/>
       <c r="AJ98" s="13"/>
@@ -60216,7 +60312,7 @@
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
       <c r="N99" s="4" t="s">
-        <v>1657</v>
+        <v>1663</v>
       </c>
       <c r="O99" s="6"/>
       <c r="P99" s="6"/>
@@ -60241,7 +60337,7 @@
         <v>315</v>
       </c>
       <c r="W99" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X99" s="13"/>
       <c r="Y99" s="13"/>
@@ -60253,14 +60349,14 @@
       </c>
       <c r="AD99" s="13"/>
       <c r="AE99" s="1" t="s">
-        <v>1658</v>
+        <v>1664</v>
       </c>
       <c r="AF99" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG99" s="13"/>
       <c r="AH99" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI99" s="13"/>
       <c r="AJ99" s="13"/>
@@ -60310,7 +60406,7 @@
         <v>315</v>
       </c>
       <c r="W100" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X100" s="13"/>
       <c r="Y100" s="13"/>
@@ -60320,14 +60416,14 @@
       <c r="AC100" s="13"/>
       <c r="AD100" s="13"/>
       <c r="AE100" s="1" t="s">
-        <v>1659</v>
+        <v>1665</v>
       </c>
       <c r="AF100" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG100" s="13"/>
       <c r="AH100" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI100" s="13"/>
       <c r="AJ100" s="13"/>
@@ -60354,7 +60450,7 @@
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
       <c r="N101" s="4" t="s">
-        <v>1660</v>
+        <v>1666</v>
       </c>
       <c r="O101" s="6"/>
       <c r="P101" s="6"/>
@@ -60379,7 +60475,7 @@
         <v>315</v>
       </c>
       <c r="W101" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X101" s="13"/>
       <c r="Y101" s="13"/>
@@ -60393,14 +60489,14 @@
         <v>985</v>
       </c>
       <c r="AE101" s="1" t="s">
-        <v>1661</v>
+        <v>1667</v>
       </c>
       <c r="AF101" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG101" s="13"/>
       <c r="AH101" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI101" s="13"/>
       <c r="AJ101" s="13"/>
@@ -60452,7 +60548,7 @@
         <v>315</v>
       </c>
       <c r="W102" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X102" s="13"/>
       <c r="Y102" s="13"/>
@@ -60471,7 +60567,7 @@
       </c>
       <c r="AG102" s="13"/>
       <c r="AH102" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI102" s="13"/>
       <c r="AJ102" s="13"/>
@@ -60498,7 +60594,7 @@
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4" t="s">
-        <v>1662</v>
+        <v>1668</v>
       </c>
       <c r="O103" s="6"/>
       <c r="P103" s="6"/>
@@ -60523,7 +60619,7 @@
         <v>315</v>
       </c>
       <c r="W103" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X103" s="13"/>
       <c r="Y103" s="13"/>
@@ -60535,14 +60631,14 @@
       </c>
       <c r="AD103" s="13"/>
       <c r="AE103" s="1" t="s">
-        <v>1663</v>
+        <v>1669</v>
       </c>
       <c r="AF103" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG103" s="13"/>
       <c r="AH103" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI103" s="13"/>
       <c r="AJ103" s="13"/>
@@ -60569,7 +60665,7 @@
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4" t="s">
-        <v>1664</v>
+        <v>1670</v>
       </c>
       <c r="O104" s="6"/>
       <c r="P104" s="6"/>
@@ -60594,7 +60690,7 @@
         <v>315</v>
       </c>
       <c r="W104" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X104" s="13"/>
       <c r="Y104" s="13"/>
@@ -60606,14 +60702,14 @@
       </c>
       <c r="AD104" s="13"/>
       <c r="AE104" s="1" t="s">
-        <v>1665</v>
+        <v>1671</v>
       </c>
       <c r="AF104" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG104" s="13"/>
       <c r="AH104" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI104" s="13"/>
       <c r="AJ104" s="13"/>
@@ -60640,7 +60736,7 @@
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4" t="s">
-        <v>1666</v>
+        <v>1672</v>
       </c>
       <c r="O105" s="6"/>
       <c r="P105" s="6"/>
@@ -60665,7 +60761,7 @@
         <v>315</v>
       </c>
       <c r="W105" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X105" s="13"/>
       <c r="Y105" s="13"/>
@@ -60679,14 +60775,14 @@
         <v>704</v>
       </c>
       <c r="AE105" s="1" t="s">
-        <v>1667</v>
+        <v>1673</v>
       </c>
       <c r="AF105" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG105" s="13"/>
       <c r="AH105" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI105" s="13"/>
       <c r="AJ105" s="13"/>
@@ -60714,7 +60810,7 @@
       <c r="M106" s="4"/>
       <c r="AG106" s="13"/>
       <c r="AH106" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI106" s="13"/>
       <c r="AJ106" s="13"/>
@@ -60764,7 +60860,7 @@
         <v>315</v>
       </c>
       <c r="W107" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X107" s="13"/>
       <c r="Y107" s="13"/>
@@ -60774,14 +60870,14 @@
       <c r="AC107" s="13"/>
       <c r="AD107" s="13"/>
       <c r="AE107" s="1" t="s">
-        <v>1668</v>
+        <v>1674</v>
       </c>
       <c r="AF107" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG107" s="13"/>
       <c r="AH107" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI107" s="13"/>
       <c r="AJ107" s="13"/>
@@ -60831,7 +60927,7 @@
         <v>315</v>
       </c>
       <c r="W108" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X108" s="13"/>
       <c r="Y108" s="13"/>
@@ -60844,11 +60940,11 @@
         <v>68</v>
       </c>
       <c r="AF108" s="1" t="s">
-        <v>1669</v>
+        <v>1675</v>
       </c>
       <c r="AG108" s="13"/>
       <c r="AH108" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI108" s="13"/>
       <c r="AJ108" s="13"/>
@@ -60875,7 +60971,7 @@
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4" t="s">
-        <v>1670</v>
+        <v>1676</v>
       </c>
       <c r="O109" s="6"/>
       <c r="P109" s="6"/>
@@ -60900,7 +60996,7 @@
         <v>315</v>
       </c>
       <c r="W109" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X109" s="13"/>
       <c r="Y109" s="13"/>
@@ -60908,20 +61004,20 @@
       <c r="AA109" s="13"/>
       <c r="AB109" s="13"/>
       <c r="AC109" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AD109" s="1" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="AE109" s="1" t="s">
-        <v>1671</v>
+        <v>1677</v>
       </c>
       <c r="AF109" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG109" s="13"/>
       <c r="AH109" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI109" s="13"/>
       <c r="AJ109" s="13"/>
@@ -60948,7 +61044,7 @@
       <c r="L110" s="4"/>
       <c r="M110" s="4"/>
       <c r="N110" s="4" t="s">
-        <v>1672</v>
+        <v>1678</v>
       </c>
       <c r="O110" s="6"/>
       <c r="P110" s="6"/>
@@ -60973,7 +61069,7 @@
         <v>315</v>
       </c>
       <c r="W110" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X110" s="13"/>
       <c r="Y110" s="13"/>
@@ -60985,14 +61081,14 @@
       </c>
       <c r="AD110" s="13"/>
       <c r="AE110" s="1" t="s">
-        <v>1673</v>
+        <v>1679</v>
       </c>
       <c r="AF110" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG110" s="13"/>
       <c r="AH110" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI110" s="13"/>
       <c r="AJ110" s="13"/>
@@ -61042,7 +61138,7 @@
         <v>315</v>
       </c>
       <c r="W111" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X111" s="13"/>
       <c r="Y111" s="13"/>
@@ -61052,14 +61148,14 @@
       <c r="AC111" s="13"/>
       <c r="AD111" s="13"/>
       <c r="AE111" s="1" t="s">
-        <v>1673</v>
+        <v>1679</v>
       </c>
       <c r="AF111" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG111" s="13"/>
       <c r="AH111" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI111" s="13"/>
       <c r="AJ111" s="13"/>
@@ -61109,7 +61205,7 @@
         <v>315</v>
       </c>
       <c r="W112" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X112" s="13"/>
       <c r="Y112" s="13"/>
@@ -61118,17 +61214,17 @@
       <c r="AB112" s="13"/>
       <c r="AC112" s="13"/>
       <c r="AD112" s="1" t="s">
-        <v>1626</v>
+        <v>1632</v>
       </c>
       <c r="AE112" s="1" t="s">
-        <v>1674</v>
+        <v>1680</v>
       </c>
       <c r="AF112" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG112" s="13"/>
       <c r="AH112" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI112" s="13"/>
       <c r="AJ112" s="13"/>
@@ -61178,7 +61274,7 @@
         <v>315</v>
       </c>
       <c r="W113" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X113" s="13"/>
       <c r="Y113" s="13"/>
@@ -61187,17 +61283,17 @@
       <c r="AB113" s="13"/>
       <c r="AC113" s="13"/>
       <c r="AD113" s="1" t="s">
-        <v>1626</v>
+        <v>1632</v>
       </c>
       <c r="AE113" s="1" t="s">
-        <v>1675</v>
+        <v>1681</v>
       </c>
       <c r="AF113" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG113" s="13"/>
       <c r="AH113" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI113" s="13"/>
       <c r="AJ113" s="13"/>
@@ -61224,7 +61320,7 @@
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
       <c r="N114" s="4" t="s">
-        <v>1676</v>
+        <v>1682</v>
       </c>
       <c r="O114" s="6"/>
       <c r="P114" s="6"/>
@@ -61249,7 +61345,7 @@
         <v>315</v>
       </c>
       <c r="W114" s="1" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="X114" s="13"/>
       <c r="Y114" s="13"/>
@@ -61264,7 +61360,7 @@
       <c r="AF114" s="13"/>
       <c r="AG114" s="13"/>
       <c r="AH114" s="14" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AI114" s="13"/>
       <c r="AJ114" s="13"/>
@@ -61319,14 +61415,14 @@
       <c r="X115" s="34"/>
       <c r="Y115" s="34"/>
       <c r="Z115" s="36" t="s">
-        <v>1677</v>
+        <v>1683</v>
       </c>
       <c r="AA115" s="36" t="s">
-        <v>1678</v>
+        <v>1684</v>
       </c>
       <c r="AB115" s="34"/>
       <c r="AC115" s="34" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AD115" s="34"/>
       <c r="AE115" s="34"/>
@@ -61489,7 +61585,7 @@
       <c r="K116" s="34"/>
       <c r="L116" s="34"/>
       <c r="M116" s="36" t="s">
-        <v>1679</v>
+        <v>1685</v>
       </c>
       <c r="N116" s="34"/>
       <c r="O116" s="34"/>
@@ -61522,14 +61618,14 @@
       <c r="X116" s="34"/>
       <c r="Y116" s="34"/>
       <c r="Z116" s="36" t="s">
-        <v>1679</v>
+        <v>1685</v>
       </c>
       <c r="AA116" s="36" t="s">
-        <v>1680</v>
+        <v>1686</v>
       </c>
       <c r="AB116" s="34"/>
       <c r="AC116" s="34" t="s">
-        <v>1681</v>
+        <v>1687</v>
       </c>
       <c r="AD116" s="34"/>
       <c r="AE116" s="34"/>
@@ -61551,7 +61647,7 @@
       <c r="AU116" s="34"/>
       <c r="AV116" s="37"/>
       <c r="AW116" s="37" t="s">
-        <v>1682</v>
+        <v>1688</v>
       </c>
       <c r="AX116" s="37"/>
       <c r="AY116" s="37"/>
@@ -61725,14 +61821,14 @@
       <c r="X117" s="34"/>
       <c r="Y117" s="34"/>
       <c r="Z117" s="36" t="s">
-        <v>1683</v>
+        <v>1689</v>
       </c>
       <c r="AA117" s="36" t="s">
-        <v>1684</v>
+        <v>1690</v>
       </c>
       <c r="AB117" s="34"/>
       <c r="AC117" s="34" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="AD117" s="34"/>
       <c r="AE117" s="34"/>
@@ -61754,7 +61850,7 @@
       <c r="AU117" s="34"/>
       <c r="AV117" s="37"/>
       <c r="AW117" s="37" t="s">
-        <v>1682</v>
+        <v>1688</v>
       </c>
       <c r="AX117" s="37"/>
       <c r="AY117" s="37"/>
@@ -61883,13 +61979,13 @@
     </row>
     <row r="118" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A118" s="38" t="s">
-        <v>1685</v>
+        <v>1691</v>
       </c>
       <c r="B118" s="39" t="s">
-        <v>1686</v>
+        <v>1692</v>
       </c>
       <c r="C118" s="38" t="s">
-        <v>1687</v>
+        <v>1693</v>
       </c>
       <c r="D118" s="38"/>
       <c r="E118" s="38" t="s">
@@ -61905,10 +62001,10 @@
       <c r="M118" s="39"/>
       <c r="N118" s="39"/>
       <c r="O118" s="38" t="s">
-        <v>1688</v>
+        <v>1694</v>
       </c>
       <c r="P118" s="38" t="s">
-        <v>1688</v>
+        <v>1694</v>
       </c>
       <c r="Q118" s="40" t="s">
         <v>609</v>
@@ -61946,12 +62042,12 @@
       <c r="AH118" s="39"/>
       <c r="AI118" s="39"/>
       <c r="AJ118" s="38" t="s">
-        <v>1689</v>
+        <v>1695</v>
       </c>
       <c r="AK118" s="38"/>
       <c r="AL118" s="38"/>
       <c r="AM118" s="38" t="s">
-        <v>1689</v>
+        <v>1695</v>
       </c>
       <c r="AN118" s="38"/>
       <c r="AO118" s="38" t="s">
@@ -61970,14 +62066,14 @@
         <v>69</v>
       </c>
       <c r="AT118" s="38" t="s">
-        <v>1685</v>
+        <v>1691</v>
       </c>
       <c r="AU118" s="39" t="s">
-        <v>1686</v>
+        <v>1692</v>
       </c>
       <c r="AV118" s="39"/>
       <c r="AW118" s="39" t="s">
-        <v>1690</v>
+        <v>1696</v>
       </c>
       <c r="AX118" s="39"/>
       <c r="AY118" s="39"/>
@@ -62106,13 +62202,13 @@
     </row>
     <row r="119" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A119" s="38" t="s">
-        <v>1691</v>
+        <v>1697</v>
       </c>
       <c r="B119" s="39" t="s">
-        <v>1692</v>
+        <v>1698</v>
       </c>
       <c r="C119" s="38" t="s">
-        <v>1693</v>
+        <v>1699</v>
       </c>
       <c r="D119" s="38"/>
       <c r="E119" s="38" t="s">
@@ -62128,10 +62224,10 @@
       <c r="M119" s="39"/>
       <c r="N119" s="39"/>
       <c r="O119" s="38" t="s">
-        <v>1688</v>
+        <v>1694</v>
       </c>
       <c r="P119" s="38" t="s">
-        <v>1688</v>
+        <v>1694</v>
       </c>
       <c r="Q119" s="40" t="s">
         <v>359</v>
@@ -62169,12 +62265,12 @@
       <c r="AH119" s="39"/>
       <c r="AI119" s="39"/>
       <c r="AJ119" s="38" t="s">
-        <v>1694</v>
+        <v>1700</v>
       </c>
       <c r="AK119" s="38"/>
       <c r="AL119" s="38"/>
       <c r="AM119" s="38" t="s">
-        <v>1694</v>
+        <v>1700</v>
       </c>
       <c r="AN119" s="38"/>
       <c r="AO119" s="38" t="s">
@@ -62193,14 +62289,14 @@
         <v>69</v>
       </c>
       <c r="AT119" s="38" t="s">
-        <v>1691</v>
+        <v>1697</v>
       </c>
       <c r="AU119" s="39" t="s">
-        <v>1692</v>
+        <v>1698</v>
       </c>
       <c r="AV119" s="39"/>
       <c r="AW119" s="39" t="s">
-        <v>1690</v>
+        <v>1696</v>
       </c>
       <c r="AX119" s="39"/>
       <c r="AY119" s="39"/>
@@ -62329,13 +62425,13 @@
     </row>
     <row r="120" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A120" s="38" t="s">
-        <v>1695</v>
+        <v>1701</v>
       </c>
       <c r="B120" s="39" t="s">
-        <v>1696</v>
+        <v>1702</v>
       </c>
       <c r="C120" s="38" t="s">
-        <v>1697</v>
+        <v>1703</v>
       </c>
       <c r="D120" s="38"/>
       <c r="E120" s="38" t="s">
@@ -62351,10 +62447,10 @@
       <c r="M120" s="39"/>
       <c r="N120" s="39"/>
       <c r="O120" s="38" t="s">
-        <v>1688</v>
+        <v>1694</v>
       </c>
       <c r="P120" s="38" t="s">
-        <v>1688</v>
+        <v>1694</v>
       </c>
       <c r="Q120" s="40" t="s">
         <v>909</v>
@@ -62392,12 +62488,12 @@
       <c r="AH120" s="39"/>
       <c r="AI120" s="39"/>
       <c r="AJ120" s="38" t="s">
-        <v>1698</v>
+        <v>1704</v>
       </c>
       <c r="AK120" s="38"/>
       <c r="AL120" s="38"/>
       <c r="AM120" s="38" t="s">
-        <v>1698</v>
+        <v>1704</v>
       </c>
       <c r="AN120" s="38"/>
       <c r="AO120" s="38" t="s">
@@ -62416,14 +62512,14 @@
         <v>69</v>
       </c>
       <c r="AT120" s="38" t="s">
-        <v>1695</v>
+        <v>1701</v>
       </c>
       <c r="AU120" s="39" t="s">
-        <v>1696</v>
+        <v>1702</v>
       </c>
       <c r="AV120" s="39"/>
       <c r="AW120" s="39" t="s">
-        <v>1699</v>
+        <v>1705</v>
       </c>
       <c r="AX120" s="39"/>
       <c r="AY120" s="39"/>
@@ -62552,13 +62648,13 @@
     </row>
     <row r="121" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A121" s="38" t="s">
-        <v>1700</v>
+        <v>1706</v>
       </c>
       <c r="B121" s="39" t="s">
-        <v>1701</v>
+        <v>1707</v>
       </c>
       <c r="C121" s="38" t="s">
-        <v>1702</v>
+        <v>1708</v>
       </c>
       <c r="D121" s="38"/>
       <c r="E121" s="38" t="s">
@@ -62574,10 +62670,10 @@
       <c r="M121" s="39"/>
       <c r="N121" s="39"/>
       <c r="O121" s="38" t="s">
-        <v>1688</v>
+        <v>1694</v>
       </c>
       <c r="P121" s="38" t="s">
-        <v>1688</v>
+        <v>1694</v>
       </c>
       <c r="Q121" s="40" t="s">
         <v>99</v>
@@ -62615,12 +62711,12 @@
       <c r="AH121" s="39"/>
       <c r="AI121" s="39"/>
       <c r="AJ121" s="38" t="s">
-        <v>1703</v>
+        <v>1709</v>
       </c>
       <c r="AK121" s="38"/>
       <c r="AL121" s="38"/>
       <c r="AM121" s="38" t="s">
-        <v>1698</v>
+        <v>1704</v>
       </c>
       <c r="AN121" s="38"/>
       <c r="AO121" s="38" t="s">
@@ -62639,14 +62735,14 @@
         <v>69</v>
       </c>
       <c r="AT121" s="38" t="s">
-        <v>1700</v>
+        <v>1706</v>
       </c>
       <c r="AU121" s="39" t="s">
-        <v>1701</v>
+        <v>1707</v>
       </c>
       <c r="AV121" s="39"/>
       <c r="AW121" s="39" t="s">
-        <v>1690</v>
+        <v>1696</v>
       </c>
       <c r="AX121" s="39"/>
       <c r="AY121" s="39"/>
@@ -62775,13 +62871,13 @@
     </row>
     <row r="122" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A122" s="38" t="s">
-        <v>1691</v>
+        <v>1697</v>
       </c>
       <c r="B122" s="39" t="s">
-        <v>1692</v>
+        <v>1698</v>
       </c>
       <c r="C122" s="38" t="s">
-        <v>1704</v>
+        <v>1710</v>
       </c>
       <c r="D122" s="38"/>
       <c r="E122" s="38" t="s">
@@ -62797,10 +62893,10 @@
       <c r="M122" s="39"/>
       <c r="N122" s="39"/>
       <c r="O122" s="38" t="s">
-        <v>1691</v>
+        <v>1697</v>
       </c>
       <c r="P122" s="38" t="s">
-        <v>1691</v>
+        <v>1697</v>
       </c>
       <c r="Q122" s="40" t="s">
         <v>909</v>
@@ -62838,12 +62934,12 @@
       <c r="AH122" s="39"/>
       <c r="AI122" s="39"/>
       <c r="AJ122" s="38" t="s">
-        <v>1704</v>
+        <v>1710</v>
       </c>
       <c r="AK122" s="38"/>
       <c r="AL122" s="38"/>
       <c r="AM122" s="38" t="s">
-        <v>1704</v>
+        <v>1710</v>
       </c>
       <c r="AN122" s="38"/>
       <c r="AO122" s="38" t="s">
@@ -62862,14 +62958,14 @@
         <v>69</v>
       </c>
       <c r="AT122" s="38" t="s">
-        <v>1691</v>
+        <v>1697</v>
       </c>
       <c r="AU122" s="39" t="s">
-        <v>1692</v>
+        <v>1698</v>
       </c>
       <c r="AV122" s="39"/>
       <c r="AW122" s="39" t="s">
-        <v>1690</v>
+        <v>1696</v>
       </c>
       <c r="AX122" s="39"/>
       <c r="AY122" s="39"/>
@@ -62998,13 +63094,13 @@
     </row>
     <row r="123" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A123" s="32" t="s">
-        <v>1705</v>
+        <v>1711</v>
       </c>
       <c r="B123" s="42" t="s">
-        <v>1706</v>
+        <v>1712</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>1707</v>
+        <v>1713</v>
       </c>
       <c r="D123" s="32"/>
       <c r="E123" s="32" t="s">
@@ -63020,10 +63116,10 @@
       <c r="M123" s="42"/>
       <c r="N123" s="42"/>
       <c r="O123" s="32" t="s">
-        <v>1705</v>
+        <v>1711</v>
       </c>
       <c r="P123" s="32" t="s">
-        <v>1705</v>
+        <v>1711</v>
       </c>
       <c r="Q123" s="43" t="s">
         <v>609</v>
@@ -63061,12 +63157,12 @@
       <c r="AH123" s="42"/>
       <c r="AI123" s="42"/>
       <c r="AJ123" s="32" t="s">
-        <v>1707</v>
+        <v>1713</v>
       </c>
       <c r="AK123" s="32"/>
       <c r="AL123" s="32"/>
       <c r="AM123" s="32" t="s">
-        <v>1708</v>
+        <v>1714</v>
       </c>
       <c r="AN123" s="32"/>
       <c r="AO123" s="32" t="s">
@@ -63085,14 +63181,14 @@
         <v>69</v>
       </c>
       <c r="AT123" s="32" t="s">
-        <v>1705</v>
+        <v>1711</v>
       </c>
       <c r="AU123" s="42" t="s">
-        <v>1706</v>
+        <v>1712</v>
       </c>
       <c r="AV123" s="42"/>
       <c r="AW123" s="42" t="s">
-        <v>1709</v>
+        <v>1715</v>
       </c>
       <c r="AX123" s="42"/>
       <c r="AY123" s="42"/>
@@ -63221,13 +63317,13 @@
     </row>
     <row r="124" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A124" s="32" t="s">
-        <v>1710</v>
+        <v>1716</v>
       </c>
       <c r="B124" s="42" t="s">
-        <v>1711</v>
+        <v>1717</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>1712</v>
+        <v>1718</v>
       </c>
       <c r="D124" s="32"/>
       <c r="E124" s="32" t="s">
@@ -63243,10 +63339,10 @@
       <c r="M124" s="42"/>
       <c r="N124" s="42"/>
       <c r="O124" s="32" t="s">
-        <v>1710</v>
+        <v>1716</v>
       </c>
       <c r="P124" s="32" t="s">
-        <v>1710</v>
+        <v>1716</v>
       </c>
       <c r="Q124" s="43" t="s">
         <v>609</v>
@@ -63284,12 +63380,12 @@
       <c r="AH124" s="42"/>
       <c r="AI124" s="42"/>
       <c r="AJ124" s="32" t="s">
-        <v>1712</v>
+        <v>1718</v>
       </c>
       <c r="AK124" s="32"/>
       <c r="AL124" s="32"/>
       <c r="AM124" s="32" t="s">
-        <v>1712</v>
+        <v>1718</v>
       </c>
       <c r="AN124" s="32"/>
       <c r="AO124" s="32" t="s">
@@ -63308,14 +63404,14 @@
         <v>92</v>
       </c>
       <c r="AT124" s="32" t="s">
-        <v>1710</v>
+        <v>1716</v>
       </c>
       <c r="AU124" s="42" t="s">
-        <v>1711</v>
+        <v>1717</v>
       </c>
       <c r="AV124" s="42"/>
       <c r="AW124" s="42" t="s">
-        <v>1713</v>
+        <v>1719</v>
       </c>
       <c r="AX124" s="42"/>
       <c r="AY124" s="42"/>

</xml_diff>

<commit_message>
change public to internal
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VirJenDB\virjendb_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F428A2D2-3E89-40F5-8D1F-698D49466DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{481EBF3F-8C52-4821-9002-B464E948C944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D7962945-3ACF-49DB-B8FB-E785F5F91D27}"/>
   </bookViews>
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5433" uniqueCount="1720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5437" uniqueCount="1721">
   <si>
     <t>VJDBv0.3</t>
   </si>
@@ -4808,6 +4808,9 @@
   </si>
   <si>
     <t>0id</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>host_imgm_genome_id</t>
@@ -6334,8 +6337,8 @@
   <dimension ref="A1:FY218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B209" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A217" sqref="A217"/>
+      <pane xSplit="1" topLeftCell="AV214" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AY216" sqref="AY216:AY218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="23.25" customHeight="1"/>
@@ -52633,7 +52636,7 @@
         <v>60</v>
       </c>
       <c r="E217" s="56" t="s">
-        <v>938</v>
+        <v>61</v>
       </c>
       <c r="S217" s="63" t="s">
         <v>113</v>
@@ -52660,19 +52663,25 @@
       <c r="AW217" t="s">
         <v>1523</v>
       </c>
+      <c r="AY217" t="s">
+        <v>71</v>
+      </c>
+      <c r="AZ217" t="s">
+        <v>1524</v>
+      </c>
     </row>
     <row r="218" spans="1:53" ht="23.25" customHeight="1">
       <c r="A218" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="B218" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D218" t="s">
         <v>60</v>
       </c>
       <c r="E218" s="56" t="s">
-        <v>938</v>
+        <v>61</v>
       </c>
       <c r="S218" s="63" t="s">
         <v>113</v>
@@ -52697,7 +52706,13 @@
         <v>789</v>
       </c>
       <c r="AW218" t="s">
-        <v>1526</v>
+        <v>1527</v>
+      </c>
+      <c r="AY218" t="s">
+        <v>71</v>
+      </c>
+      <c r="AZ218" t="s">
+        <v>1524</v>
       </c>
     </row>
   </sheetData>
@@ -53899,7 +53914,7 @@
         <v>315</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
@@ -53909,14 +53924,14 @@
       <c r="AC5" s="8"/>
       <c r="AD5" s="8"/>
       <c r="AE5" s="2" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="AG5" s="8"/>
       <c r="AH5" s="9" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI5" s="8"/>
       <c r="AJ5" s="8"/>
@@ -53943,7 +53958,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -53968,7 +53983,7 @@
         <v>315</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
@@ -53980,14 +53995,14 @@
       </c>
       <c r="AD6" s="13"/>
       <c r="AE6" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG6" s="13"/>
       <c r="AH6" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI6" s="13"/>
       <c r="AJ6" s="13"/>
@@ -54037,7 +54052,7 @@
         <v>315</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
@@ -54049,14 +54064,14 @@
         <v>985</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="AF7" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG7" s="13"/>
       <c r="AH7" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI7" s="13"/>
       <c r="AJ7" s="13"/>
@@ -54106,7 +54121,7 @@
         <v>315</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X8" s="13"/>
       <c r="Y8" s="13"/>
@@ -54116,14 +54131,14 @@
       <c r="AC8" s="13"/>
       <c r="AD8" s="13"/>
       <c r="AE8" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG8" s="13"/>
       <c r="AH8" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI8" s="13"/>
       <c r="AJ8" s="13"/>
@@ -54173,7 +54188,7 @@
         <v>315</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
@@ -54183,14 +54198,14 @@
       <c r="AC9" s="13"/>
       <c r="AD9" s="13"/>
       <c r="AE9" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="AF9" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG9" s="13"/>
       <c r="AH9" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI9" s="13"/>
       <c r="AJ9" s="13"/>
@@ -54217,7 +54232,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -54242,7 +54257,7 @@
         <v>315</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
@@ -54254,14 +54269,14 @@
       </c>
       <c r="AD10" s="13"/>
       <c r="AE10" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="AF10" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG10" s="13"/>
       <c r="AH10" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI10" s="13"/>
       <c r="AJ10" s="13"/>
@@ -54288,7 +54303,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -54313,7 +54328,7 @@
         <v>315</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -54325,14 +54340,14 @@
       </c>
       <c r="AD11" s="13"/>
       <c r="AE11" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="AF11" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG11" s="13"/>
       <c r="AH11" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI11" s="13"/>
       <c r="AJ11" s="13"/>
@@ -54382,7 +54397,7 @@
         <v>315</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
@@ -54392,14 +54407,14 @@
       <c r="AC12" s="13"/>
       <c r="AD12" s="13"/>
       <c r="AE12" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="AF12" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG12" s="13"/>
       <c r="AH12" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI12" s="13"/>
       <c r="AJ12" s="13"/>
@@ -54449,7 +54464,7 @@
         <v>315</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -54459,14 +54474,14 @@
       <c r="AC13" s="13"/>
       <c r="AD13" s="13"/>
       <c r="AE13" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="AF13" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG13" s="13"/>
       <c r="AH13" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI13" s="13"/>
       <c r="AJ13" s="13"/>
@@ -54493,7 +54508,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -54518,7 +54533,7 @@
         <v>315</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
@@ -54526,20 +54541,20 @@
       <c r="AA14" s="13"/>
       <c r="AB14" s="13"/>
       <c r="AC14" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE14" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="AF14" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG14" s="13"/>
       <c r="AH14" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI14" s="13"/>
       <c r="AJ14" s="13"/>
@@ -54589,7 +54604,7 @@
         <v>315</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -54598,17 +54613,17 @@
       <c r="AB15" s="13"/>
       <c r="AC15" s="13"/>
       <c r="AD15" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="AF15" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG15" s="13"/>
       <c r="AH15" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI15" s="13"/>
       <c r="AJ15" s="13"/>
@@ -54658,7 +54673,7 @@
         <v>315</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -54668,14 +54683,14 @@
       <c r="AC16" s="13"/>
       <c r="AD16" s="13"/>
       <c r="AE16" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="AF16" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG16" s="13"/>
       <c r="AH16" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI16" s="13"/>
       <c r="AJ16" s="13"/>
@@ -54702,7 +54717,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -54727,7 +54742,7 @@
         <v>315</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -54735,20 +54750,20 @@
       <c r="AA17" s="13"/>
       <c r="AB17" s="13"/>
       <c r="AC17" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="AF17" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG17" s="13"/>
       <c r="AH17" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI17" s="13"/>
       <c r="AJ17" s="13"/>
@@ -54775,7 +54790,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
@@ -54800,7 +54815,7 @@
         <v>315</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X18" s="13"/>
       <c r="Y18" s="13"/>
@@ -54808,20 +54823,20 @@
       <c r="AA18" s="13"/>
       <c r="AB18" s="13"/>
       <c r="AC18" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="AF18" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG18" s="13"/>
       <c r="AH18" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI18" s="13"/>
       <c r="AJ18" s="13"/>
@@ -54848,7 +54863,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
@@ -54873,7 +54888,7 @@
         <v>315</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -54887,14 +54902,14 @@
         <v>1059</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="AF19" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG19" s="13"/>
       <c r="AH19" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI19" s="13"/>
       <c r="AJ19" s="13"/>
@@ -54921,7 +54936,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
@@ -54946,7 +54961,7 @@
         <v>315</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X20" s="13"/>
       <c r="Y20" s="13"/>
@@ -54958,14 +54973,14 @@
       </c>
       <c r="AD20" s="13"/>
       <c r="AE20" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="AF20" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG20" s="13"/>
       <c r="AH20" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI20" s="13"/>
       <c r="AJ20" s="13"/>
@@ -55037,7 +55052,7 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
@@ -55062,7 +55077,7 @@
         <v>315</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
@@ -55070,20 +55085,20 @@
       <c r="AA22" s="13"/>
       <c r="AB22" s="13"/>
       <c r="AC22" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="AF22" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG22" s="13"/>
       <c r="AH22" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI22" s="13"/>
       <c r="AJ22" s="13"/>
@@ -55110,7 +55125,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -55135,7 +55150,7 @@
         <v>315</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
@@ -55149,14 +55164,14 @@
         <v>985</v>
       </c>
       <c r="AE23" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="AF23" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG23" s="13"/>
       <c r="AH23" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI23" s="13"/>
       <c r="AJ23" s="13"/>
@@ -55183,7 +55198,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
@@ -55208,7 +55223,7 @@
         <v>315</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -55220,14 +55235,14 @@
       </c>
       <c r="AD24" s="13"/>
       <c r="AE24" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="AF24" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG24" s="13"/>
       <c r="AH24" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI24" s="13"/>
       <c r="AJ24" s="13"/>
@@ -55277,7 +55292,7 @@
         <v>315</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
@@ -55287,14 +55302,14 @@
       <c r="AC25" s="13"/>
       <c r="AD25" s="13"/>
       <c r="AE25" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="AF25" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG25" s="13"/>
       <c r="AH25" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI25" s="13"/>
       <c r="AJ25" s="13"/>
@@ -55321,7 +55336,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
@@ -55346,7 +55361,7 @@
         <v>315</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X26" s="13"/>
       <c r="Y26" s="13"/>
@@ -55358,14 +55373,14 @@
       </c>
       <c r="AD26" s="13"/>
       <c r="AE26" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="AF26" s="1" t="s">
         <v>351</v>
       </c>
       <c r="AG26" s="13"/>
       <c r="AH26" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI26" s="13"/>
       <c r="AJ26" s="13"/>
@@ -55392,7 +55407,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -55417,7 +55432,7 @@
         <v>315</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X27" s="13"/>
       <c r="Y27" s="13"/>
@@ -55431,14 +55446,14 @@
         <v>1059</v>
       </c>
       <c r="AE27" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="AF27" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG27" s="13"/>
       <c r="AH27" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI27" s="13"/>
       <c r="AJ27" s="13"/>
@@ -55465,7 +55480,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
@@ -55490,7 +55505,7 @@
         <v>315</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -55504,14 +55519,14 @@
         <v>1059</v>
       </c>
       <c r="AE28" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="AF28" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG28" s="13"/>
       <c r="AH28" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI28" s="13"/>
       <c r="AJ28" s="13"/>
@@ -55538,7 +55553,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
@@ -55563,7 +55578,7 @@
         <v>315</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X29" s="13"/>
       <c r="Y29" s="13"/>
@@ -55577,14 +55592,14 @@
         <v>1059</v>
       </c>
       <c r="AE29" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="AF29" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG29" s="13"/>
       <c r="AH29" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI29" s="13"/>
       <c r="AJ29" s="13"/>
@@ -55634,7 +55649,7 @@
         <v>315</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X30" s="13"/>
       <c r="Y30" s="13"/>
@@ -55643,17 +55658,17 @@
       <c r="AB30" s="13"/>
       <c r="AC30" s="13"/>
       <c r="AD30" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE30" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="AF30" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG30" s="13"/>
       <c r="AH30" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI30" s="13"/>
       <c r="AJ30" s="13"/>
@@ -55703,7 +55718,7 @@
         <v>315</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
@@ -55712,17 +55727,17 @@
       <c r="AB31" s="13"/>
       <c r="AC31" s="13"/>
       <c r="AD31" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE31" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="AF31" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG31" s="13"/>
       <c r="AH31" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI31" s="13"/>
       <c r="AJ31" s="13"/>
@@ -55749,7 +55764,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
@@ -55774,7 +55789,7 @@
         <v>315</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>
@@ -55786,14 +55801,14 @@
       </c>
       <c r="AD32" s="13"/>
       <c r="AE32" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="AF32" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG32" s="13"/>
       <c r="AH32" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI32" s="13"/>
       <c r="AJ32" s="13"/>
@@ -55843,7 +55858,7 @@
         <v>315</v>
       </c>
       <c r="W33" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
@@ -55853,14 +55868,14 @@
       <c r="AC33" s="13"/>
       <c r="AD33" s="13"/>
       <c r="AE33" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="AF33" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG33" s="13"/>
       <c r="AH33" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI33" s="13"/>
       <c r="AJ33" s="13"/>
@@ -55887,7 +55902,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
@@ -55912,7 +55927,7 @@
         <v>315</v>
       </c>
       <c r="W34" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X34" s="13"/>
       <c r="Y34" s="13"/>
@@ -55924,14 +55939,14 @@
       </c>
       <c r="AD34" s="13"/>
       <c r="AE34" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="AF34" s="1" t="s">
         <v>351</v>
       </c>
       <c r="AG34" s="13"/>
       <c r="AH34" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI34" s="13"/>
       <c r="AJ34" s="13"/>
@@ -55981,7 +55996,7 @@
         <v>315</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X35" s="13"/>
       <c r="Y35" s="13"/>
@@ -55993,14 +56008,14 @@
         <v>985</v>
       </c>
       <c r="AE35" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="AF35" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG35" s="13"/>
       <c r="AH35" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI35" s="13"/>
       <c r="AJ35" s="13"/>
@@ -56050,7 +56065,7 @@
         <v>315</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X36" s="13"/>
       <c r="Y36" s="13"/>
@@ -56067,7 +56082,7 @@
       </c>
       <c r="AG36" s="13"/>
       <c r="AH36" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI36" s="13"/>
       <c r="AJ36" s="13"/>
@@ -56094,7 +56109,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
@@ -56119,7 +56134,7 @@
         <v>315</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X37" s="13"/>
       <c r="Y37" s="13"/>
@@ -56127,20 +56142,20 @@
       <c r="AA37" s="13"/>
       <c r="AB37" s="13"/>
       <c r="AC37" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="AD37" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="AE37" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="AF37" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG37" s="13"/>
       <c r="AH37" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI37" s="13"/>
       <c r="AJ37" s="13"/>
@@ -56167,7 +56182,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
@@ -56192,7 +56207,7 @@
         <v>315</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X38" s="13"/>
       <c r="Y38" s="13"/>
@@ -56200,20 +56215,20 @@
       <c r="AA38" s="13"/>
       <c r="AB38" s="13"/>
       <c r="AC38" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="AD38" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="AE38" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="AF38" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG38" s="13"/>
       <c r="AH38" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI38" s="13"/>
       <c r="AJ38" s="13"/>
@@ -56240,7 +56255,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
@@ -56265,7 +56280,7 @@
         <v>315</v>
       </c>
       <c r="W39" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X39" s="13"/>
       <c r="Y39" s="13"/>
@@ -56273,20 +56288,20 @@
       <c r="AA39" s="13"/>
       <c r="AB39" s="13"/>
       <c r="AC39" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="AD39" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="AE39" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="AF39" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG39" s="13"/>
       <c r="AH39" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI39" s="13"/>
       <c r="AJ39" s="13"/>
@@ -56313,7 +56328,7 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
@@ -56338,7 +56353,7 @@
         <v>315</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X40" s="13"/>
       <c r="Y40" s="13"/>
@@ -56346,18 +56361,18 @@
       <c r="AA40" s="13"/>
       <c r="AB40" s="13"/>
       <c r="AC40" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="AD40" s="13"/>
       <c r="AE40" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="AF40" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG40" s="13"/>
       <c r="AH40" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI40" s="13"/>
       <c r="AJ40" s="13"/>
@@ -56384,7 +56399,7 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
@@ -56409,7 +56424,7 @@
         <v>315</v>
       </c>
       <c r="W41" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X41" s="13"/>
       <c r="Y41" s="13"/>
@@ -56423,14 +56438,14 @@
         <v>985</v>
       </c>
       <c r="AE41" s="1" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="AF41" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG41" s="13"/>
       <c r="AH41" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI41" s="13"/>
       <c r="AJ41" s="13"/>
@@ -56480,7 +56495,7 @@
         <v>315</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X42" s="13"/>
       <c r="Y42" s="13"/>
@@ -56490,14 +56505,14 @@
       <c r="AC42" s="13"/>
       <c r="AD42" s="13"/>
       <c r="AE42" s="1" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="AF42" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG42" s="13"/>
       <c r="AH42" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI42" s="13"/>
       <c r="AJ42" s="13"/>
@@ -56524,7 +56539,7 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
@@ -56549,7 +56564,7 @@
         <v>315</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X43" s="13"/>
       <c r="Y43" s="13"/>
@@ -56561,14 +56576,14 @@
       </c>
       <c r="AD43" s="13"/>
       <c r="AE43" s="1" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="AF43" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG43" s="13"/>
       <c r="AH43" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI43" s="13"/>
       <c r="AJ43" s="13"/>
@@ -56595,7 +56610,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
@@ -56620,7 +56635,7 @@
         <v>315</v>
       </c>
       <c r="W44" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X44" s="13"/>
       <c r="Y44" s="13"/>
@@ -56632,14 +56647,14 @@
       </c>
       <c r="AD44" s="13"/>
       <c r="AE44" s="1" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="AF44" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG44" s="13"/>
       <c r="AH44" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI44" s="13"/>
       <c r="AJ44" s="13"/>
@@ -56666,7 +56681,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
@@ -56691,7 +56706,7 @@
         <v>315</v>
       </c>
       <c r="W45" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X45" s="13"/>
       <c r="Y45" s="13"/>
@@ -56703,14 +56718,14 @@
       </c>
       <c r="AD45" s="13"/>
       <c r="AE45" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="AF45" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG45" s="13"/>
       <c r="AH45" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI45" s="13"/>
       <c r="AJ45" s="13"/>
@@ -56760,7 +56775,7 @@
         <v>315</v>
       </c>
       <c r="W46" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X46" s="13"/>
       <c r="Y46" s="13"/>
@@ -56770,14 +56785,14 @@
       <c r="AC46" s="13"/>
       <c r="AD46" s="13"/>
       <c r="AE46" s="1" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="AF46" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG46" s="13"/>
       <c r="AH46" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI46" s="13"/>
       <c r="AJ46" s="13"/>
@@ -56804,7 +56819,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
@@ -56829,7 +56844,7 @@
         <v>315</v>
       </c>
       <c r="W47" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X47" s="13"/>
       <c r="Y47" s="13"/>
@@ -56841,14 +56856,14 @@
       </c>
       <c r="AD47" s="13"/>
       <c r="AE47" s="1" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="AF47" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG47" s="13"/>
       <c r="AH47" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI47" s="13"/>
       <c r="AJ47" s="13"/>
@@ -56898,7 +56913,7 @@
         <v>315</v>
       </c>
       <c r="W48" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X48" s="13"/>
       <c r="Y48" s="13"/>
@@ -56908,14 +56923,14 @@
       <c r="AC48" s="13"/>
       <c r="AD48" s="13"/>
       <c r="AE48" s="1" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="AF48" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG48" s="13"/>
       <c r="AH48" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI48" s="13"/>
       <c r="AJ48" s="13"/>
@@ -56942,7 +56957,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
@@ -56967,7 +56982,7 @@
         <v>315</v>
       </c>
       <c r="W49" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X49" s="13"/>
       <c r="Y49" s="13"/>
@@ -56979,14 +56994,14 @@
       </c>
       <c r="AD49" s="13"/>
       <c r="AE49" s="1" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="AF49" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG49" s="13"/>
       <c r="AH49" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI49" s="13"/>
       <c r="AJ49" s="13"/>
@@ -57036,7 +57051,7 @@
         <v>315</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X50" s="13"/>
       <c r="Y50" s="13"/>
@@ -57046,14 +57061,14 @@
       <c r="AC50" s="13"/>
       <c r="AD50" s="13"/>
       <c r="AE50" s="1" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="AF50" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG50" s="13"/>
       <c r="AH50" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI50" s="13"/>
       <c r="AJ50" s="13"/>
@@ -57103,7 +57118,7 @@
         <v>315</v>
       </c>
       <c r="W51" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X51" s="13"/>
       <c r="Y51" s="13"/>
@@ -57112,17 +57127,17 @@
       <c r="AB51" s="13"/>
       <c r="AC51" s="13"/>
       <c r="AD51" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE51" s="1" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="AF51" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG51" s="13"/>
       <c r="AH51" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI51" s="13"/>
       <c r="AJ51" s="13"/>
@@ -57172,7 +57187,7 @@
         <v>315</v>
       </c>
       <c r="W52" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X52" s="13"/>
       <c r="Y52" s="13"/>
@@ -57181,17 +57196,17 @@
       <c r="AB52" s="13"/>
       <c r="AC52" s="13"/>
       <c r="AD52" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE52" s="1" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="AF52" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG52" s="13"/>
       <c r="AH52" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI52" s="13"/>
       <c r="AJ52" s="13"/>
@@ -57218,7 +57233,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
@@ -57243,7 +57258,7 @@
         <v>315</v>
       </c>
       <c r="W53" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X53" s="13"/>
       <c r="Y53" s="13"/>
@@ -57257,14 +57272,14 @@
         <v>985</v>
       </c>
       <c r="AE53" s="1" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="AF53" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG53" s="13"/>
       <c r="AH53" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI53" s="13"/>
       <c r="AJ53" s="13"/>
@@ -57314,7 +57329,7 @@
         <v>315</v>
       </c>
       <c r="W54" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X54" s="13"/>
       <c r="Y54" s="13"/>
@@ -57326,14 +57341,14 @@
         <v>985</v>
       </c>
       <c r="AE54" s="1" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="AF54" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG54" s="13"/>
       <c r="AH54" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI54" s="13"/>
       <c r="AJ54" s="13"/>
@@ -57360,7 +57375,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
@@ -57385,7 +57400,7 @@
         <v>315</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X55" s="13"/>
       <c r="Y55" s="13"/>
@@ -57399,14 +57414,14 @@
         <v>985</v>
       </c>
       <c r="AE55" s="1" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="AF55" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG55" s="13"/>
       <c r="AH55" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI55" s="13"/>
       <c r="AJ55" s="13"/>
@@ -57480,7 +57495,7 @@
         <v>315</v>
       </c>
       <c r="W57" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X57" s="13"/>
       <c r="Y57" s="13"/>
@@ -57492,14 +57507,14 @@
         <v>985</v>
       </c>
       <c r="AE57" s="1" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="AF57" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG57" s="13"/>
       <c r="AH57" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI57" s="13"/>
       <c r="AJ57" s="13"/>
@@ -57549,7 +57564,7 @@
         <v>315</v>
       </c>
       <c r="W58" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X58" s="13"/>
       <c r="Y58" s="13"/>
@@ -57561,14 +57576,14 @@
         <v>985</v>
       </c>
       <c r="AE58" s="1" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="AF58" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG58" s="13"/>
       <c r="AH58" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI58" s="13"/>
       <c r="AJ58" s="13"/>
@@ -57595,7 +57610,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
@@ -57620,7 +57635,7 @@
         <v>315</v>
       </c>
       <c r="W59" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X59" s="13"/>
       <c r="Y59" s="13"/>
@@ -57628,20 +57643,20 @@
       <c r="AA59" s="13"/>
       <c r="AB59" s="13"/>
       <c r="AC59" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AD59" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE59" s="1" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="AF59" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG59" s="13"/>
       <c r="AH59" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI59" s="13"/>
       <c r="AJ59" s="13"/>
@@ -57691,7 +57706,7 @@
         <v>315</v>
       </c>
       <c r="W60" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X60" s="13"/>
       <c r="Y60" s="13"/>
@@ -57700,17 +57715,17 @@
       <c r="AB60" s="13"/>
       <c r="AC60" s="13"/>
       <c r="AD60" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE60" s="1" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="AF60" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG60" s="13"/>
       <c r="AH60" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI60" s="13"/>
       <c r="AJ60" s="13"/>
@@ -57737,7 +57752,7 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
@@ -57762,7 +57777,7 @@
         <v>315</v>
       </c>
       <c r="W61" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X61" s="13"/>
       <c r="Y61" s="13"/>
@@ -57774,14 +57789,14 @@
       </c>
       <c r="AD61" s="13"/>
       <c r="AE61" s="1" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="AF61" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG61" s="13"/>
       <c r="AH61" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI61" s="13"/>
       <c r="AJ61" s="13"/>
@@ -57831,7 +57846,7 @@
         <v>315</v>
       </c>
       <c r="W62" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X62" s="13"/>
       <c r="Y62" s="13"/>
@@ -57841,14 +57856,14 @@
       <c r="AC62" s="13"/>
       <c r="AD62" s="13"/>
       <c r="AE62" s="1" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="AF62" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG62" s="13"/>
       <c r="AH62" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI62" s="13"/>
       <c r="AJ62" s="13"/>
@@ -57875,7 +57890,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="O63" s="6"/>
       <c r="P63" s="6"/>
@@ -57900,7 +57915,7 @@
         <v>315</v>
       </c>
       <c r="W63" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X63" s="13"/>
       <c r="Y63" s="13"/>
@@ -57912,14 +57927,14 @@
       </c>
       <c r="AD63" s="13"/>
       <c r="AE63" s="1" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="AF63" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG63" s="13"/>
       <c r="AH63" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI63" s="13"/>
       <c r="AJ63" s="13"/>
@@ -57969,7 +57984,7 @@
         <v>315</v>
       </c>
       <c r="W64" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X64" s="13"/>
       <c r="Y64" s="13"/>
@@ -57979,14 +57994,14 @@
       <c r="AC64" s="13"/>
       <c r="AD64" s="13"/>
       <c r="AE64" s="1" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="AF64" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG64" s="13"/>
       <c r="AH64" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI64" s="13"/>
       <c r="AJ64" s="13"/>
@@ -58036,7 +58051,7 @@
         <v>315</v>
       </c>
       <c r="W65" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X65" s="13"/>
       <c r="Y65" s="13"/>
@@ -58045,17 +58060,17 @@
       <c r="AB65" s="13"/>
       <c r="AC65" s="13"/>
       <c r="AD65" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="AE65" s="1" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="AF65" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG65" s="13"/>
       <c r="AH65" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI65" s="13"/>
       <c r="AJ65" s="13"/>
@@ -58105,7 +58120,7 @@
         <v>315</v>
       </c>
       <c r="W66" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X66" s="13"/>
       <c r="Y66" s="13"/>
@@ -58115,14 +58130,14 @@
       <c r="AC66" s="13"/>
       <c r="AD66" s="13"/>
       <c r="AE66" s="1" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="AF66" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG66" s="13"/>
       <c r="AH66" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI66" s="13"/>
       <c r="AJ66" s="13"/>
@@ -58196,7 +58211,7 @@
         <v>315</v>
       </c>
       <c r="W68" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X68" s="13"/>
       <c r="Y68" s="13"/>
@@ -58213,7 +58228,7 @@
       </c>
       <c r="AG68" s="13"/>
       <c r="AH68" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI68" s="13"/>
       <c r="AJ68" s="13"/>
@@ -58240,7 +58255,7 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="O69" s="6"/>
       <c r="P69" s="6"/>
@@ -58265,7 +58280,7 @@
         <v>315</v>
       </c>
       <c r="W69" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X69" s="13"/>
       <c r="Y69" s="13"/>
@@ -58277,14 +58292,14 @@
       </c>
       <c r="AD69" s="13"/>
       <c r="AE69" s="1" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="AF69" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG69" s="13"/>
       <c r="AH69" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI69" s="13"/>
       <c r="AJ69" s="13"/>
@@ -58311,7 +58326,7 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="O70" s="6"/>
       <c r="P70" s="6"/>
@@ -58336,7 +58351,7 @@
         <v>315</v>
       </c>
       <c r="W70" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X70" s="13"/>
       <c r="Y70" s="13"/>
@@ -58350,14 +58365,14 @@
         <v>985</v>
       </c>
       <c r="AE70" s="1" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="AF70" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG70" s="13"/>
       <c r="AH70" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI70" s="13"/>
       <c r="AJ70" s="13"/>
@@ -58384,7 +58399,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
       <c r="N71" s="4" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="O71" s="6"/>
       <c r="P71" s="6"/>
@@ -58409,7 +58424,7 @@
         <v>315</v>
       </c>
       <c r="W71" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X71" s="13"/>
       <c r="Y71" s="13"/>
@@ -58421,14 +58436,14 @@
       </c>
       <c r="AD71" s="13"/>
       <c r="AE71" s="1" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="AF71" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG71" s="13"/>
       <c r="AH71" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI71" s="13"/>
       <c r="AJ71" s="13"/>
@@ -58455,7 +58470,7 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
       <c r="N72" s="4" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="O72" s="6"/>
       <c r="P72" s="6"/>
@@ -58480,7 +58495,7 @@
         <v>315</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X72" s="13"/>
       <c r="Y72" s="13"/>
@@ -58492,14 +58507,14 @@
       </c>
       <c r="AD72" s="13"/>
       <c r="AE72" s="1" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="AF72" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG72" s="13"/>
       <c r="AH72" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI72" s="13"/>
       <c r="AJ72" s="13"/>
@@ -58549,7 +58564,7 @@
         <v>315</v>
       </c>
       <c r="W73" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X73" s="13"/>
       <c r="Y73" s="13"/>
@@ -58558,17 +58573,17 @@
       <c r="AB73" s="13"/>
       <c r="AC73" s="13"/>
       <c r="AD73" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="AE73" s="1" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="AF73" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG73" s="13"/>
       <c r="AH73" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI73" s="13"/>
       <c r="AJ73" s="13"/>
@@ -58595,7 +58610,7 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="O74" s="6"/>
       <c r="P74" s="6"/>
@@ -58620,7 +58635,7 @@
         <v>315</v>
       </c>
       <c r="W74" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X74" s="13"/>
       <c r="Y74" s="13"/>
@@ -58631,17 +58646,17 @@
         <v>349</v>
       </c>
       <c r="AD74" s="1" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="AE74" s="1" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="AF74" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG74" s="13"/>
       <c r="AH74" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI74" s="13"/>
       <c r="AJ74" s="13"/>
@@ -58691,7 +58706,7 @@
         <v>315</v>
       </c>
       <c r="W75" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X75" s="13"/>
       <c r="Y75" s="13"/>
@@ -58701,14 +58716,14 @@
       <c r="AC75" s="13"/>
       <c r="AD75" s="13"/>
       <c r="AE75" s="1" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="AF75" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG75" s="13"/>
       <c r="AH75" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI75" s="13"/>
       <c r="AJ75" s="13"/>
@@ -58758,7 +58773,7 @@
         <v>315</v>
       </c>
       <c r="W76" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X76" s="13"/>
       <c r="Y76" s="13"/>
@@ -58768,14 +58783,14 @@
       <c r="AC76" s="13"/>
       <c r="AD76" s="13"/>
       <c r="AE76" s="1" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="AF76" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG76" s="13"/>
       <c r="AH76" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI76" s="13"/>
       <c r="AJ76" s="13"/>
@@ -58825,7 +58840,7 @@
         <v>315</v>
       </c>
       <c r="W77" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X77" s="13"/>
       <c r="Y77" s="13"/>
@@ -58834,17 +58849,17 @@
       <c r="AB77" s="13"/>
       <c r="AC77" s="13"/>
       <c r="AD77" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE77" s="1" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="AF77" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG77" s="13"/>
       <c r="AH77" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI77" s="13"/>
       <c r="AJ77" s="13"/>
@@ -58894,7 +58909,7 @@
         <v>315</v>
       </c>
       <c r="W78" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X78" s="13"/>
       <c r="Y78" s="13"/>
@@ -58903,17 +58918,17 @@
       <c r="AB78" s="13"/>
       <c r="AC78" s="13"/>
       <c r="AD78" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE78" s="1" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="AF78" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG78" s="13"/>
       <c r="AH78" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI78" s="13"/>
       <c r="AJ78" s="13"/>
@@ -58940,7 +58955,7 @@
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
       <c r="N79" s="4" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="O79" s="6"/>
       <c r="P79" s="6"/>
@@ -58965,7 +58980,7 @@
         <v>315</v>
       </c>
       <c r="W79" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X79" s="13"/>
       <c r="Y79" s="13"/>
@@ -58977,14 +58992,14 @@
       </c>
       <c r="AD79" s="13"/>
       <c r="AE79" s="1" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="AF79" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG79" s="13"/>
       <c r="AH79" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI79" s="13"/>
       <c r="AJ79" s="13"/>
@@ -59011,7 +59026,7 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
       <c r="N80" s="4" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="O80" s="6"/>
       <c r="P80" s="6"/>
@@ -59036,7 +59051,7 @@
         <v>315</v>
       </c>
       <c r="W80" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X80" s="13"/>
       <c r="Y80" s="13"/>
@@ -59048,14 +59063,14 @@
       </c>
       <c r="AD80" s="13"/>
       <c r="AE80" s="1" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="AF80" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG80" s="13"/>
       <c r="AH80" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI80" s="13"/>
       <c r="AJ80" s="13"/>
@@ -59105,7 +59120,7 @@
         <v>315</v>
       </c>
       <c r="W81" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X81" s="13"/>
       <c r="Y81" s="13"/>
@@ -59114,17 +59129,17 @@
       <c r="AB81" s="13"/>
       <c r="AC81" s="13"/>
       <c r="AD81" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE81" s="1" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="AF81" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG81" s="13"/>
       <c r="AH81" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI81" s="13"/>
       <c r="AJ81" s="13"/>
@@ -59151,7 +59166,7 @@
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
       <c r="N82" s="4" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="O82" s="6"/>
       <c r="P82" s="6"/>
@@ -59176,7 +59191,7 @@
         <v>315</v>
       </c>
       <c r="W82" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X82" s="13"/>
       <c r="Y82" s="13"/>
@@ -59188,14 +59203,14 @@
       </c>
       <c r="AD82" s="13"/>
       <c r="AE82" s="1" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="AF82" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG82" s="13"/>
       <c r="AH82" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI82" s="13"/>
       <c r="AJ82" s="13"/>
@@ -59245,7 +59260,7 @@
         <v>315</v>
       </c>
       <c r="W83" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X83" s="13"/>
       <c r="Y83" s="13"/>
@@ -59255,14 +59270,14 @@
       <c r="AC83" s="13"/>
       <c r="AD83" s="13"/>
       <c r="AE83" s="1" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="AF83" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG83" s="13"/>
       <c r="AH83" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI83" s="13"/>
       <c r="AJ83" s="13"/>
@@ -59334,7 +59349,7 @@
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
       <c r="N85" s="4" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="O85" s="6"/>
       <c r="P85" s="6"/>
@@ -59359,7 +59374,7 @@
         <v>315</v>
       </c>
       <c r="W85" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X85" s="13"/>
       <c r="Y85" s="13"/>
@@ -59373,14 +59388,14 @@
         <v>1059</v>
       </c>
       <c r="AE85" s="1" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="AF85" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG85" s="13"/>
       <c r="AH85" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI85" s="13"/>
       <c r="AJ85" s="13"/>
@@ -59430,7 +59445,7 @@
         <v>315</v>
       </c>
       <c r="W86" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X86" s="13"/>
       <c r="Y86" s="13"/>
@@ -59439,17 +59454,17 @@
       <c r="AB86" s="13"/>
       <c r="AC86" s="13"/>
       <c r="AD86" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE86" s="1" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="AF86" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG86" s="13"/>
       <c r="AH86" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI86" s="13"/>
       <c r="AJ86" s="13"/>
@@ -59499,7 +59514,7 @@
         <v>315</v>
       </c>
       <c r="W87" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X87" s="13"/>
       <c r="Y87" s="13"/>
@@ -59508,17 +59523,17 @@
       <c r="AB87" s="13"/>
       <c r="AC87" s="13"/>
       <c r="AD87" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE87" s="1" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="AF87" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AG87" s="13"/>
       <c r="AH87" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI87" s="13"/>
       <c r="AJ87" s="13"/>
@@ -59545,7 +59560,7 @@
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
       <c r="N88" s="4" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="O88" s="6"/>
       <c r="P88" s="6"/>
@@ -59570,7 +59585,7 @@
         <v>315</v>
       </c>
       <c r="W88" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X88" s="13"/>
       <c r="Y88" s="13"/>
@@ -59581,7 +59596,7 @@
         <v>349</v>
       </c>
       <c r="AD88" s="1" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="AE88" s="1" t="s">
         <v>938</v>
@@ -59591,7 +59606,7 @@
       </c>
       <c r="AG88" s="13"/>
       <c r="AH88" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI88" s="13"/>
       <c r="AJ88" s="13"/>
@@ -59641,7 +59656,7 @@
         <v>315</v>
       </c>
       <c r="W89" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X89" s="13"/>
       <c r="Y89" s="13"/>
@@ -59658,7 +59673,7 @@
       </c>
       <c r="AG89" s="13"/>
       <c r="AH89" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI89" s="13"/>
       <c r="AJ89" s="13"/>
@@ -59708,7 +59723,7 @@
         <v>315</v>
       </c>
       <c r="W90" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X90" s="13"/>
       <c r="Y90" s="13"/>
@@ -59718,14 +59733,14 @@
       <c r="AC90" s="13"/>
       <c r="AD90" s="13"/>
       <c r="AE90" s="1" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="AF90" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG90" s="13"/>
       <c r="AH90" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI90" s="13"/>
       <c r="AJ90" s="13"/>
@@ -59775,7 +59790,7 @@
         <v>315</v>
       </c>
       <c r="W91" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X91" s="13"/>
       <c r="Y91" s="13"/>
@@ -59784,17 +59799,17 @@
       <c r="AB91" s="13"/>
       <c r="AC91" s="13"/>
       <c r="AD91" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE91" s="1" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="AF91" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG91" s="13"/>
       <c r="AH91" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI91" s="13"/>
       <c r="AJ91" s="13"/>
@@ -59844,7 +59859,7 @@
         <v>315</v>
       </c>
       <c r="W92" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X92" s="13"/>
       <c r="Y92" s="13"/>
@@ -59854,14 +59869,14 @@
       <c r="AC92" s="13"/>
       <c r="AD92" s="13"/>
       <c r="AE92" s="1" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="AF92" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG92" s="13"/>
       <c r="AH92" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI92" s="13"/>
       <c r="AJ92" s="13"/>
@@ -59888,7 +59903,7 @@
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6"/>
@@ -59913,7 +59928,7 @@
         <v>315</v>
       </c>
       <c r="W93" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X93" s="13"/>
       <c r="Y93" s="13"/>
@@ -59921,20 +59936,20 @@
       <c r="AA93" s="13"/>
       <c r="AB93" s="13"/>
       <c r="AC93" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AD93" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE93" s="1" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="AF93" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG93" s="13"/>
       <c r="AH93" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI93" s="13"/>
       <c r="AJ93" s="13"/>
@@ -59984,7 +59999,7 @@
         <v>315</v>
       </c>
       <c r="W94" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X94" s="13"/>
       <c r="Y94" s="13"/>
@@ -59994,14 +60009,14 @@
       <c r="AC94" s="13"/>
       <c r="AD94" s="13"/>
       <c r="AE94" s="1" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="AF94" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG94" s="13"/>
       <c r="AH94" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI94" s="13"/>
       <c r="AJ94" s="13"/>
@@ -60028,7 +60043,7 @@
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
       <c r="N95" s="4" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="O95" s="6"/>
       <c r="P95" s="6"/>
@@ -60053,7 +60068,7 @@
         <v>315</v>
       </c>
       <c r="W95" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X95" s="13"/>
       <c r="Y95" s="13"/>
@@ -60067,14 +60082,14 @@
         <v>985</v>
       </c>
       <c r="AE95" s="1" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="AF95" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG95" s="13"/>
       <c r="AH95" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI95" s="13"/>
       <c r="AJ95" s="13"/>
@@ -60126,7 +60141,7 @@
         <v>315</v>
       </c>
       <c r="W96" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X96" s="13"/>
       <c r="Y96" s="13"/>
@@ -60138,14 +60153,14 @@
       </c>
       <c r="AD96" s="13"/>
       <c r="AE96" s="1" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="AF96" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG96" s="13"/>
       <c r="AH96" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI96" s="13"/>
       <c r="AJ96" s="13"/>
@@ -60195,7 +60210,7 @@
         <v>315</v>
       </c>
       <c r="W97" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X97" s="13"/>
       <c r="Y97" s="13"/>
@@ -60207,14 +60222,14 @@
         <v>1059</v>
       </c>
       <c r="AE97" s="1" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="AF97" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG97" s="13"/>
       <c r="AH97" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI97" s="13"/>
       <c r="AJ97" s="13"/>
@@ -60241,7 +60256,7 @@
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
       <c r="N98" s="4" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="O98" s="6"/>
       <c r="P98" s="6"/>
@@ -60266,7 +60281,7 @@
         <v>315</v>
       </c>
       <c r="W98" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X98" s="13"/>
       <c r="Y98" s="13"/>
@@ -60278,14 +60293,14 @@
       </c>
       <c r="AD98" s="13"/>
       <c r="AE98" s="1" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="AF98" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG98" s="13"/>
       <c r="AH98" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI98" s="13"/>
       <c r="AJ98" s="13"/>
@@ -60312,7 +60327,7 @@
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
       <c r="N99" s="4" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="O99" s="6"/>
       <c r="P99" s="6"/>
@@ -60337,7 +60352,7 @@
         <v>315</v>
       </c>
       <c r="W99" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X99" s="13"/>
       <c r="Y99" s="13"/>
@@ -60349,14 +60364,14 @@
       </c>
       <c r="AD99" s="13"/>
       <c r="AE99" s="1" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="AF99" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG99" s="13"/>
       <c r="AH99" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI99" s="13"/>
       <c r="AJ99" s="13"/>
@@ -60406,7 +60421,7 @@
         <v>315</v>
       </c>
       <c r="W100" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X100" s="13"/>
       <c r="Y100" s="13"/>
@@ -60416,14 +60431,14 @@
       <c r="AC100" s="13"/>
       <c r="AD100" s="13"/>
       <c r="AE100" s="1" t="s">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="AF100" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG100" s="13"/>
       <c r="AH100" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI100" s="13"/>
       <c r="AJ100" s="13"/>
@@ -60450,7 +60465,7 @@
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
       <c r="N101" s="4" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="O101" s="6"/>
       <c r="P101" s="6"/>
@@ -60475,7 +60490,7 @@
         <v>315</v>
       </c>
       <c r="W101" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X101" s="13"/>
       <c r="Y101" s="13"/>
@@ -60489,14 +60504,14 @@
         <v>985</v>
       </c>
       <c r="AE101" s="1" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="AF101" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG101" s="13"/>
       <c r="AH101" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI101" s="13"/>
       <c r="AJ101" s="13"/>
@@ -60548,7 +60563,7 @@
         <v>315</v>
       </c>
       <c r="W102" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X102" s="13"/>
       <c r="Y102" s="13"/>
@@ -60567,7 +60582,7 @@
       </c>
       <c r="AG102" s="13"/>
       <c r="AH102" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI102" s="13"/>
       <c r="AJ102" s="13"/>
@@ -60594,7 +60609,7 @@
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="O103" s="6"/>
       <c r="P103" s="6"/>
@@ -60619,7 +60634,7 @@
         <v>315</v>
       </c>
       <c r="W103" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X103" s="13"/>
       <c r="Y103" s="13"/>
@@ -60631,14 +60646,14 @@
       </c>
       <c r="AD103" s="13"/>
       <c r="AE103" s="1" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="AF103" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG103" s="13"/>
       <c r="AH103" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI103" s="13"/>
       <c r="AJ103" s="13"/>
@@ -60665,7 +60680,7 @@
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="O104" s="6"/>
       <c r="P104" s="6"/>
@@ -60690,7 +60705,7 @@
         <v>315</v>
       </c>
       <c r="W104" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X104" s="13"/>
       <c r="Y104" s="13"/>
@@ -60702,14 +60717,14 @@
       </c>
       <c r="AD104" s="13"/>
       <c r="AE104" s="1" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="AF104" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG104" s="13"/>
       <c r="AH104" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI104" s="13"/>
       <c r="AJ104" s="13"/>
@@ -60736,7 +60751,7 @@
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="O105" s="6"/>
       <c r="P105" s="6"/>
@@ -60761,7 +60776,7 @@
         <v>315</v>
       </c>
       <c r="W105" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X105" s="13"/>
       <c r="Y105" s="13"/>
@@ -60775,14 +60790,14 @@
         <v>704</v>
       </c>
       <c r="AE105" s="1" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="AF105" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG105" s="13"/>
       <c r="AH105" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI105" s="13"/>
       <c r="AJ105" s="13"/>
@@ -60810,7 +60825,7 @@
       <c r="M106" s="4"/>
       <c r="AG106" s="13"/>
       <c r="AH106" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI106" s="13"/>
       <c r="AJ106" s="13"/>
@@ -60860,7 +60875,7 @@
         <v>315</v>
       </c>
       <c r="W107" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X107" s="13"/>
       <c r="Y107" s="13"/>
@@ -60870,14 +60885,14 @@
       <c r="AC107" s="13"/>
       <c r="AD107" s="13"/>
       <c r="AE107" s="1" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="AF107" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG107" s="13"/>
       <c r="AH107" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI107" s="13"/>
       <c r="AJ107" s="13"/>
@@ -60927,7 +60942,7 @@
         <v>315</v>
       </c>
       <c r="W108" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X108" s="13"/>
       <c r="Y108" s="13"/>
@@ -60940,11 +60955,11 @@
         <v>68</v>
       </c>
       <c r="AF108" s="1" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="AG108" s="13"/>
       <c r="AH108" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI108" s="13"/>
       <c r="AJ108" s="13"/>
@@ -60971,7 +60986,7 @@
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="O109" s="6"/>
       <c r="P109" s="6"/>
@@ -60996,7 +61011,7 @@
         <v>315</v>
       </c>
       <c r="W109" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X109" s="13"/>
       <c r="Y109" s="13"/>
@@ -61004,20 +61019,20 @@
       <c r="AA109" s="13"/>
       <c r="AB109" s="13"/>
       <c r="AC109" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AD109" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="AE109" s="1" t="s">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="AF109" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="AG109" s="13"/>
       <c r="AH109" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI109" s="13"/>
       <c r="AJ109" s="13"/>
@@ -61044,7 +61059,7 @@
       <c r="L110" s="4"/>
       <c r="M110" s="4"/>
       <c r="N110" s="4" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="O110" s="6"/>
       <c r="P110" s="6"/>
@@ -61069,7 +61084,7 @@
         <v>315</v>
       </c>
       <c r="W110" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X110" s="13"/>
       <c r="Y110" s="13"/>
@@ -61081,14 +61096,14 @@
       </c>
       <c r="AD110" s="13"/>
       <c r="AE110" s="1" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="AF110" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG110" s="13"/>
       <c r="AH110" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI110" s="13"/>
       <c r="AJ110" s="13"/>
@@ -61138,7 +61153,7 @@
         <v>315</v>
       </c>
       <c r="W111" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X111" s="13"/>
       <c r="Y111" s="13"/>
@@ -61148,14 +61163,14 @@
       <c r="AC111" s="13"/>
       <c r="AD111" s="13"/>
       <c r="AE111" s="1" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="AF111" s="1" t="s">
         <v>319</v>
       </c>
       <c r="AG111" s="13"/>
       <c r="AH111" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI111" s="13"/>
       <c r="AJ111" s="13"/>
@@ -61205,7 +61220,7 @@
         <v>315</v>
       </c>
       <c r="W112" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X112" s="13"/>
       <c r="Y112" s="13"/>
@@ -61214,17 +61229,17 @@
       <c r="AB112" s="13"/>
       <c r="AC112" s="13"/>
       <c r="AD112" s="1" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="AE112" s="1" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="AF112" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG112" s="13"/>
       <c r="AH112" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI112" s="13"/>
       <c r="AJ112" s="13"/>
@@ -61274,7 +61289,7 @@
         <v>315</v>
       </c>
       <c r="W113" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X113" s="13"/>
       <c r="Y113" s="13"/>
@@ -61283,17 +61298,17 @@
       <c r="AB113" s="13"/>
       <c r="AC113" s="13"/>
       <c r="AD113" s="1" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="AE113" s="1" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="AF113" s="1" t="s">
         <v>340</v>
       </c>
       <c r="AG113" s="13"/>
       <c r="AH113" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI113" s="13"/>
       <c r="AJ113" s="13"/>
@@ -61320,7 +61335,7 @@
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
       <c r="N114" s="4" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="O114" s="6"/>
       <c r="P114" s="6"/>
@@ -61345,7 +61360,7 @@
         <v>315</v>
       </c>
       <c r="W114" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="X114" s="13"/>
       <c r="Y114" s="13"/>
@@ -61360,7 +61375,7 @@
       <c r="AF114" s="13"/>
       <c r="AG114" s="13"/>
       <c r="AH114" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AI114" s="13"/>
       <c r="AJ114" s="13"/>
@@ -61415,14 +61430,14 @@
       <c r="X115" s="34"/>
       <c r="Y115" s="34"/>
       <c r="Z115" s="36" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="AA115" s="36" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="AB115" s="34"/>
       <c r="AC115" s="34" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AD115" s="34"/>
       <c r="AE115" s="34"/>
@@ -61585,7 +61600,7 @@
       <c r="K116" s="34"/>
       <c r="L116" s="34"/>
       <c r="M116" s="36" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="N116" s="34"/>
       <c r="O116" s="34"/>
@@ -61618,14 +61633,14 @@
       <c r="X116" s="34"/>
       <c r="Y116" s="34"/>
       <c r="Z116" s="36" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="AA116" s="36" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="AB116" s="34"/>
       <c r="AC116" s="34" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="AD116" s="34"/>
       <c r="AE116" s="34"/>
@@ -61647,7 +61662,7 @@
       <c r="AU116" s="34"/>
       <c r="AV116" s="37"/>
       <c r="AW116" s="37" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="AX116" s="37"/>
       <c r="AY116" s="37"/>
@@ -61821,14 +61836,14 @@
       <c r="X117" s="34"/>
       <c r="Y117" s="34"/>
       <c r="Z117" s="36" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="AA117" s="36" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="AB117" s="34"/>
       <c r="AC117" s="34" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AD117" s="34"/>
       <c r="AE117" s="34"/>
@@ -61850,7 +61865,7 @@
       <c r="AU117" s="34"/>
       <c r="AV117" s="37"/>
       <c r="AW117" s="37" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="AX117" s="37"/>
       <c r="AY117" s="37"/>
@@ -61979,13 +61994,13 @@
     </row>
     <row r="118" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A118" s="38" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="B118" s="39" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="C118" s="38" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="D118" s="38"/>
       <c r="E118" s="38" t="s">
@@ -62001,10 +62016,10 @@
       <c r="M118" s="39"/>
       <c r="N118" s="39"/>
       <c r="O118" s="38" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="P118" s="38" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="Q118" s="40" t="s">
         <v>609</v>
@@ -62042,12 +62057,12 @@
       <c r="AH118" s="39"/>
       <c r="AI118" s="39"/>
       <c r="AJ118" s="38" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="AK118" s="38"/>
       <c r="AL118" s="38"/>
       <c r="AM118" s="38" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="AN118" s="38"/>
       <c r="AO118" s="38" t="s">
@@ -62066,14 +62081,14 @@
         <v>69</v>
       </c>
       <c r="AT118" s="38" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="AU118" s="39" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="AV118" s="39"/>
       <c r="AW118" s="39" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="AX118" s="39"/>
       <c r="AY118" s="39"/>
@@ -62202,13 +62217,13 @@
     </row>
     <row r="119" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A119" s="38" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="B119" s="39" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="C119" s="38" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="D119" s="38"/>
       <c r="E119" s="38" t="s">
@@ -62224,10 +62239,10 @@
       <c r="M119" s="39"/>
       <c r="N119" s="39"/>
       <c r="O119" s="38" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="P119" s="38" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="Q119" s="40" t="s">
         <v>359</v>
@@ -62265,12 +62280,12 @@
       <c r="AH119" s="39"/>
       <c r="AI119" s="39"/>
       <c r="AJ119" s="38" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="AK119" s="38"/>
       <c r="AL119" s="38"/>
       <c r="AM119" s="38" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="AN119" s="38"/>
       <c r="AO119" s="38" t="s">
@@ -62289,14 +62304,14 @@
         <v>69</v>
       </c>
       <c r="AT119" s="38" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="AU119" s="39" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="AV119" s="39"/>
       <c r="AW119" s="39" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="AX119" s="39"/>
       <c r="AY119" s="39"/>
@@ -62425,13 +62440,13 @@
     </row>
     <row r="120" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A120" s="38" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="B120" s="39" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="C120" s="38" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="D120" s="38"/>
       <c r="E120" s="38" t="s">
@@ -62447,10 +62462,10 @@
       <c r="M120" s="39"/>
       <c r="N120" s="39"/>
       <c r="O120" s="38" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="P120" s="38" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="Q120" s="40" t="s">
         <v>909</v>
@@ -62488,12 +62503,12 @@
       <c r="AH120" s="39"/>
       <c r="AI120" s="39"/>
       <c r="AJ120" s="38" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="AK120" s="38"/>
       <c r="AL120" s="38"/>
       <c r="AM120" s="38" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="AN120" s="38"/>
       <c r="AO120" s="38" t="s">
@@ -62512,14 +62527,14 @@
         <v>69</v>
       </c>
       <c r="AT120" s="38" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="AU120" s="39" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="AV120" s="39"/>
       <c r="AW120" s="39" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="AX120" s="39"/>
       <c r="AY120" s="39"/>
@@ -62648,13 +62663,13 @@
     </row>
     <row r="121" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A121" s="38" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="B121" s="39" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="C121" s="38" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="D121" s="38"/>
       <c r="E121" s="38" t="s">
@@ -62670,10 +62685,10 @@
       <c r="M121" s="39"/>
       <c r="N121" s="39"/>
       <c r="O121" s="38" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="P121" s="38" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="Q121" s="40" t="s">
         <v>99</v>
@@ -62711,12 +62726,12 @@
       <c r="AH121" s="39"/>
       <c r="AI121" s="39"/>
       <c r="AJ121" s="38" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="AK121" s="38"/>
       <c r="AL121" s="38"/>
       <c r="AM121" s="38" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="AN121" s="38"/>
       <c r="AO121" s="38" t="s">
@@ -62735,14 +62750,14 @@
         <v>69</v>
       </c>
       <c r="AT121" s="38" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="AU121" s="39" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="AV121" s="39"/>
       <c r="AW121" s="39" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="AX121" s="39"/>
       <c r="AY121" s="39"/>
@@ -62871,13 +62886,13 @@
     </row>
     <row r="122" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A122" s="38" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="B122" s="39" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="C122" s="38" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="D122" s="38"/>
       <c r="E122" s="38" t="s">
@@ -62893,10 +62908,10 @@
       <c r="M122" s="39"/>
       <c r="N122" s="39"/>
       <c r="O122" s="38" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="P122" s="38" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="Q122" s="40" t="s">
         <v>909</v>
@@ -62934,12 +62949,12 @@
       <c r="AH122" s="39"/>
       <c r="AI122" s="39"/>
       <c r="AJ122" s="38" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="AK122" s="38"/>
       <c r="AL122" s="38"/>
       <c r="AM122" s="38" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="AN122" s="38"/>
       <c r="AO122" s="38" t="s">
@@ -62958,14 +62973,14 @@
         <v>69</v>
       </c>
       <c r="AT122" s="38" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="AU122" s="39" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="AV122" s="39"/>
       <c r="AW122" s="39" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="AX122" s="39"/>
       <c r="AY122" s="39"/>
@@ -63094,13 +63109,13 @@
     </row>
     <row r="123" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A123" s="32" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="B123" s="42" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="D123" s="32"/>
       <c r="E123" s="32" t="s">
@@ -63116,10 +63131,10 @@
       <c r="M123" s="42"/>
       <c r="N123" s="42"/>
       <c r="O123" s="32" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="P123" s="32" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="Q123" s="43" t="s">
         <v>609</v>
@@ -63157,12 +63172,12 @@
       <c r="AH123" s="42"/>
       <c r="AI123" s="42"/>
       <c r="AJ123" s="32" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="AK123" s="32"/>
       <c r="AL123" s="32"/>
       <c r="AM123" s="32" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="AN123" s="32"/>
       <c r="AO123" s="32" t="s">
@@ -63181,14 +63196,14 @@
         <v>69</v>
       </c>
       <c r="AT123" s="32" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="AU123" s="42" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="AV123" s="42"/>
       <c r="AW123" s="42" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="AX123" s="42"/>
       <c r="AY123" s="42"/>
@@ -63317,13 +63332,13 @@
     </row>
     <row r="124" spans="1:173" s="10" customFormat="1" ht="23.25" customHeight="1">
       <c r="A124" s="32" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="B124" s="42" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="D124" s="32"/>
       <c r="E124" s="32" t="s">
@@ -63339,10 +63354,10 @@
       <c r="M124" s="42"/>
       <c r="N124" s="42"/>
       <c r="O124" s="32" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="P124" s="32" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="Q124" s="43" t="s">
         <v>609</v>
@@ -63380,12 +63395,12 @@
       <c r="AH124" s="42"/>
       <c r="AI124" s="42"/>
       <c r="AJ124" s="32" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="AK124" s="32"/>
       <c r="AL124" s="32"/>
       <c r="AM124" s="32" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="AN124" s="32"/>
       <c r="AO124" s="32" t="s">
@@ -63404,14 +63419,14 @@
         <v>92</v>
       </c>
       <c r="AT124" s="32" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="AU124" s="42" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="AV124" s="42"/>
       <c r="AW124" s="42" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="AX124" s="42"/>
       <c r="AY124" s="42"/>

</xml_diff>